<commit_message>
wip added sqlite db
</commit_message>
<xml_diff>
--- a/data/EventData.xlsx
+++ b/data/EventData.xlsx
@@ -16,18 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="93">
   <si>
     <t>Movies</t>
-  </si>
-  <si>
-    <t>Channel</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Time</t>
   </si>
   <si>
     <t>M-Net Action</t>
@@ -106,9 +97,6 @@
   </si>
   <si>
     <t>Winter is coming. Let the Game of Thrones begin.</t>
-  </si>
-  <si>
-    <t>SeriesInfo</t>
   </si>
   <si>
     <t xml:space="preserve">Episode 1, S1 </t>
@@ -325,9 +313,6 @@
     <t>genre</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -353,6 +338,27 @@
   </si>
   <si>
     <t>year_produced</t>
+  </si>
+  <si>
+    <t>_id</t>
+  </si>
+  <si>
+    <t>channel</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>series_info</t>
+  </si>
+  <si>
+    <t>ev_rec_id</t>
+  </si>
+  <si>
+    <t>buy_rec_id</t>
   </si>
 </sst>
 </file>
@@ -784,98 +790,98 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -885,409 +891,483 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" customWidth="1"/>
-    <col min="5" max="5" width="32" style="9" customWidth="1"/>
-    <col min="6" max="7" width="15.85546875" style="5" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" style="12" customWidth="1"/>
-    <col min="9" max="9" width="65.28515625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="97.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" customWidth="1"/>
-    <col min="13" max="13" width="47.28515625" customWidth="1"/>
-    <col min="15" max="15" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" customWidth="1"/>
+    <col min="7" max="7" width="32" style="9" customWidth="1"/>
+    <col min="8" max="9" width="15.85546875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" style="12" customWidth="1"/>
+    <col min="11" max="11" width="65.28515625" style="7" customWidth="1"/>
+    <col min="12" max="12" width="97.7109375" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" customWidth="1"/>
+    <col min="15" max="15" width="47.28515625" customWidth="1"/>
+    <col min="17" max="17" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M1" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1" s="13" t="s">
+      <c r="N1" t="s">
         <v>82</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="O1" t="s">
+        <v>83</v>
+      </c>
+      <c r="P1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="124.5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="9">
+        <v>40807</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="K1" t="s">
-        <v>86</v>
-      </c>
-      <c r="L1" t="s">
-        <v>87</v>
-      </c>
-      <c r="M1" t="s">
-        <v>88</v>
-      </c>
-      <c r="N1" t="s">
-        <v>89</v>
-      </c>
-      <c r="O1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="124.5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="9">
-        <v>40807</v>
-      </c>
-      <c r="F2" s="5">
-        <v>0.85416666666666663</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="90.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:17" ht="90.75" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="9">
+      <c r="E3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="9">
         <v>40811</v>
       </c>
-      <c r="F3" s="5">
+      <c r="H3" s="5">
         <v>0.85763888888888884</v>
       </c>
-      <c r="H3" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="57" x14ac:dyDescent="0.25">
+      <c r="J3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="57" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A12" si="0">A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="9">
+      <c r="E4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="9">
         <v>40812</v>
       </c>
-      <c r="F4" s="4">
+      <c r="H4" s="4">
         <v>0.9375</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="248.25" x14ac:dyDescent="0.25">
+      <c r="I4" s="4"/>
+      <c r="J4" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="248.25" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="G5" s="9">
+        <v>40812</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="9">
-        <v>40812</v>
-      </c>
-      <c r="F5" s="5">
-        <v>0.89583333333333337</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="203.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:17" ht="203.25" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="G6" s="9">
+        <v>40807</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0.8125</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="9">
-        <v>40807</v>
-      </c>
-      <c r="F6" s="5">
-        <v>0.8125</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="158.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:17" ht="158.25" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>34</v>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="9">
+        <v>16</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="9">
         <v>40807</v>
       </c>
-      <c r="F7" s="5">
+      <c r="H7" s="5">
         <v>0.83333333333333337</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="113.25" x14ac:dyDescent="0.25">
+      <c r="I7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="113.25" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>39</v>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
       </c>
       <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="9">
+        <v>40807</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="9">
-        <v>40807</v>
-      </c>
-      <c r="F8" s="5">
-        <v>0.85416666666666663</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="409.6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:17" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="9">
+        <v>40808</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="J9" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="9">
-        <v>40808</v>
-      </c>
-      <c r="F9" s="5">
-        <v>0.375</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="K9" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>48</v>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="9">
+        <v>39</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="9">
         <v>40807</v>
       </c>
-      <c r="F10" s="5">
+      <c r="H10" s="5">
         <v>0.85416666666666663</v>
       </c>
-      <c r="H10" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="225.75" x14ac:dyDescent="0.25">
+      <c r="J10" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="225.75" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>53</v>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="9">
+        <v>39</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="9">
         <v>40809</v>
       </c>
-      <c r="F11" s="5">
+      <c r="H11" s="5">
         <v>0.66666666666666663</v>
       </c>
-      <c r="H11" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="315.75" x14ac:dyDescent="0.25">
+      <c r="J11" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="315.75" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>56</v>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="9">
+        <v>39</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="9">
         <v>40810</v>
       </c>
-      <c r="F12" s="5">
+      <c r="H12" s="5">
         <v>0.42708333333333331</v>
       </c>
-      <c r="H12" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>57</v>
+      <c r="J12" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J3" r:id="rId1"/>
-    <hyperlink ref="J4" r:id="rId2"/>
-    <hyperlink ref="J5" r:id="rId3"/>
-    <hyperlink ref="J6" r:id="rId4"/>
-    <hyperlink ref="J8" r:id="rId5"/>
+    <hyperlink ref="L3" r:id="rId1"/>
+    <hyperlink ref="L4" r:id="rId2"/>
+    <hyperlink ref="L5" r:id="rId3"/>
+    <hyperlink ref="L6" r:id="rId4"/>
+    <hyperlink ref="L8" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>

</xml_diff>

<commit_message>
Display of date and event name in listview from sqlite db.
Added image(hardcoded for now) to vertical list row layout.
</commit_message>
<xml_diff>
--- a/data/EventData.xlsx
+++ b/data/EventData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="WBS" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="96">
   <si>
     <t>Movies</t>
   </si>
@@ -256,9 +256,6 @@
     <t>Play youtube videos from app/emulator</t>
   </si>
   <si>
-    <t>abstract data provider to be able to plugin more dynamic content later</t>
-  </si>
-  <si>
     <t>Source sample Content(Event, Images, Videos, Recommended, BuyThis)</t>
   </si>
   <si>
@@ -359,6 +356,18 @@
   </si>
   <si>
     <t>buy_rec_id</t>
+  </si>
+  <si>
+    <t>banner_30rock.jpg</t>
+  </si>
+  <si>
+    <t>buy_box_office.jpeg</t>
+  </si>
+  <si>
+    <t>DatabaseHelper to access SQLite db</t>
+  </si>
+  <si>
+    <t>Content Provider to abstract data layer</t>
   </si>
 </sst>
 </file>
@@ -776,10 +785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C16"/>
+  <dimension ref="B2:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,10 +799,10 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
@@ -801,7 +810,7 @@
         <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
@@ -814,74 +823,82 @@
         <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>58</v>
+        <v>94</v>
+      </c>
+      <c r="C7" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>62</v>
+        <v>71</v>
+      </c>
+      <c r="C9" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>61</v>
       </c>
-      <c r="C10" t="s">
-        <v>68</v>
-      </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>65</v>
+        <v>60</v>
+      </c>
+      <c r="C11" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>75</v>
+        <v>68</v>
+      </c>
+      <c r="C16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -893,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,63 +926,63 @@
     <col min="10" max="10" width="15.85546875" style="12" customWidth="1"/>
     <col min="11" max="11" width="65.28515625" style="7" customWidth="1"/>
     <col min="12" max="12" width="97.7109375" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" customWidth="1"/>
-    <col min="14" max="14" width="16.28515625" customWidth="1"/>
+    <col min="13" max="13" width="41.5703125" customWidth="1"/>
+    <col min="14" max="14" width="23.5703125" customWidth="1"/>
     <col min="15" max="15" width="47.28515625" customWidth="1"/>
     <col min="17" max="17" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="13" t="s">
+      <c r="G1" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="L1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" t="s">
         <v>80</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>81</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>82</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>83</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>84</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="124.5" x14ac:dyDescent="0.25">
@@ -1001,6 +1018,12 @@
       </c>
       <c r="L2" t="s">
         <v>2</v>
+      </c>
+      <c r="M2" t="s">
+        <v>92</v>
+      </c>
+      <c r="N2" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="90.75" x14ac:dyDescent="0.25">
@@ -1038,6 +1061,12 @@
       <c r="L3" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="M3" t="s">
+        <v>92</v>
+      </c>
+      <c r="N3" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="4" spans="1:17" ht="57" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1075,6 +1104,12 @@
       <c r="L4" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="M4" t="s">
+        <v>92</v>
+      </c>
+      <c r="N4" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="5" spans="1:17" ht="248.25" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -1114,6 +1149,12 @@
       <c r="L5" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="M5" t="s">
+        <v>92</v>
+      </c>
+      <c r="N5" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="6" spans="1:17" ht="203.25" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1153,6 +1194,12 @@
       <c r="L6" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="M6" t="s">
+        <v>92</v>
+      </c>
+      <c r="N6" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="7" spans="1:17" ht="158.25" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1189,6 +1236,12 @@
       <c r="K7" s="7" t="s">
         <v>37</v>
       </c>
+      <c r="M7" t="s">
+        <v>92</v>
+      </c>
+      <c r="N7" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="8" spans="1:17" ht="113.25" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1228,6 +1281,12 @@
       <c r="L8" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="M8" t="s">
+        <v>92</v>
+      </c>
+      <c r="N8" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="9" spans="1:17" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -1261,6 +1320,12 @@
       <c r="K9" s="7" t="s">
         <v>42</v>
       </c>
+      <c r="M9" t="s">
+        <v>92</v>
+      </c>
+      <c r="N9" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="10" spans="1:17" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1294,6 +1359,12 @@
       <c r="K10" s="7" t="s">
         <v>46</v>
       </c>
+      <c r="M10" t="s">
+        <v>92</v>
+      </c>
+      <c r="N10" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="11" spans="1:17" ht="225.75" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1327,6 +1398,12 @@
       <c r="K11" s="7" t="s">
         <v>51</v>
       </c>
+      <c r="M11" t="s">
+        <v>92</v>
+      </c>
+      <c r="N11" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="12" spans="1:17" ht="315.75" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1359,6 +1436,12 @@
       </c>
       <c r="K12" s="7" t="s">
         <v>53</v>
+      </c>
+      <c r="M12" t="s">
+        <v>92</v>
+      </c>
+      <c r="N12" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
display image for view recommendation
1. Image stored in SD card(mnt/sdcard/WhatsON_Images)
2. Image name stored in sqlite db
</commit_message>
<xml_diff>
--- a/data/EventData.xlsx
+++ b/data/EventData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="WBS" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="249">
   <si>
     <t>Movies</t>
   </si>
@@ -58,10 +58,6 @@
   </si>
   <si>
     <t>A Texas Ranger works with a State Trooper to take down a dangerous arms dealer.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Lone Wolf McQuade</t>
   </si>
   <si>
     <t>http://www.youtube.com/watch?v=k0DA75eOltA&amp;feature=player_embedded</t>
@@ -342,12 +338,6 @@
     <t>buy_rec_id</t>
   </si>
   <si>
-    <t>banner_30rock.jpg</t>
-  </si>
-  <si>
-    <t>buy_box_office.jpeg</t>
-  </si>
-  <si>
     <t>DatabaseHelper to access SQLite db</t>
   </si>
   <si>
@@ -748,6 +738,96 @@
   </si>
   <si>
     <t>Recommended Events Long Description 11</t>
+  </si>
+  <si>
+    <t>Connects to db. Now to "pretty" it up with images and a good layout.</t>
+  </si>
+  <si>
+    <t>Not Started</t>
+  </si>
+  <si>
+    <t>Can do this once the core app is working/finished</t>
+  </si>
+  <si>
+    <t>POC saving images on SD card and image id in db. Then display image.</t>
+  </si>
+  <si>
+    <t>Now to implement wherever images need to be displayed. NB: Might also want to use adapter and gallery/coverflow widgets. (Nice to have)</t>
+  </si>
+  <si>
+    <t>Nice to have for buy recommendations if we finish everything else</t>
+  </si>
+  <si>
+    <t>Vaugan/Satya</t>
+  </si>
+  <si>
+    <t>ddaily093.jpg</t>
+  </si>
+  <si>
+    <t>Lone Wolf McQuade</t>
+  </si>
+  <si>
+    <t>ddaily094.jpg</t>
+  </si>
+  <si>
+    <t>ddaily095.jpg</t>
+  </si>
+  <si>
+    <t>ddaily096.jpg</t>
+  </si>
+  <si>
+    <t>ddaily097.jpg</t>
+  </si>
+  <si>
+    <t>ddaily098.jpg</t>
+  </si>
+  <si>
+    <t>ddaily099.jpg</t>
+  </si>
+  <si>
+    <t>ddaily100.jpg</t>
+  </si>
+  <si>
+    <t>ddaily092.jpg</t>
+  </si>
+  <si>
+    <t>ddaily091.jpg</t>
+  </si>
+  <si>
+    <t>ddaily101.jpg</t>
+  </si>
+  <si>
+    <t>ddaily102.jpg</t>
+  </si>
+  <si>
+    <t>ddaily103.jpg</t>
+  </si>
+  <si>
+    <t>ddaily104.jpg</t>
+  </si>
+  <si>
+    <t>ddaily105.jpg</t>
+  </si>
+  <si>
+    <t>ddaily106.jpg</t>
+  </si>
+  <si>
+    <t>ddaily107.jpg</t>
+  </si>
+  <si>
+    <t>ddaily108.jpg</t>
+  </si>
+  <si>
+    <t>ddaily109.jpg</t>
+  </si>
+  <si>
+    <t>ddaily110.jpg</t>
+  </si>
+  <si>
+    <t>ddaily111.jpg</t>
+  </si>
+  <si>
+    <t>ddaily112.jpg</t>
   </si>
 </sst>
 </file>
@@ -861,7 +941,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -926,6 +1006,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1231,7 +1319,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1246,22 +1334,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="F1" s="21" t="s">
         <v>91</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1269,19 +1357,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D2" s="19">
         <v>50</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1290,19 +1378,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>67</v>
+        <v>225</v>
       </c>
       <c r="D3" s="19">
         <v>50</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1311,16 +1399,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D4" s="23">
         <v>100</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F4" s="24"/>
     </row>
@@ -1330,19 +1418,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D5" s="19">
         <v>10</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1351,40 +1439,40 @@
         <v>5</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6" s="19">
         <v>50</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="19">
+      <c r="A7" s="23">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="19">
-        <v>50</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>104</v>
+      <c r="B7" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="23">
+        <v>100</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1393,16 +1481,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D8" s="19">
         <v>0</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F8" s="22"/>
     </row>
@@ -1412,10 +1500,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D9" s="19">
         <v>0</v>
@@ -1429,7 +1517,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C10" s="16"/>
       <c r="D10" s="19">
@@ -1444,17 +1532,17 @@
         <v>10</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D11" s="19">
         <v>0</v>
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="22" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1463,16 +1551,18 @@
         <v>11</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D12" s="19">
         <v>80</v>
       </c>
       <c r="E12" s="19"/>
-      <c r="F12" s="22"/>
+      <c r="F12" s="22" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="19">
@@ -1480,16 +1570,18 @@
         <v>12</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D13" s="19">
         <v>80</v>
       </c>
       <c r="E13" s="19"/>
-      <c r="F13" s="22"/>
+      <c r="F13" s="22" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
@@ -1497,10 +1589,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D14" s="19">
         <v>80</v>
@@ -1514,15 +1606,17 @@
         <v>14</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D15" s="19">
         <v>0</v>
       </c>
-      <c r="E15" s="19"/>
+      <c r="E15" s="19" t="s">
+        <v>108</v>
+      </c>
       <c r="F15" s="22"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1531,14 +1625,18 @@
         <v>15</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="19">
         <v>0</v>
       </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="22"/>
+      <c r="E16" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="23">
@@ -1546,19 +1644,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D17" s="23">
         <v>100</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F17" s="24" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1567,19 +1665,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D18" s="19">
         <v>80</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F18" s="22" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1588,13 +1686,34 @@
         <v>18</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="19">
+        <v>137</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="23">
         <f t="shared" si="0"/>
         <v>19</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="28">
+        <v>100</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="F20" s="29" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1625,8 +1744,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="F13" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection activeCell="F1" sqref="F1"/>
+      <selection pane="topRight" activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1649,58 +1770,58 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F1" s="13" t="s">
+      <c r="H1" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K1" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="K1" s="11" t="s">
+      <c r="L1" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="M1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" t="s">
         <v>73</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>74</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>75</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>76</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>77</v>
-      </c>
-      <c r="R1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="124.5" x14ac:dyDescent="0.25">
@@ -1720,7 +1841,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>12</v>
+        <v>227</v>
       </c>
       <c r="G2" t="s">
         <v>1</v>
@@ -1741,10 +1862,10 @@
         <v>2</v>
       </c>
       <c r="N2" t="s">
-        <v>86</v>
+        <v>236</v>
       </c>
       <c r="O2" t="s">
-        <v>87</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="90.75" x14ac:dyDescent="0.25">
@@ -1783,13 +1904,13 @@
         <v>4</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N3" t="s">
-        <v>86</v>
+        <v>235</v>
       </c>
       <c r="O3" t="s">
-        <v>87</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="57" x14ac:dyDescent="0.25">
@@ -1826,16 +1947,16 @@
         <v>8</v>
       </c>
       <c r="L4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M4" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="N4" t="s">
-        <v>86</v>
+        <v>226</v>
       </c>
       <c r="O4" t="s">
-        <v>87</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="248.25" x14ac:dyDescent="0.25">
@@ -1853,13 +1974,13 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
         <v>18</v>
-      </c>
-      <c r="G5" t="s">
-        <v>19</v>
       </c>
       <c r="H5" s="9">
         <v>40812</v>
@@ -1868,22 +1989,22 @@
         <v>0.89583333333333337</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M5" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="N5" t="s">
-        <v>86</v>
+        <v>228</v>
       </c>
       <c r="O5" t="s">
-        <v>87</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="203.25" x14ac:dyDescent="0.25">
@@ -1901,13 +2022,13 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H6" s="9">
         <v>40807</v>
@@ -1916,22 +2037,22 @@
         <v>0.8125</v>
       </c>
       <c r="J6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="L6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="M6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="M6" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="N6" t="s">
-        <v>86</v>
+        <v>229</v>
       </c>
       <c r="O6" t="s">
-        <v>87</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="158.25" x14ac:dyDescent="0.25">
@@ -1949,13 +2070,13 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" t="s">
         <v>30</v>
-      </c>
-      <c r="G7" t="s">
-        <v>31</v>
       </c>
       <c r="H7" s="9">
         <v>40807</v>
@@ -1964,19 +2085,19 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N7" t="s">
-        <v>86</v>
+        <v>230</v>
       </c>
       <c r="O7" t="s">
-        <v>87</v>
+        <v>230</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="113.25" x14ac:dyDescent="0.25">
@@ -1994,13 +2115,13 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H8" s="9">
         <v>40807</v>
@@ -2009,22 +2130,22 @@
         <v>0.85416666666666663</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N8" t="s">
-        <v>86</v>
+        <v>231</v>
       </c>
       <c r="O8" t="s">
-        <v>87</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="409.6" x14ac:dyDescent="0.25">
@@ -2042,13 +2163,13 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="G9" t="s">
         <v>40</v>
-      </c>
-      <c r="G9" t="s">
-        <v>41</v>
       </c>
       <c r="H9" s="9">
         <v>40808</v>
@@ -2057,16 +2178,16 @@
         <v>0.375</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N9" t="s">
-        <v>86</v>
+        <v>232</v>
       </c>
       <c r="O9" t="s">
-        <v>87</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="409.6" x14ac:dyDescent="0.25">
@@ -2084,13 +2205,13 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" t="s">
         <v>44</v>
-      </c>
-      <c r="G10" t="s">
-        <v>45</v>
       </c>
       <c r="H10" s="9">
         <v>40807</v>
@@ -2099,16 +2220,16 @@
         <v>0.85416666666666663</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N10" t="s">
-        <v>86</v>
+        <v>233</v>
       </c>
       <c r="O10" t="s">
-        <v>87</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="225.75" x14ac:dyDescent="0.25">
@@ -2126,13 +2247,13 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" t="s">
         <v>49</v>
-      </c>
-      <c r="G11" t="s">
-        <v>50</v>
       </c>
       <c r="H11" s="9">
         <v>40809</v>
@@ -2141,16 +2262,16 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N11" t="s">
-        <v>86</v>
+        <v>234</v>
       </c>
       <c r="O11" t="s">
-        <v>87</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="315.75" x14ac:dyDescent="0.25">
@@ -2168,13 +2289,13 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H12" s="9">
         <v>40810</v>
@@ -2183,16 +2304,16 @@
         <v>0.42708333333333331</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N12" t="s">
-        <v>86</v>
+        <v>237</v>
       </c>
       <c r="O12" t="s">
-        <v>87</v>
+        <v>237</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -2210,13 +2331,13 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G13" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H13" s="9">
         <v>40811</v>
@@ -2225,10 +2346,16 @@
         <v>0.46875</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>211</v>
+        <v>208</v>
+      </c>
+      <c r="N13" t="s">
+        <v>238</v>
+      </c>
+      <c r="O13" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -2246,13 +2373,13 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="G14" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H14" s="9">
         <v>40812</v>
@@ -2261,10 +2388,16 @@
         <v>0.51041666666666696</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>212</v>
+        <v>209</v>
+      </c>
+      <c r="N14" t="s">
+        <v>239</v>
+      </c>
+      <c r="O14" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -2282,13 +2415,13 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
+        <v>174</v>
+      </c>
+      <c r="F15" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>180</v>
-      </c>
       <c r="G15" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="H15" s="9">
         <v>40813</v>
@@ -2297,10 +2430,16 @@
         <v>0.55208333333333304</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>213</v>
+        <v>210</v>
+      </c>
+      <c r="N15" t="s">
+        <v>240</v>
+      </c>
+      <c r="O15" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -2318,13 +2457,13 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="G16" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="H16" s="9">
         <v>40814</v>
@@ -2333,13 +2472,19 @@
         <v>0.59375</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+      <c r="N16" t="s">
+        <v>241</v>
+      </c>
+      <c r="O16" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2354,13 +2499,13 @@
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G17" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="H17" s="9">
         <v>40815</v>
@@ -2369,13 +2514,19 @@
         <v>0.63541666666666696</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N17" t="s">
+        <v>242</v>
+      </c>
+      <c r="O17" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2390,13 +2541,13 @@
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G18" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H18" s="9">
         <v>40816</v>
@@ -2405,13 +2556,19 @@
         <v>0.67708333333333304</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+      <c r="N18" t="s">
+        <v>243</v>
+      </c>
+      <c r="O18" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2426,13 +2583,13 @@
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G19" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H19" s="9">
         <v>40817</v>
@@ -2441,13 +2598,19 @@
         <v>0.71875</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+      <c r="N19" t="s">
+        <v>244</v>
+      </c>
+      <c r="O19" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2462,13 +2625,13 @@
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G20" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="H20" s="9">
         <v>40818</v>
@@ -2477,13 +2640,19 @@
         <v>0.76041666666666696</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="L20" s="7" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+      <c r="N20" t="s">
+        <v>245</v>
+      </c>
+      <c r="O20" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2498,13 +2667,13 @@
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G21" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H21" s="9">
         <v>40819</v>
@@ -2513,13 +2682,19 @@
         <v>0.80208333333333304</v>
       </c>
       <c r="K21" s="12" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+      <c r="N21" t="s">
+        <v>246</v>
+      </c>
+      <c r="O21" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2534,13 +2709,13 @@
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G22" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H22" s="9">
         <v>40820</v>
@@ -2549,13 +2724,19 @@
         <v>0.84375</v>
       </c>
       <c r="K22" s="12" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="L22" s="7" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+      <c r="N22" t="s">
+        <v>247</v>
+      </c>
+      <c r="O22" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2570,13 +2751,13 @@
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G23" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H23" s="9">
         <v>40821</v>
@@ -2585,10 +2766,16 @@
         <v>0.88541666666666696</v>
       </c>
       <c r="K23" s="12" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="L23" s="7" t="s">
-        <v>221</v>
+        <v>218</v>
+      </c>
+      <c r="N23" t="s">
+        <v>248</v>
+      </c>
+      <c r="O23" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -2608,7 +2795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
@@ -2621,37 +2808,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" t="s">
         <v>115</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>116</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>117</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>118</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>119</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>120</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>121</v>
-      </c>
-      <c r="I1" t="s">
-        <v>122</v>
-      </c>
-      <c r="J1" t="s">
-        <v>123</v>
-      </c>
-      <c r="K1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2995,37 +3182,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" t="s">
         <v>125</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>126</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>127</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>128</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>129</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>130</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>131</v>
-      </c>
-      <c r="I1" t="s">
-        <v>132</v>
-      </c>
-      <c r="J1" t="s">
-        <v>133</v>
-      </c>
-      <c r="K1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -3188,25 +3375,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G1" t="s">
         <v>135</v>
-      </c>
-      <c r="C1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F1" t="s">
-        <v>141</v>
-      </c>
-      <c r="G1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3214,16 +3401,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2">
         <v>150</v>
       </c>
       <c r="F2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3232,16 +3419,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3">
         <v>150</v>
       </c>
       <c r="F3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -3250,16 +3437,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D4">
         <v>150</v>
       </c>
       <c r="F4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -3268,16 +3455,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" t="s">
         <v>145</v>
-      </c>
-      <c r="C5" t="s">
-        <v>148</v>
       </c>
       <c r="D5">
         <v>150</v>
       </c>
       <c r="F5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -3286,16 +3473,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C6" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D6">
         <v>150</v>
       </c>
       <c r="F6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -3304,16 +3491,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C7" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D7">
         <v>129</v>
       </c>
       <c r="F7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -3322,16 +3509,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D8">
         <v>129</v>
       </c>
       <c r="F8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -3340,16 +3527,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D9">
         <v>129</v>
       </c>
       <c r="F9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -3358,16 +3545,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C10" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D10">
         <v>129</v>
       </c>
       <c r="F10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -3376,16 +3563,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C11" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D11">
         <v>129</v>
       </c>
       <c r="F11" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -3394,16 +3581,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C12" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D12">
         <v>99</v>
       </c>
       <c r="F12" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -3412,16 +3599,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D13">
         <v>99</v>
       </c>
       <c r="F13" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -3430,16 +3617,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C14" t="s">
         <v>155</v>
-      </c>
-      <c r="C14" t="s">
-        <v>158</v>
       </c>
       <c r="D14">
         <v>99</v>
       </c>
       <c r="F14" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -3448,16 +3635,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C15" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D15">
         <v>99</v>
       </c>
       <c r="F15" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -3466,16 +3653,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D16">
         <v>99</v>
       </c>
       <c r="F16" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -3484,16 +3671,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C17" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D17">
         <v>99</v>
       </c>
       <c r="F17" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -3502,16 +3689,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C18" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D18">
         <v>99</v>
       </c>
       <c r="F18" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -3520,232 +3707,232 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C19" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D19">
         <v>99</v>
       </c>
       <c r="F19" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f>A19+1</f>
+        <f t="shared" ref="A20:A31" si="1">A19+1</f>
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C20" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D20">
         <v>99</v>
       </c>
       <c r="F20" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f>A20+1</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C21" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D21">
         <v>99</v>
       </c>
       <c r="F21" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f>A21+1</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C22" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D22">
         <v>25</v>
       </c>
       <c r="F22" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f>A22+1</f>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C23" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D23">
         <v>25</v>
       </c>
       <c r="F23" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f>A23+1</f>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>163</v>
+      </c>
+      <c r="C24" t="s">
         <v>166</v>
-      </c>
-      <c r="C24" t="s">
-        <v>169</v>
       </c>
       <c r="D24">
         <v>25</v>
       </c>
       <c r="F24" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f>A24+1</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C25" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D25">
         <v>25</v>
       </c>
       <c r="F25" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f>A25+1</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C26" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D26">
         <v>25</v>
       </c>
       <c r="F26" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f>A26+1</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C27" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D27">
         <v>25</v>
       </c>
       <c r="F27" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f>A27+1</f>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C28" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D28">
         <v>25</v>
       </c>
       <c r="F28" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f>A28+1</f>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C29" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D29">
         <v>25</v>
       </c>
       <c r="F29" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f>A29+1</f>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C30" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D30">
         <v>25</v>
       </c>
       <c r="F30" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f>A30+1</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C31" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D31">
         <v>25</v>
       </c>
       <c r="F31" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added category field to db
</commit_message>
<xml_diff>
--- a/data/EventData.xlsx
+++ b/data/EventData.xlsx
@@ -13,12 +13,12 @@
     <sheet name="BuyRecommendations" sheetId="4" r:id="rId4"/>
     <sheet name="BuyData" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="250">
   <si>
     <t>Movies</t>
   </si>
@@ -828,6 +828,9 @@
   </si>
   <si>
     <t>ddaily112.jpg</t>
+  </si>
+  <si>
+    <t>category</t>
   </si>
 </sst>
 </file>
@@ -1742,33 +1745,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F13" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection activeCell="F1" sqref="F1"/>
-      <selection pane="topRight" activeCell="N31" sqref="N31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" customWidth="1"/>
-    <col min="8" max="8" width="32" style="9" customWidth="1"/>
-    <col min="9" max="10" width="15.85546875" style="5" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" style="12" customWidth="1"/>
-    <col min="12" max="12" width="65.28515625" style="7" customWidth="1"/>
-    <col min="13" max="13" width="97.7109375" customWidth="1"/>
-    <col min="14" max="14" width="41.5703125" customWidth="1"/>
-    <col min="15" max="15" width="23.5703125" customWidth="1"/>
-    <col min="16" max="16" width="47.28515625" customWidth="1"/>
-    <col min="18" max="18" width="15.5703125" customWidth="1"/>
+    <col min="3" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="24.85546875" customWidth="1"/>
+    <col min="9" max="9" width="32" style="9" customWidth="1"/>
+    <col min="10" max="11" width="15.85546875" style="5" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" style="12" customWidth="1"/>
+    <col min="13" max="13" width="65.28515625" style="7" customWidth="1"/>
+    <col min="14" max="14" width="97.7109375" customWidth="1"/>
+    <col min="15" max="15" width="41.5703125" customWidth="1"/>
+    <col min="16" max="16" width="23.5703125" customWidth="1"/>
+    <col min="17" max="17" width="47.28515625" customWidth="1"/>
+    <col min="19" max="19" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>78</v>
       </c>
@@ -1781,50 +1782,53 @@
       <c r="D1" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
+        <v>249</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="M1" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>73</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>74</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>75</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>76</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="124.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="124.5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1840,35 +1844,38 @@
       <c r="E2" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="9">
+      <c r="I2" s="9">
         <v>40807</v>
       </c>
-      <c r="I2" s="5">
+      <c r="J2" s="5">
         <v>0.85416666666666663</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="L2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="M2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>2</v>
-      </c>
-      <c r="N2" t="s">
-        <v>236</v>
       </c>
       <c r="O2" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" ht="90.75" x14ac:dyDescent="0.25">
+      <c r="P2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="90.75" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -1885,35 +1892,38 @@
       <c r="E3" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="9">
+      <c r="I3" s="9">
         <v>40811</v>
       </c>
-      <c r="I3" s="5">
+      <c r="J3" s="5">
         <v>0.85763888888888884</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="L3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="M3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="N3" t="s">
-        <v>235</v>
       </c>
       <c r="O3" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" ht="57" x14ac:dyDescent="0.25">
+      <c r="P3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="57" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A23" si="0">A3+1</f>
         <v>3</v>
@@ -1930,36 +1940,39 @@
       <c r="E4" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="9">
+      <c r="I4" s="9">
         <v>40812</v>
       </c>
-      <c r="I4" s="4">
+      <c r="J4" s="4">
         <v>0.9375</v>
       </c>
-      <c r="J4" s="4"/>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="4"/>
+      <c r="L4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="M4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="N4" t="s">
-        <v>226</v>
       </c>
       <c r="O4" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" ht="248.25" x14ac:dyDescent="0.25">
+      <c r="P4" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="248.25" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1976,38 +1989,41 @@
       <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="9">
+      <c r="I5" s="9">
         <v>40812</v>
       </c>
-      <c r="I5" s="5">
+      <c r="J5" s="5">
         <v>0.89583333333333337</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="L5" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="M5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="N5" t="s">
-        <v>228</v>
       </c>
       <c r="O5" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" ht="203.25" x14ac:dyDescent="0.25">
+      <c r="P5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="203.25" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2024,38 +2040,41 @@
       <c r="E6" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="9">
+      <c r="I6" s="9">
         <v>40807</v>
       </c>
-      <c r="I6" s="5">
+      <c r="J6" s="5">
         <v>0.8125</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="K6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="L6" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="M6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="N6" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="N6" t="s">
-        <v>229</v>
       </c>
       <c r="O6" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" ht="158.25" x14ac:dyDescent="0.25">
+      <c r="P6" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="158.25" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2072,35 +2091,38 @@
       <c r="E7" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="9">
+      <c r="I7" s="9">
         <v>40807</v>
       </c>
-      <c r="I7" s="5">
+      <c r="J7" s="5">
         <v>0.83333333333333337</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="K7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="L7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="M7" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="N7" t="s">
-        <v>230</v>
       </c>
       <c r="O7" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" ht="113.25" x14ac:dyDescent="0.25">
+      <c r="P7" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="113.25" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2117,38 +2139,41 @@
       <c r="E8" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="9">
+      <c r="I8" s="9">
         <v>40807</v>
       </c>
-      <c r="I8" s="5">
+      <c r="J8" s="5">
         <v>0.85416666666666663</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="K8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="12" t="s">
+      <c r="L8" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="M8" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="N8" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="N8" t="s">
-        <v>231</v>
       </c>
       <c r="O8" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="P8" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2165,32 +2190,35 @@
       <c r="E9" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="9">
+      <c r="I9" s="9">
         <v>40808</v>
       </c>
-      <c r="I9" s="5">
+      <c r="J9" s="5">
         <v>0.375</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="L9" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="L9" s="7" t="s">
+      <c r="M9" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="N9" t="s">
-        <v>232</v>
       </c>
       <c r="O9" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="P9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2207,32 +2235,35 @@
       <c r="E10" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>44</v>
       </c>
-      <c r="H10" s="9">
+      <c r="I10" s="9">
         <v>40807</v>
       </c>
-      <c r="I10" s="5">
+      <c r="J10" s="5">
         <v>0.85416666666666663</v>
       </c>
-      <c r="K10" s="12" t="s">
+      <c r="L10" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="L10" s="7" t="s">
+      <c r="M10" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="N10" t="s">
-        <v>233</v>
       </c>
       <c r="O10" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" ht="225.75" x14ac:dyDescent="0.25">
+      <c r="P10" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="225.75" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2249,32 +2280,35 @@
       <c r="E11" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>49</v>
       </c>
-      <c r="H11" s="9">
+      <c r="I11" s="9">
         <v>40809</v>
       </c>
-      <c r="I11" s="5">
+      <c r="J11" s="5">
         <v>0.66666666666666663</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="L11" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="L11" s="7" t="s">
+      <c r="M11" s="7" t="s">
         <v>50</v>
-      </c>
-      <c r="N11" t="s">
-        <v>234</v>
       </c>
       <c r="O11" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" ht="315.75" x14ac:dyDescent="0.25">
+      <c r="P11" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="315.75" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2291,32 +2325,35 @@
       <c r="E12" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="9">
+      <c r="I12" s="9">
         <v>40810</v>
       </c>
-      <c r="I12" s="5">
+      <c r="J12" s="5">
         <v>0.42708333333333331</v>
       </c>
-      <c r="K12" s="12" t="s">
+      <c r="L12" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="L12" s="7" t="s">
+      <c r="M12" s="7" t="s">
         <v>52</v>
-      </c>
-      <c r="N12" t="s">
-        <v>237</v>
       </c>
       <c r="O12" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2330,35 +2367,35 @@
       <c r="D13" t="b">
         <v>0</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>174</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="G13" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>186</v>
       </c>
-      <c r="H13" s="9">
+      <c r="I13" s="9">
         <v>40811</v>
       </c>
-      <c r="I13" s="5">
+      <c r="J13" s="5">
         <v>0.46875</v>
       </c>
-      <c r="K13" s="12" t="s">
+      <c r="L13" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="L13" s="7" t="s">
+      <c r="M13" s="7" t="s">
         <v>208</v>
-      </c>
-      <c r="N13" t="s">
-        <v>238</v>
       </c>
       <c r="O13" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P13" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2372,35 +2409,35 @@
       <c r="D14" t="b">
         <v>0</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>174</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="G14" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>187</v>
       </c>
-      <c r="H14" s="9">
+      <c r="I14" s="9">
         <v>40812</v>
       </c>
-      <c r="I14" s="5">
+      <c r="J14" s="5">
         <v>0.51041666666666696</v>
       </c>
-      <c r="K14" s="12" t="s">
+      <c r="L14" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="L14" s="7" t="s">
+      <c r="M14" s="7" t="s">
         <v>209</v>
-      </c>
-      <c r="N14" t="s">
-        <v>239</v>
       </c>
       <c r="O14" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P14" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2414,35 +2451,35 @@
       <c r="D15" t="b">
         <v>0</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>174</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="G15" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>188</v>
       </c>
-      <c r="H15" s="9">
+      <c r="I15" s="9">
         <v>40813</v>
       </c>
-      <c r="I15" s="5">
+      <c r="J15" s="5">
         <v>0.55208333333333304</v>
       </c>
-      <c r="K15" s="12" t="s">
+      <c r="L15" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="L15" s="7" t="s">
+      <c r="M15" s="7" t="s">
         <v>210</v>
-      </c>
-      <c r="N15" t="s">
-        <v>240</v>
       </c>
       <c r="O15" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P15" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2456,35 +2493,35 @@
       <c r="D16" t="b">
         <v>0</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>174</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="G16" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>189</v>
       </c>
-      <c r="H16" s="9">
+      <c r="I16" s="9">
         <v>40814</v>
       </c>
-      <c r="I16" s="5">
+      <c r="J16" s="5">
         <v>0.59375</v>
       </c>
-      <c r="K16" s="12" t="s">
+      <c r="L16" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="L16" s="7" t="s">
+      <c r="M16" s="7" t="s">
         <v>211</v>
-      </c>
-      <c r="N16" t="s">
-        <v>241</v>
       </c>
       <c r="O16" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P16" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2498,35 +2535,35 @@
       <c r="D17" t="b">
         <v>0</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>174</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="G17" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>190</v>
       </c>
-      <c r="H17" s="9">
+      <c r="I17" s="9">
         <v>40815</v>
       </c>
-      <c r="I17" s="5">
+      <c r="J17" s="5">
         <v>0.63541666666666696</v>
       </c>
-      <c r="K17" s="12" t="s">
+      <c r="L17" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="L17" s="7" t="s">
+      <c r="M17" s="7" t="s">
         <v>212</v>
-      </c>
-      <c r="N17" t="s">
-        <v>242</v>
       </c>
       <c r="O17" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P17" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2540,35 +2577,35 @@
       <c r="D18" t="b">
         <v>0</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>174</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="G18" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>191</v>
       </c>
-      <c r="H18" s="9">
+      <c r="I18" s="9">
         <v>40816</v>
       </c>
-      <c r="I18" s="5">
+      <c r="J18" s="5">
         <v>0.67708333333333304</v>
       </c>
-      <c r="K18" s="12" t="s">
+      <c r="L18" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="L18" s="7" t="s">
+      <c r="M18" s="7" t="s">
         <v>213</v>
-      </c>
-      <c r="N18" t="s">
-        <v>243</v>
       </c>
       <c r="O18" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P18" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2582,35 +2619,35 @@
       <c r="D19" t="b">
         <v>0</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>174</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="G19" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>192</v>
       </c>
-      <c r="H19" s="9">
+      <c r="I19" s="9">
         <v>40817</v>
       </c>
-      <c r="I19" s="5">
+      <c r="J19" s="5">
         <v>0.71875</v>
       </c>
-      <c r="K19" s="12" t="s">
+      <c r="L19" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="L19" s="7" t="s">
+      <c r="M19" s="7" t="s">
         <v>214</v>
-      </c>
-      <c r="N19" t="s">
-        <v>244</v>
       </c>
       <c r="O19" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P19" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2624,35 +2661,35 @@
       <c r="D20" t="b">
         <v>0</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>174</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="G20" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>193</v>
       </c>
-      <c r="H20" s="9">
+      <c r="I20" s="9">
         <v>40818</v>
       </c>
-      <c r="I20" s="5">
+      <c r="J20" s="5">
         <v>0.76041666666666696</v>
       </c>
-      <c r="K20" s="12" t="s">
+      <c r="L20" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="L20" s="7" t="s">
+      <c r="M20" s="7" t="s">
         <v>215</v>
-      </c>
-      <c r="N20" t="s">
-        <v>245</v>
       </c>
       <c r="O20" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P20" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2666,35 +2703,35 @@
       <c r="D21" t="b">
         <v>0</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>174</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="G21" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>194</v>
       </c>
-      <c r="H21" s="9">
+      <c r="I21" s="9">
         <v>40819</v>
       </c>
-      <c r="I21" s="5">
+      <c r="J21" s="5">
         <v>0.80208333333333304</v>
       </c>
-      <c r="K21" s="12" t="s">
+      <c r="L21" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="L21" s="7" t="s">
+      <c r="M21" s="7" t="s">
         <v>216</v>
-      </c>
-      <c r="N21" t="s">
-        <v>246</v>
       </c>
       <c r="O21" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P21" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2708,35 +2745,35 @@
       <c r="D22" t="b">
         <v>0</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>174</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="G22" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>195</v>
       </c>
-      <c r="H22" s="9">
+      <c r="I22" s="9">
         <v>40820</v>
       </c>
-      <c r="I22" s="5">
+      <c r="J22" s="5">
         <v>0.84375</v>
       </c>
-      <c r="K22" s="12" t="s">
+      <c r="L22" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="L22" s="7" t="s">
+      <c r="M22" s="7" t="s">
         <v>217</v>
-      </c>
-      <c r="N22" t="s">
-        <v>247</v>
       </c>
       <c r="O22" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P22" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2750,41 +2787,41 @@
       <c r="D23" t="b">
         <v>0</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>174</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="G23" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>196</v>
       </c>
-      <c r="H23" s="9">
+      <c r="I23" s="9">
         <v>40821</v>
       </c>
-      <c r="I23" s="5">
+      <c r="J23" s="5">
         <v>0.88541666666666696</v>
       </c>
-      <c r="K23" s="12" t="s">
+      <c r="L23" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="L23" s="7" t="s">
+      <c r="M23" s="7" t="s">
         <v>218</v>
-      </c>
-      <c r="N23" t="s">
-        <v>248</v>
       </c>
       <c r="O23" t="s">
         <v>248</v>
       </c>
+      <c r="P23" t="s">
+        <v>248</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M3" r:id="rId1"/>
-    <hyperlink ref="M4" r:id="rId2"/>
-    <hyperlink ref="M5" r:id="rId3"/>
-    <hyperlink ref="M6" r:id="rId4"/>
-    <hyperlink ref="M8" r:id="rId5"/>
+    <hyperlink ref="N3" r:id="rId1"/>
+    <hyperlink ref="N4" r:id="rId2"/>
+    <hyperlink ref="N5" r:id="rId3"/>
+    <hyperlink ref="N6" r:id="rId4"/>
+    <hyperlink ref="N8" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>

</xml_diff>

<commit_message>
updated event db with youtube video ids for events
</commit_message>
<xml_diff>
--- a/data/EventData.xlsx
+++ b/data/EventData.xlsx
@@ -18,15 +18,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="254">
   <si>
     <t>Movies</t>
   </si>
   <si>
     <t>M-Net Action</t>
-  </si>
-  <si>
-    <t>http://www.youtube.com/watch?v=TkudKzFo7zs&amp;feature=player_embedded</t>
   </si>
   <si>
     <t>JJ McQuade is a Texas Ranger with a reputation for doing things his own way. But after his "lone wolf" ways get too much for his superiors, he is forced to work with Texas State Trooper Kayo Ramos.
@@ -60,14 +57,8 @@
     <t>A Texas Ranger works with a State Trooper to take down a dangerous arms dealer.</t>
   </si>
   <si>
-    <t>http://www.youtube.com/watch?v=k0DA75eOltA&amp;feature=player_embedded</t>
-  </si>
-  <si>
     <t>When Catherine, a successful doctor, begins to question her husband David's fidelity, she sets out to resolve her suspicions with the help of an alluring young woman, Chloe.
 Soon caught in a web of sexual desire, Catherine finds herself on a journey that places her family in great danger.</t>
-  </si>
-  <si>
-    <t>http://www.youtube.com/watch?v=JWLEz-1VzSk&amp;feature=player_embedded</t>
   </si>
   <si>
     <t>Series</t>
@@ -91,9 +82,6 @@
 Want to read the book? Get Game of Thrones, the first volume in the hugely popular and highly acclaimed epic fantasy series, A Song of Ice and Fire.</t>
   </si>
   <si>
-    <t>http://www.youtube.com/watch?v=J7JYw5kQg_Y&amp;feature=player_embedded</t>
-  </si>
-  <si>
     <t>Winter is coming. Let the Game of Thrones begin.</t>
   </si>
   <si>
@@ -116,21 +104,6 @@
 Modern Family won five Emmy Awards for its first season (own it now), including one for Outstanding Comedy Series. It also brought home a Peabody Award, Writers Guild Award, Directors Guilds Award and Television Critics Award. They also collected more gongs at this year's Emmy Awards on Sunday for the second season, including Outstanding Comedy Series, Best Supporting Actress (Julie Bowen) and Best Supporting Actor (Ty Burrell). Not too shabby for a modern family.</t>
   </si>
   <si>
-    <t>http://www.youtube.com/watch?v=GF17_NEqFPk&amp;feature=player_embedded</t>
-  </si>
-  <si>
-    <t>The final word on the Emmys red carpet fashion with E! fashion experts.</t>
-  </si>
-  <si>
-    <t>Fashion Police: 2011 Emmy Awards</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> E! Entertainment Television</t>
-  </si>
-  <si>
-    <t>Special</t>
-  </si>
-  <si>
     <t xml:space="preserve">Episode 1, S3 </t>
   </si>
   <si>
@@ -143,15 +116,6 @@
     <t xml:space="preserve">It's senior year and gang from 90210 return for a third season of more drama.
 In the season three premiere, Beverly Hills is rocked by an earthquake. Naomi has spent the summer dealing with the aftermath of her rape by Mr. Cannon, Annie and Dixon are dealing with the absence of their father while Debbie tries to hold the family together. 
 Teddy and Silver find themselves happier than ever until he suffers an injury that could end his tennis career. Navid welcomes Adrianna back from her summer tour with Javier, but their arrival brings an unexpected death. Ivy and Dixon return from their summer vacation in Australia, while Annie and Liam discover their friendship may be best if it ends. </t>
-  </si>
-  <si>
-    <t>This Wednesday the Fashion Police foursome will be looking at all the hottest trends on the carpet at TV’s biggest night with Fashion Police: The 2011 Emmy Awards. 
-Joan Rivers hosts a special hour of E!’s Fashion Police highlighting the best and worst looks from the previous night’s Emmy awards with Kelly Osbourne, Giuliana Rancic, George Kotsiopoulos and special guest Project Runway and Marie Claire editor Nina Garcia. 
-This special will dissect all your favorite Hollywood stars red carpet looks as they arrive amid a sea of flashbulbs, get honored at the big show and let loose at the after-parties. Joan will “face off” against the fashions from some of the biggest names in television including the casts of Mad Men, The Good Wife, Glee, Modern Family, Boardwalk Empire, 30 Rock, Dexter and more. 
-Find out who got the look right from the fashion police and who missed the mark.</t>
-  </si>
-  <si>
-    <t>http://www.youtube.com/watch?v=rAOMZDXJkDI&amp;feature=player_embedded</t>
   </si>
   <si>
     <t>Sport</t>
@@ -831,6 +795,51 @@
   </si>
   <si>
     <t>category</t>
+  </si>
+  <si>
+    <t>Dexter</t>
+  </si>
+  <si>
+    <t>S06E01</t>
+  </si>
+  <si>
+    <t>Has Dexter finally seen the light? Get ready for the most rapturous season yet.</t>
+  </si>
+  <si>
+    <t>After a relatively hit or miss fifth year installment, the Dexter season 6 premiere serves as a welcome breath of fresh air to the series, by not only fulfilling the lofty promises made by producers that this season would return the hit drama to the familiar thematic form that garnered such critical claim early on, but by also gracefully maturing every element of the program through the masterful handling of an extremely difficult (and often misused) televisual faux pas.</t>
+  </si>
+  <si>
+    <t>RsvGslI_KcM</t>
+  </si>
+  <si>
+    <t>bV3EYzP0HrQ</t>
+  </si>
+  <si>
+    <t>k0DA75eOltA</t>
+  </si>
+  <si>
+    <t>JWLEz-1VzSk</t>
+  </si>
+  <si>
+    <t>8ixEWrTLiZg</t>
+  </si>
+  <si>
+    <t>PyUNRWJg0P8</t>
+  </si>
+  <si>
+    <t>rAOMZDXJkDI</t>
+  </si>
+  <si>
+    <t>Frpk-91vGrc</t>
+  </si>
+  <si>
+    <t>pM1Jg3mYV6E</t>
+  </si>
+  <si>
+    <t>DHFj7kGz6G4</t>
+  </si>
+  <si>
+    <t>D-Bfk9MxqkE</t>
   </si>
 </sst>
 </file>
@@ -1337,22 +1346,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1360,19 +1369,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D2" s="19">
         <v>50</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1381,19 +1390,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="D3" s="19">
         <v>50</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1402,16 +1411,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>55</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>66</v>
       </c>
       <c r="D4" s="23">
         <v>100</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="F4" s="24"/>
     </row>
@@ -1421,19 +1430,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="D5" s="19">
         <v>10</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1442,19 +1451,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="D6" s="19">
         <v>50</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1463,19 +1472,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D7" s="23">
         <v>100</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1484,16 +1493,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D8" s="19">
         <v>0</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="F8" s="22"/>
     </row>
@@ -1503,10 +1512,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="D9" s="19">
         <v>0</v>
@@ -1520,7 +1529,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C10" s="16"/>
       <c r="D10" s="19">
@@ -1535,17 +1544,17 @@
         <v>10</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="D11" s="19">
         <v>0</v>
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="22" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1554,17 +1563,17 @@
         <v>11</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D12" s="19">
         <v>80</v>
       </c>
       <c r="E12" s="19"/>
       <c r="F12" s="22" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1573,17 +1582,17 @@
         <v>12</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D13" s="19">
         <v>80</v>
       </c>
       <c r="E13" s="19"/>
       <c r="F13" s="22" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1592,10 +1601,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D14" s="19">
         <v>80</v>
@@ -1609,16 +1618,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="D15" s="19">
         <v>0</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="F15" s="22"/>
     </row>
@@ -1628,17 +1637,17 @@
         <v>15</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="19">
         <v>0</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1647,19 +1656,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="D17" s="23">
         <v>100</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="F17" s="24" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1668,19 +1677,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D18" s="19">
         <v>80</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="F18" s="22" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1689,13 +1698,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1704,19 +1713,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D20" s="28">
         <v>100</v>
       </c>
       <c r="E20" s="28" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="F20" s="29" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1747,8 +1756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="L12" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1771,61 +1780,61 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="C1" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="D1" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="E1" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="I1" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>80</v>
-      </c>
       <c r="J1" s="3" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="M1" s="14" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="O1" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="P1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="Q1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="R1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="S1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="124.5" x14ac:dyDescent="0.25">
@@ -1848,7 +1857,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="H2" t="s">
         <v>1</v>
@@ -1860,19 +1869,19 @@
         <v>0.85416666666666663</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N2" t="s">
-        <v>2</v>
+        <v>244</v>
       </c>
       <c r="O2" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="P2" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="90.75" x14ac:dyDescent="0.25">
@@ -1896,10 +1905,10 @@
         <v>0</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I3" s="9">
         <v>40811</v>
@@ -1908,19 +1917,19 @@
         <v>0.85763888888888884</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>12</v>
+        <v>245</v>
       </c>
       <c r="O3" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="P3" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="57" x14ac:dyDescent="0.25">
@@ -1944,10 +1953,10 @@
         <v>0</v>
       </c>
       <c r="G4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" t="s">
         <v>9</v>
-      </c>
-      <c r="H4" t="s">
-        <v>10</v>
       </c>
       <c r="I4" s="9">
         <v>40812</v>
@@ -1957,19 +1966,19 @@
       </c>
       <c r="K4" s="4"/>
       <c r="L4" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>14</v>
+        <v>246</v>
       </c>
       <c r="O4" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="P4" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="248.25" x14ac:dyDescent="0.25">
@@ -1987,16 +1996,16 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
         <v>15</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" t="s">
-        <v>18</v>
       </c>
       <c r="I5" s="9">
         <v>40812</v>
@@ -2005,22 +2014,22 @@
         <v>0.89583333333333337</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>20</v>
+        <v>247</v>
       </c>
       <c r="O5" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="P5" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="203.25" x14ac:dyDescent="0.25">
@@ -2038,16 +2047,16 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" t="s">
         <v>15</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" t="s">
-        <v>18</v>
       </c>
       <c r="I6" s="9">
         <v>40807</v>
@@ -2056,25 +2065,25 @@
         <v>0.8125</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>27</v>
+        <v>248</v>
       </c>
       <c r="O6" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="P6" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="158.25" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="68.25" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2089,16 +2098,16 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>29</v>
+        <v>239</v>
       </c>
       <c r="H7" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="I7" s="9">
         <v>40807</v>
@@ -2107,19 +2116,22 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>28</v>
+        <v>240</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>241</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>36</v>
+        <v>242</v>
+      </c>
+      <c r="N7" t="s">
+        <v>243</v>
       </c>
       <c r="O7" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="P7" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="113.25" x14ac:dyDescent="0.25">
@@ -2137,16 +2149,16 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="H8" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="I8" s="9">
         <v>40807</v>
@@ -2155,22 +2167,22 @@
         <v>0.85416666666666663</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="L8" s="12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>37</v>
+        <v>249</v>
       </c>
       <c r="O8" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="P8" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="409.6" x14ac:dyDescent="0.25">
@@ -2188,16 +2200,16 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="H9" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="I9" s="9">
         <v>40808</v>
@@ -2206,16 +2218,19 @@
         <v>0.375</v>
       </c>
       <c r="L9" s="12" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>41</v>
+        <v>30</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>250</v>
       </c>
       <c r="O9" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="P9" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="409.6" x14ac:dyDescent="0.25">
@@ -2233,16 +2248,16 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="H10" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="I10" s="9">
         <v>40807</v>
@@ -2251,16 +2266,19 @@
         <v>0.85416666666666663</v>
       </c>
       <c r="L10" s="12" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>45</v>
+        <v>34</v>
+      </c>
+      <c r="N10" t="s">
+        <v>251</v>
       </c>
       <c r="O10" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="P10" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="225.75" x14ac:dyDescent="0.25">
@@ -2278,16 +2296,16 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" t="s">
         <v>38</v>
-      </c>
-      <c r="F11" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H11" t="s">
-        <v>49</v>
       </c>
       <c r="I11" s="9">
         <v>40809</v>
@@ -2296,16 +2314,19 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="L11" s="12" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>50</v>
+        <v>39</v>
+      </c>
+      <c r="N11" t="s">
+        <v>252</v>
       </c>
       <c r="O11" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="P11" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="315.75" x14ac:dyDescent="0.25">
@@ -2323,16 +2344,16 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H12" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="I12" s="9">
         <v>40810</v>
@@ -2341,16 +2362,19 @@
         <v>0.42708333333333331</v>
       </c>
       <c r="L12" s="12" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>52</v>
+        <v>41</v>
+      </c>
+      <c r="N12" t="s">
+        <v>253</v>
       </c>
       <c r="O12" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="P12" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -2368,13 +2392,13 @@
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="G13" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="H13" t="s">
         <v>175</v>
-      </c>
-      <c r="H13" t="s">
-        <v>186</v>
       </c>
       <c r="I13" s="9">
         <v>40811</v>
@@ -2383,16 +2407,16 @@
         <v>0.46875</v>
       </c>
       <c r="L13" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="M13" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="M13" s="7" t="s">
-        <v>208</v>
-      </c>
       <c r="O13" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="P13" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -2410,13 +2434,13 @@
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="G14" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="H14" t="s">
         <v>176</v>
-      </c>
-      <c r="H14" t="s">
-        <v>187</v>
       </c>
       <c r="I14" s="9">
         <v>40812</v>
@@ -2425,16 +2449,16 @@
         <v>0.51041666666666696</v>
       </c>
       <c r="L14" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="M14" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="M14" s="7" t="s">
-        <v>209</v>
-      </c>
       <c r="O14" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="P14" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -2452,13 +2476,13 @@
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="G15" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="H15" t="s">
         <v>177</v>
-      </c>
-      <c r="H15" t="s">
-        <v>188</v>
       </c>
       <c r="I15" s="9">
         <v>40813</v>
@@ -2467,16 +2491,16 @@
         <v>0.55208333333333304</v>
       </c>
       <c r="L15" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="M15" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="M15" s="7" t="s">
-        <v>210</v>
-      </c>
       <c r="O15" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="P15" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -2494,13 +2518,13 @@
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="G16" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="H16" t="s">
         <v>178</v>
-      </c>
-      <c r="H16" t="s">
-        <v>189</v>
       </c>
       <c r="I16" s="9">
         <v>40814</v>
@@ -2509,16 +2533,16 @@
         <v>0.59375</v>
       </c>
       <c r="L16" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="M16" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="M16" s="7" t="s">
-        <v>211</v>
-      </c>
       <c r="O16" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="P16" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -2536,13 +2560,13 @@
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="G17" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="H17" t="s">
         <v>179</v>
-      </c>
-      <c r="H17" t="s">
-        <v>190</v>
       </c>
       <c r="I17" s="9">
         <v>40815</v>
@@ -2551,16 +2575,16 @@
         <v>0.63541666666666696</v>
       </c>
       <c r="L17" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="M17" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="M17" s="7" t="s">
-        <v>212</v>
-      </c>
       <c r="O17" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="P17" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -2578,13 +2602,13 @@
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="G18" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="H18" t="s">
         <v>180</v>
-      </c>
-      <c r="H18" t="s">
-        <v>191</v>
       </c>
       <c r="I18" s="9">
         <v>40816</v>
@@ -2593,16 +2617,16 @@
         <v>0.67708333333333304</v>
       </c>
       <c r="L18" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="M18" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="M18" s="7" t="s">
-        <v>213</v>
-      </c>
       <c r="O18" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="P18" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -2620,13 +2644,13 @@
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="G19" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="H19" t="s">
         <v>181</v>
-      </c>
-      <c r="H19" t="s">
-        <v>192</v>
       </c>
       <c r="I19" s="9">
         <v>40817</v>
@@ -2635,16 +2659,16 @@
         <v>0.71875</v>
       </c>
       <c r="L19" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="M19" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="M19" s="7" t="s">
-        <v>214</v>
-      </c>
       <c r="O19" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="P19" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -2662,13 +2686,13 @@
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="G20" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="H20" t="s">
         <v>182</v>
-      </c>
-      <c r="H20" t="s">
-        <v>193</v>
       </c>
       <c r="I20" s="9">
         <v>40818</v>
@@ -2677,16 +2701,16 @@
         <v>0.76041666666666696</v>
       </c>
       <c r="L20" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="M20" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="M20" s="7" t="s">
-        <v>215</v>
-      </c>
       <c r="O20" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="P20" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -2704,13 +2728,13 @@
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="G21" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="H21" t="s">
         <v>183</v>
-      </c>
-      <c r="H21" t="s">
-        <v>194</v>
       </c>
       <c r="I21" s="9">
         <v>40819</v>
@@ -2719,16 +2743,16 @@
         <v>0.80208333333333304</v>
       </c>
       <c r="L21" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="M21" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="M21" s="7" t="s">
-        <v>216</v>
-      </c>
       <c r="O21" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="P21" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -2746,13 +2770,13 @@
         <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="G22" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="H22" t="s">
         <v>184</v>
-      </c>
-      <c r="H22" t="s">
-        <v>195</v>
       </c>
       <c r="I22" s="9">
         <v>40820</v>
@@ -2761,16 +2785,16 @@
         <v>0.84375</v>
       </c>
       <c r="L22" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="M22" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="M22" s="7" t="s">
-        <v>217</v>
-      </c>
       <c r="O22" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="P22" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -2788,13 +2812,13 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
+        <v>163</v>
+      </c>
+      <c r="G23" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="H23" t="s">
         <v>185</v>
-      </c>
-      <c r="H23" t="s">
-        <v>196</v>
       </c>
       <c r="I23" s="9">
         <v>40821</v>
@@ -2803,28 +2827,21 @@
         <v>0.88541666666666696</v>
       </c>
       <c r="L23" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="M23" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="M23" s="7" t="s">
-        <v>218</v>
-      </c>
       <c r="O23" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="P23" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="N3" r:id="rId1"/>
-    <hyperlink ref="N4" r:id="rId2"/>
-    <hyperlink ref="N5" r:id="rId3"/>
-    <hyperlink ref="N6" r:id="rId4"/>
-    <hyperlink ref="N8" r:id="rId5"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2845,37 +2862,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="C1" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="D1" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="E1" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="F1" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="G1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="H1" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="I1" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="J1" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="K1" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -3219,37 +3236,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="C1" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="D1" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="E1" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="F1" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="G1" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="H1" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="I1" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="J1" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="K1" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -3412,25 +3429,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="C1" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="D1" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="E1" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="F1" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="G1" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3438,16 +3455,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D2">
         <v>150</v>
       </c>
       <c r="F2" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3456,16 +3473,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D3">
         <v>150</v>
       </c>
       <c r="F3" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -3474,16 +3491,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="C4" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="D4">
         <v>150</v>
       </c>
       <c r="F4" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -3492,16 +3509,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="C5" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="D5">
         <v>150</v>
       </c>
       <c r="F5" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -3510,16 +3527,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="C6" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="D6">
         <v>150</v>
       </c>
       <c r="F6" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -3528,16 +3545,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="C7" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="D7">
         <v>129</v>
       </c>
       <c r="F7" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -3546,16 +3563,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="C8" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="D8">
         <v>129</v>
       </c>
       <c r="F8" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -3564,16 +3581,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="C9" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="D9">
         <v>129</v>
       </c>
       <c r="F9" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -3582,16 +3599,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="C10" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="D10">
         <v>129</v>
       </c>
       <c r="F10" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -3600,16 +3617,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="C11" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="D11">
         <v>129</v>
       </c>
       <c r="F11" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -3618,16 +3635,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="C12" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="D12">
         <v>99</v>
       </c>
       <c r="F12" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -3636,16 +3653,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="C13" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="D13">
         <v>99</v>
       </c>
       <c r="F13" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -3654,16 +3671,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="C14" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="D14">
         <v>99</v>
       </c>
       <c r="F14" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -3672,16 +3689,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="C15" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="D15">
         <v>99</v>
       </c>
       <c r="F15" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -3690,16 +3707,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="C16" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="D16">
         <v>99</v>
       </c>
       <c r="F16" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -3708,16 +3725,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="C17" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="D17">
         <v>99</v>
       </c>
       <c r="F17" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -3726,16 +3743,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="C18" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="D18">
         <v>99</v>
       </c>
       <c r="F18" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -3744,16 +3761,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="C19" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="D19">
         <v>99</v>
       </c>
       <c r="F19" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -3762,16 +3779,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="C20" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="D20">
         <v>99</v>
       </c>
       <c r="F20" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -3780,16 +3797,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="C21" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="D21">
         <v>99</v>
       </c>
       <c r="F21" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -3798,16 +3815,16 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C22" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="D22">
         <v>25</v>
       </c>
       <c r="F22" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -3816,16 +3833,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C23" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="D23">
         <v>25</v>
       </c>
       <c r="F23" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -3834,16 +3851,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C24" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="D24">
         <v>25</v>
       </c>
       <c r="F24" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -3852,16 +3869,16 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C25" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="D25">
         <v>25</v>
       </c>
       <c r="F25" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -3870,16 +3887,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C26" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="D26">
         <v>25</v>
       </c>
       <c r="F26" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -3888,16 +3905,16 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C27" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="D27">
         <v>25</v>
       </c>
       <c r="F27" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -3906,16 +3923,16 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C28" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="D28">
         <v>25</v>
       </c>
       <c r="F28" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -3924,16 +3941,16 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C29" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="D29">
         <v>25</v>
       </c>
       <c r="F29" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -3942,16 +3959,16 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C30" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="D30">
         <v>25</v>
       </c>
       <c r="F30" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -3960,16 +3977,16 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C31" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="D31">
         <v>25</v>
       </c>
       <c r="F31" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the db with new images and banners for movies
</commit_message>
<xml_diff>
--- a/data/EventData.xlsx
+++ b/data/EventData.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="WBS" sheetId="2" r:id="rId1"/>
-    <sheet name="Events" sheetId="1" r:id="rId2"/>
+    <sheet name="EventData" sheetId="1" r:id="rId2"/>
     <sheet name="ViewRecommendations" sheetId="3" r:id="rId3"/>
     <sheet name="BuyRecommendations" sheetId="4" r:id="rId4"/>
     <sheet name="BuyData" sheetId="5" r:id="rId5"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="368">
   <si>
     <t>Movies</t>
   </si>
@@ -27,24 +27,6 @@
   </si>
   <si>
     <t>SONY</t>
-  </si>
-  <si>
-    <t>A fast-talking lawyer finds himself unable to tell a lie for 24 hours.</t>
-  </si>
-  <si>
-    <t>Liar Liar</t>
-  </si>
-  <si>
-    <t>A woman hires an escort in order to test her husband's fidelity.</t>
-  </si>
-  <si>
-    <t>Chloe</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 13 eme Rue</t>
-  </si>
-  <si>
-    <t>A Texas Ranger works with a State Trooper to take down a dangerous arms dealer.</t>
   </si>
   <si>
     <t>Series</t>
@@ -141,9 +123,6 @@
     <t>Fragment for launching our activities</t>
   </si>
   <si>
-    <t>carousel widget - Integrate</t>
-  </si>
-  <si>
     <t>Actvitity  "Kalahari" mockup</t>
   </si>
   <si>
@@ -240,12 +219,6 @@
     <t>On Hold</t>
   </si>
   <si>
-    <t>Can launch the YouTube app to play videos using intent. Todo: Try to get embedded player.</t>
-  </si>
-  <si>
-    <t>Satya</t>
-  </si>
-  <si>
     <t>Shaik</t>
   </si>
   <si>
@@ -267,9 +240,6 @@
     <t xml:space="preserve">Fragment Buy </t>
   </si>
   <si>
-    <t>KondaReddy</t>
-  </si>
-  <si>
     <t>Shaik to try implementing a webview to take you directly to box office site</t>
   </si>
   <si>
@@ -585,12 +555,6 @@
     <t>Vaugan/Satya</t>
   </si>
   <si>
-    <t>ddaily093.jpg</t>
-  </si>
-  <si>
-    <t>Lone Wolf McQuade</t>
-  </si>
-  <si>
     <t>ddaily094.jpg</t>
   </si>
   <si>
@@ -612,12 +576,6 @@
     <t>ddaily100.jpg</t>
   </si>
   <si>
-    <t>ddaily092.jpg</t>
-  </si>
-  <si>
-    <t>ddaily091.jpg</t>
-  </si>
-  <si>
     <t>ddaily101.jpg</t>
   </si>
   <si>
@@ -664,15 +622,6 @@
   </si>
   <si>
     <t>RsvGslI_KcM</t>
-  </si>
-  <si>
-    <t>bV3EYzP0HrQ</t>
-  </si>
-  <si>
-    <t>k0DA75eOltA</t>
-  </si>
-  <si>
-    <t>JWLEz-1VzSk</t>
   </si>
   <si>
     <t>8ixEWrTLiZg</t>
@@ -975,25 +924,208 @@
     <t>Lifestyle10.jpg</t>
   </si>
   <si>
-    <t>Kill Bill 2</t>
-  </si>
-  <si>
-    <t>Thor</t>
-  </si>
-  <si>
-    <t>The Matrix</t>
-  </si>
-  <si>
-    <t>Tombstone</t>
-  </si>
-  <si>
-    <t>Black Swan</t>
-  </si>
-  <si>
-    <t>Transformers 2</t>
-  </si>
-  <si>
-    <t>Iron Man 2</t>
+    <t>Can launch the YouTube app to play videos using intent.</t>
+  </si>
+  <si>
+    <t>CoverFlow widget - Integrate</t>
+  </si>
+  <si>
+    <t>Todo: Put proper links to actual products in buy rec db.</t>
+  </si>
+  <si>
+    <t>Started</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Real Steel </t>
+  </si>
+  <si>
+    <t>Shawn Levy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hugh Jackman, Evangeline Lilly and Dakota Goyo</t>
+  </si>
+  <si>
+    <t>Set in the near future, where robot boxing is a top sport, a struggling promoter feels he's found a champion in a discarded robot. During his hopeful rise to the top, he discovers he has an 11-year-old son who wants to know his father.</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>movie_poster01.jpg</t>
+  </si>
+  <si>
+    <t>ei5l3r1dV4I</t>
+  </si>
+  <si>
+    <t>The Thing</t>
+  </si>
+  <si>
+    <t>movie_poster02.jpg</t>
+  </si>
+  <si>
+    <t>At an Antarctica research site, the discovery of an alien craft leads to a confrontation between graduate student Kate Lloyd and scientist Dr. Sander Halvorson.</t>
+  </si>
+  <si>
+    <t>Matthijs van Heijningen Jr.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mary Elizabeth Winstead, Joel Edgerton and Ulrich Thomsen</t>
+  </si>
+  <si>
+    <t>ouZkkIsLiNg</t>
+  </si>
+  <si>
+    <t>MM2</t>
+  </si>
+  <si>
+    <t>The Ides of March</t>
+  </si>
+  <si>
+    <t>MM1</t>
+  </si>
+  <si>
+    <t>An idealistic staffer for a newbie presidential candidate gets a crash course on dirty politics during his stint on the campaign trail. Based on the play by Beau Willimon.</t>
+  </si>
+  <si>
+    <t>BMFPh_ZrrjE</t>
+  </si>
+  <si>
+    <t>movie_poster03.jpg</t>
+  </si>
+  <si>
+    <t>George Clooney</t>
+  </si>
+  <si>
+    <t>Paul Giamatti, George Clooney and Philip Seymour Hoffman</t>
+  </si>
+  <si>
+    <t>What's Your Number?</t>
+  </si>
+  <si>
+    <t>M-Net</t>
+  </si>
+  <si>
+    <t>A woman looks back at the past twenty men she's had relationships with in her life and wonders if one of them might be her one true love.</t>
+  </si>
+  <si>
+    <t>8NSM0YCDr1o</t>
+  </si>
+  <si>
+    <t>movie_poster04.jpg</t>
+  </si>
+  <si>
+    <t>Mark Mylod</t>
+  </si>
+  <si>
+    <t>Anna Faris, Chris Evans and Ari Graynor</t>
+  </si>
+  <si>
+    <t>Johnny English Reborn</t>
+  </si>
+  <si>
+    <t>Johnny English goes up against international assassins hunting down the Chinese premier.</t>
+  </si>
+  <si>
+    <t>_883cRmOZXs</t>
+  </si>
+  <si>
+    <t>movie_poster05.jpg</t>
+  </si>
+  <si>
+    <t>Oliver Parker</t>
+  </si>
+  <si>
+    <t>Rowan Atkinson, Rosamund Pike and Dominic West</t>
+  </si>
+  <si>
+    <t>The Rum Diary</t>
+  </si>
+  <si>
+    <t>American journalist Paul Kemp takes on a freelance job in Puerto Rico for a local newspaper during the 1950s and struggles to find a balance between island culture and the ex-patriots who live there.</t>
+  </si>
+  <si>
+    <t>am80hxPrnPE</t>
+  </si>
+  <si>
+    <t>movie_poster06.jpg</t>
+  </si>
+  <si>
+    <t>Johnny Depp, Giovanni Ribisi and Aaron Eckhart</t>
+  </si>
+  <si>
+    <t>Bruce Robinson</t>
+  </si>
+  <si>
+    <t>Jack and Jill</t>
+  </si>
+  <si>
+    <t>A family man is forced to deal with his twin sister from the Bronx comes to Los Angeles for a visit -- then won't leave.</t>
+  </si>
+  <si>
+    <t>xeRrw32Fn94</t>
+  </si>
+  <si>
+    <t>movie_poster07.jpg</t>
+  </si>
+  <si>
+    <t>Dennis Dugan</t>
+  </si>
+  <si>
+    <t>Adam Sandler, Katie Holmes and Al Pacino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carnage </t>
+  </si>
+  <si>
+    <t>Tells the story of two sets of parents who decide to have a cordial meeting after their sons are involved in a schoolyard brawl.</t>
+  </si>
+  <si>
+    <t>YFeo_JtCYx0</t>
+  </si>
+  <si>
+    <t>movie_poster08.jpg</t>
+  </si>
+  <si>
+    <t>Roman Polanski</t>
+  </si>
+  <si>
+    <t>Jodie Foster, Kate Winslet and Christoph Waltz</t>
+  </si>
+  <si>
+    <t>Alvin and the Chipmunks: Chip-Wrecked</t>
+  </si>
+  <si>
+    <t>Playing around while aboard a cruise ship, the Chipmunks and Chipettes accidentally go overboard and end up marooned in a tropical paradise. They discover their new turf is not as deserted as it seems.</t>
+  </si>
+  <si>
+    <t>kKJ7kDLd2o8</t>
+  </si>
+  <si>
+    <t>movie_poster09.jpg</t>
+  </si>
+  <si>
+    <t>Mike Mitchell</t>
+  </si>
+  <si>
+    <t>Justin Long, Matthew Gray Gubler and Jesse McCartney</t>
+  </si>
+  <si>
+    <t>Father of Invention</t>
+  </si>
+  <si>
+    <t>Robert Axel, an eccentric inventor who through wealth and fame, finds unexpected misfortune and after many hardships is ready to redeem his name and rebuild his billion dollar empire.</t>
+  </si>
+  <si>
+    <t>znE5tTpHTM4</t>
+  </si>
+  <si>
+    <t>movie_poster10.jpg</t>
+  </si>
+  <si>
+    <t>2010Trent Cooper</t>
+  </si>
+  <si>
+    <t>Kevin Spacey, Camilla Belle and Heather Graham</t>
   </si>
 </sst>
 </file>
@@ -1485,7 +1617,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1500,22 +1632,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1523,19 +1655,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D2" s="19">
         <v>50</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1544,19 +1676,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="D3" s="19">
         <v>50</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1565,38 +1697,38 @@
         <v>3</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D4" s="23">
         <v>100</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="F4" s="24"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="19">
+      <c r="A5" s="23">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="D5" s="19">
-        <v>10</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="F5" s="22" t="s">
-        <v>73</v>
+      <c r="B5" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="23">
+        <v>100</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1605,19 +1737,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>40</v>
+        <v>301</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D6" s="19">
         <v>50</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1626,19 +1758,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D7" s="23">
         <v>100</v>
       </c>
       <c r="E7" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="24" t="s">
         <v>68</v>
-      </c>
-      <c r="F7" s="24" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1647,16 +1779,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D8" s="19">
         <v>0</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="F8" s="22"/>
     </row>
@@ -1666,16 +1798,18 @@
         <v>8</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D9" s="19">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E9" s="19"/>
-      <c r="F9" s="22"/>
+      <c r="F9" s="22" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
@@ -1683,11 +1817,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="16"/>
+        <v>30</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>66</v>
+      </c>
       <c r="D10" s="19">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E10" s="19"/>
       <c r="F10" s="22"/>
@@ -1698,17 +1834,17 @@
         <v>10</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D11" s="19">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="22" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1717,17 +1853,17 @@
         <v>11</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D12" s="19">
         <v>80</v>
       </c>
       <c r="E12" s="19"/>
       <c r="F12" s="22" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1736,17 +1872,17 @@
         <v>12</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D13" s="19">
         <v>80</v>
       </c>
       <c r="E13" s="19"/>
       <c r="F13" s="22" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1755,10 +1891,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D14" s="19">
         <v>80</v>
@@ -1772,16 +1908,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="D15" s="19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>84</v>
+        <v>303</v>
       </c>
       <c r="F15" s="22"/>
     </row>
@@ -1791,17 +1927,17 @@
         <v>15</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="19">
         <v>0</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1810,19 +1946,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D17" s="23">
         <v>100</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="F17" s="24" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1831,19 +1967,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D18" s="19">
         <v>80</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="F18" s="22" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1852,13 +1988,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1867,19 +2003,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D20" s="28">
         <v>100</v>
       </c>
       <c r="E20" s="28" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="F20" s="29" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1908,10 +2044,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S61"/>
+  <dimension ref="A1:T61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D49" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" topLeftCell="D34" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1930,71 +2066,75 @@
     <col min="12" max="12" width="15.85546875" style="12" customWidth="1"/>
     <col min="13" max="13" width="7.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="47.28515625" customWidth="1"/>
-    <col min="19" max="19" width="15.5703125" customWidth="1"/>
+    <col min="18" max="18" width="13.28515625" customWidth="1"/>
+    <col min="20" max="20" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="E1" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q1" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="R1" t="s">
+        <v>308</v>
+      </c>
+      <c r="S1" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="L1" s="11" t="s">
+      <c r="T1" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="O1" t="s">
-        <v>49</v>
-      </c>
-      <c r="P1" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>51</v>
-      </c>
-      <c r="R1" t="s">
-        <v>52</v>
-      </c>
-      <c r="S1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" ht="60.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:20" ht="180.75" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2014,7 +2154,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>189</v>
+        <v>304</v>
       </c>
       <c r="H2" t="s">
         <v>1</v>
@@ -2026,19 +2166,28 @@
         <v>0.85416666666666663</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>8</v>
+        <v>307</v>
       </c>
       <c r="N2" t="s">
-        <v>215</v>
+        <v>310</v>
       </c>
       <c r="O2" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="P2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="60.75" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>306</v>
+      </c>
+      <c r="S2" t="s">
+        <v>305</v>
+      </c>
+      <c r="T2">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="108.75" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -2059,10 +2208,10 @@
         <v>0</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>4</v>
+        <v>311</v>
       </c>
       <c r="H3" t="s">
-        <v>2</v>
+        <v>317</v>
       </c>
       <c r="I3" s="9">
         <v>40834</v>
@@ -2071,21 +2220,30 @@
         <v>0.89583333333333337</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>3</v>
+        <v>313</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>216</v>
+        <v>316</v>
       </c>
       <c r="O3" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
       <c r="P3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="48.75" x14ac:dyDescent="0.25">
+        <v>312</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>315</v>
+      </c>
+      <c r="S3" t="s">
+        <v>314</v>
+      </c>
+      <c r="T3">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="132.75" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A61" si="0">A3+1</f>
+        <f>A3+1</f>
         <v>3</v>
       </c>
       <c r="B4">
@@ -2104,10 +2262,10 @@
         <v>0</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>6</v>
+        <v>318</v>
       </c>
       <c r="H4" t="s">
-        <v>7</v>
+        <v>319</v>
       </c>
       <c r="I4" s="9">
         <v>40834</v>
@@ -2117,21 +2275,31 @@
       </c>
       <c r="K4" s="4"/>
       <c r="L4" s="12" t="s">
-        <v>5</v>
+        <v>320</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>217</v>
+        <v>321</v>
       </c>
       <c r="O4" t="s">
-        <v>265</v>
+        <v>248</v>
       </c>
       <c r="P4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="60.75" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>324</v>
+      </c>
+      <c r="S4" t="s">
+        <v>323</v>
+      </c>
+      <c r="T4">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="108.75" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <f>A4+1</f>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2149,10 +2317,10 @@
         <v>0</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="H5" t="s">
-        <v>1</v>
+        <v>326</v>
       </c>
       <c r="I5" s="9">
         <v>40834</v>
@@ -2161,22 +2329,31 @@
         <v>0.97916666666666696</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>8</v>
+        <v>327</v>
       </c>
       <c r="N5" t="s">
-        <v>215</v>
+        <v>328</v>
       </c>
       <c r="O5" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="P5" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="60.75" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>331</v>
+      </c>
+      <c r="S5" t="s">
+        <v>330</v>
+      </c>
+      <c r="T5">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>A5+1</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -2194,10 +2371,10 @@
         <v>0</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>318</v>
+        <v>332</v>
       </c>
       <c r="H6" t="s">
-        <v>2</v>
+        <v>317</v>
       </c>
       <c r="I6" s="9">
         <v>40834</v>
@@ -2206,22 +2383,31 @@
         <v>1.0208333333333299</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>3</v>
+        <v>333</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>216</v>
+        <v>334</v>
       </c>
       <c r="O6" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="P6" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="48.75" x14ac:dyDescent="0.25">
+        <v>335</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>337</v>
+      </c>
+      <c r="S6" t="s">
+        <v>336</v>
+      </c>
+      <c r="T6">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="156.75" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f t="shared" ref="A7:A61" si="0">A6+1</f>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -2239,10 +2425,10 @@
         <v>0</v>
       </c>
       <c r="G7" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="H7" t="s">
         <v>319</v>
-      </c>
-      <c r="H7" t="s">
-        <v>7</v>
       </c>
       <c r="I7" s="9">
         <v>40834</v>
@@ -2252,21 +2438,31 @@
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="12" t="s">
-        <v>5</v>
+        <v>339</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>217</v>
+        <v>340</v>
       </c>
       <c r="O7" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="P7" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="60.75" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>342</v>
+      </c>
+      <c r="S7" t="s">
+        <v>343</v>
+      </c>
+      <c r="T7">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="84.75" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2284,10 +2480,10 @@
         <v>0</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>320</v>
+        <v>344</v>
       </c>
       <c r="H8" t="s">
-        <v>1</v>
+        <v>317</v>
       </c>
       <c r="I8" s="9">
         <v>40834</v>
@@ -2296,22 +2492,31 @@
         <v>1.1041666666666701</v>
       </c>
       <c r="L8" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="N8" t="s">
+        <v>346</v>
+      </c>
+      <c r="O8" t="s">
+        <v>252</v>
+      </c>
+      <c r="P8" t="s">
+        <v>347</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>349</v>
+      </c>
+      <c r="S8" t="s">
+        <v>348</v>
+      </c>
+      <c r="T8">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="96.75" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
         <v>8</v>
-      </c>
-      <c r="N8" t="s">
-        <v>215</v>
-      </c>
-      <c r="O8" t="s">
-        <v>269</v>
-      </c>
-      <c r="P8" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="60.75" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f>A8+1</f>
-        <v>2</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -2329,7 +2534,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>321</v>
+        <v>350</v>
       </c>
       <c r="H9" t="s">
         <v>2</v>
@@ -2341,22 +2546,31 @@
         <v>1.1458333333333299</v>
       </c>
       <c r="L9" s="12" t="s">
-        <v>3</v>
+        <v>351</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>216</v>
+        <v>352</v>
       </c>
       <c r="O9" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
       <c r="P9" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="48.75" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>355</v>
+      </c>
+      <c r="S9" t="s">
+        <v>354</v>
+      </c>
+      <c r="T9">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="156.75" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -2374,10 +2588,10 @@
         <v>0</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>322</v>
+        <v>356</v>
       </c>
       <c r="H10" t="s">
-        <v>7</v>
+        <v>319</v>
       </c>
       <c r="I10" s="9">
         <v>40834</v>
@@ -2387,21 +2601,31 @@
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="12" t="s">
-        <v>5</v>
+        <v>357</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>217</v>
+        <v>358</v>
       </c>
       <c r="O10" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="P10" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="60.75" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>361</v>
+      </c>
+      <c r="S10" t="s">
+        <v>360</v>
+      </c>
+      <c r="T10">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="144.75" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -2419,7 +2643,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>323</v>
+        <v>362</v>
       </c>
       <c r="H11" t="s">
         <v>1</v>
@@ -2431,22 +2655,28 @@
         <v>1.2291666666666701</v>
       </c>
       <c r="L11" s="12" t="s">
-        <v>8</v>
+        <v>363</v>
       </c>
       <c r="N11" t="s">
-        <v>215</v>
+        <v>364</v>
       </c>
       <c r="O11" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
       <c r="P11" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" ht="36.75" x14ac:dyDescent="0.25">
+        <v>365</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>367</v>
+      </c>
+      <c r="S11" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f>A4+1</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>4</v>
@@ -2458,16 +2688,16 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F12" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="H12" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="I12" s="9">
         <v>40834</v>
@@ -2476,25 +2706,25 @@
         <v>1.2708333333333299</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L12" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="O12" t="s">
+        <v>209</v>
+      </c>
+      <c r="P12" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="60.75" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
         <v>12</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="O12" t="s">
-        <v>226</v>
-      </c>
-      <c r="P12" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" ht="60.75" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f t="shared" si="0"/>
-        <v>5</v>
       </c>
       <c r="B13">
         <v>5</v>
@@ -2506,16 +2736,16 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F13" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
       <c r="H13" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="I13" s="9">
         <v>40834</v>
@@ -2524,25 +2754,25 @@
         <v>1.3125</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="L13" s="12" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
       <c r="O13" t="s">
-        <v>244</v>
+        <v>227</v>
       </c>
       <c r="P13" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" ht="60.75" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>6</v>
@@ -2554,16 +2784,16 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F14" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="H14" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I14" s="9">
         <v>40834</v>
@@ -2572,25 +2802,25 @@
         <v>1.3541666666666701</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="L14" s="12" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="N14" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="O14" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="P14" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="60.75" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>7</v>
@@ -2602,16 +2832,16 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F15" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="H15" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="I15" s="9">
         <v>40834</v>
@@ -2620,25 +2850,25 @@
         <v>1.3958333333333299</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="L15" s="12" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="O15" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
       <c r="P15" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="36.75" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -2650,16 +2880,16 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="H16" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="I16" s="9">
         <v>40834</v>
@@ -2668,25 +2898,25 @@
         <v>1.4375</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L16" s="12" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="O16" t="s">
-        <v>247</v>
+        <v>230</v>
       </c>
       <c r="P16" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>5</v>
@@ -2698,16 +2928,16 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F17" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="H17" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="I17" s="9">
         <v>40834</v>
@@ -2716,25 +2946,25 @@
         <v>1.4791666666666701</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="L17" s="12" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
       <c r="O17" t="s">
-        <v>248</v>
+        <v>231</v>
       </c>
       <c r="P17" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>6</v>
@@ -2746,16 +2976,16 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="H18" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I18" s="9">
         <v>40834</v>
@@ -2764,25 +2994,25 @@
         <v>1.5208333333333299</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="L18" s="12" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="N18" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="O18" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="P18" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>7</v>
@@ -2794,16 +3024,16 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F19" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
       <c r="H19" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="I19" s="9">
         <v>40834</v>
@@ -2812,25 +3042,25 @@
         <v>1.5625</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="L19" s="12" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="O19" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="P19" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>6</v>
@@ -2842,16 +3072,16 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F20" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="H20" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I20" s="9">
         <v>40834</v>
@@ -2860,25 +3090,25 @@
         <v>1.6041666666666701</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="L20" s="12" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="N20" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="O20" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
       <c r="P20" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B21">
         <v>7</v>
@@ -2890,16 +3120,16 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F21" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
       <c r="H21" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="I21" s="9">
         <v>40834</v>
@@ -2908,25 +3138,25 @@
         <v>1.6458333333333299</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L21" s="12" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="O21" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="P21" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f>A15+1</f>
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>21</v>
       </c>
       <c r="B22">
         <v>8</v>
@@ -2938,16 +3168,16 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F22" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H22" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="I22" s="9">
         <v>40834</v>
@@ -2956,22 +3186,22 @@
         <v>1.6875</v>
       </c>
       <c r="L22" s="12" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>221</v>
+        <v>204</v>
       </c>
       <c r="O22" t="s">
-        <v>253</v>
+        <v>236</v>
       </c>
       <c r="P22" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B23">
         <v>9</v>
@@ -2983,16 +3213,16 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F23" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="H23" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I23" s="9">
         <v>40834</v>
@@ -3001,22 +3231,22 @@
         <v>1.7291666666666701</v>
       </c>
       <c r="L23" s="12" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="N23" t="s">
-        <v>222</v>
+        <v>205</v>
       </c>
       <c r="O23" t="s">
-        <v>254</v>
+        <v>237</v>
       </c>
       <c r="P23" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -3028,16 +3258,16 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F24" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H24" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="I24" s="9">
         <v>40834</v>
@@ -3046,22 +3276,22 @@
         <v>1.7708333333333299</v>
       </c>
       <c r="L24" s="12" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="N24" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="O24" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="P24" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -3073,16 +3303,16 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F25" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="H25" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="I25" s="9">
         <v>40834</v>
@@ -3091,22 +3321,22 @@
         <v>1.8125</v>
       </c>
       <c r="L25" s="12" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="N25" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="O25" t="s">
-        <v>256</v>
+        <v>239</v>
       </c>
       <c r="P25" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f>A19+1</f>
-        <v>12</v>
+        <f t="shared" si="0"/>
+        <v>25</v>
       </c>
       <c r="B26">
         <v>8</v>
@@ -3118,16 +3348,16 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F26" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H26" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="I26" s="9">
         <v>40834</v>
@@ -3136,22 +3366,22 @@
         <v>1.8541666666666701</v>
       </c>
       <c r="L26" s="12" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="O26" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="P26" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B27">
         <v>9</v>
@@ -3163,16 +3393,16 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F27" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="H27" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I27" s="9">
         <v>40834</v>
@@ -3181,43 +3411,43 @@
         <v>1.8958333333333299</v>
       </c>
       <c r="L27" s="12" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="N27" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="O27" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="P27" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f>A25+1</f>
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="b">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
         <v>12</v>
       </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="D28" t="b">
-        <v>1</v>
-      </c>
-      <c r="E28" t="s">
-        <v>18</v>
-      </c>
       <c r="F28" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
       <c r="H28" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="I28" s="9">
         <v>40834</v>
@@ -3226,22 +3456,22 @@
         <v>1.9375</v>
       </c>
       <c r="L28" s="12" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="N28" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="O28" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="P28" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -3253,16 +3483,16 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F29" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="H29" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="I29" s="9">
         <v>40834</v>
@@ -3271,22 +3501,22 @@
         <v>1.9791666666666701</v>
       </c>
       <c r="L29" s="12" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="N29" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="O29" t="s">
-        <v>260</v>
+        <v>243</v>
       </c>
       <c r="P29" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f>A27+1</f>
-        <v>14</v>
+        <f t="shared" si="0"/>
+        <v>29</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -3298,16 +3528,16 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F30" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>235</v>
+        <v>218</v>
       </c>
       <c r="H30" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="I30" s="9">
         <v>40834</v>
@@ -3316,22 +3546,22 @@
         <v>2.0208333333333299</v>
       </c>
       <c r="L30" s="12" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="N30" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="O30" t="s">
-        <v>261</v>
+        <v>244</v>
       </c>
       <c r="P30" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -3343,16 +3573,16 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F31" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
       <c r="H31" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="I31" s="9">
         <v>40834</v>
@@ -3361,22 +3591,22 @@
         <v>2.0625</v>
       </c>
       <c r="L31" s="12" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="N31" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="O31" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="P31" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -3388,16 +3618,16 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="F32" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>306</v>
+        <v>289</v>
       </c>
       <c r="H32" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
       <c r="I32" s="9">
         <v>40834</v>
@@ -3406,22 +3636,22 @@
         <v>2.1041666666666701</v>
       </c>
       <c r="L32" s="12" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="N32" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="O32" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="P32" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -3433,16 +3663,16 @@
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="F33" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="H33" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
       <c r="I33" s="9">
         <v>40834</v>
@@ -3451,22 +3681,22 @@
         <v>2.1458333333333299</v>
       </c>
       <c r="L33" s="12" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="N33" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="O33" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
       <c r="P33" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -3478,16 +3708,16 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="F34" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>304</v>
+        <v>287</v>
       </c>
       <c r="H34" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
       <c r="I34" s="9">
         <v>40834</v>
@@ -3496,22 +3726,22 @@
         <v>2.1875</v>
       </c>
       <c r="L34" s="12" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="N34" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="O34" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="P34" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -3523,16 +3753,16 @@
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="F35" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>302</v>
+        <v>285</v>
       </c>
       <c r="H35" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
       <c r="I35" s="9">
         <v>40834</v>
@@ -3541,22 +3771,22 @@
         <v>2.2291666666666701</v>
       </c>
       <c r="L35" s="12" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="N35" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="O35" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="P35" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -3568,16 +3798,16 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="F36" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>301</v>
+        <v>284</v>
       </c>
       <c r="H36" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="I36" s="9">
         <v>40834</v>
@@ -3586,22 +3816,22 @@
         <v>2.2708333333333299</v>
       </c>
       <c r="L36" s="12" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="N36" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="O36" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="P36" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -3613,16 +3843,16 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="F37" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>300</v>
+        <v>283</v>
       </c>
       <c r="H37" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="I37" s="9">
         <v>40834</v>
@@ -3631,22 +3861,22 @@
         <v>2.3125</v>
       </c>
       <c r="L37" s="12" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="N37" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="O37" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="P37" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -3658,16 +3888,16 @@
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="F38" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>299</v>
+        <v>282</v>
       </c>
       <c r="H38" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="I38" s="9">
         <v>40834</v>
@@ -3676,22 +3906,22 @@
         <v>2.3541666666666701</v>
       </c>
       <c r="L38" s="12" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="N38" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="O38" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
       <c r="P38" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -3703,16 +3933,16 @@
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="F39" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>298</v>
+        <v>281</v>
       </c>
       <c r="H39" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="I39" s="9">
         <v>40834</v>
@@ -3721,22 +3951,22 @@
         <v>2.3958333333333299</v>
       </c>
       <c r="L39" s="12" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="N39" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="O39" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
       <c r="P39" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -3748,16 +3978,16 @@
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="F40" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>297</v>
+        <v>280</v>
       </c>
       <c r="H40" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="I40" s="9">
         <v>40834</v>
@@ -3766,22 +3996,22 @@
         <v>2.4375</v>
       </c>
       <c r="L40" s="12" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="N40" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="O40" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="P40" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="41" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -3793,16 +4023,16 @@
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="F41" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>296</v>
+        <v>279</v>
       </c>
       <c r="H41" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="I41" s="9">
         <v>40834</v>
@@ -3811,22 +4041,22 @@
         <v>2.4791666666666701</v>
       </c>
       <c r="L41" s="12" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="N41" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="O41" t="s">
-        <v>282</v>
+        <v>265</v>
       </c>
       <c r="P41" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -3838,16 +4068,16 @@
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="F42" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>286</v>
+        <v>269</v>
       </c>
       <c r="H42" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
       <c r="I42" s="9">
         <v>40834</v>
@@ -3856,22 +4086,22 @@
         <v>2.5208333333333299</v>
       </c>
       <c r="L42" s="12" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="N42" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="O42" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
       <c r="P42" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="43" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -3883,16 +4113,16 @@
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="F43" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>287</v>
+        <v>270</v>
       </c>
       <c r="H43" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
       <c r="I43" s="9">
         <v>40834</v>
@@ -3901,22 +4131,22 @@
         <v>2.5625</v>
       </c>
       <c r="L43" s="12" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="N43" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="O43" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
       <c r="P43" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="44" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -3928,16 +4158,16 @@
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="F44" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>288</v>
+        <v>271</v>
       </c>
       <c r="H44" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
       <c r="I44" s="9">
         <v>40834</v>
@@ -3946,22 +4176,22 @@
         <v>2.6041666666666701</v>
       </c>
       <c r="L44" s="12" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="N44" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="O44" t="s">
-        <v>309</v>
+        <v>292</v>
       </c>
       <c r="P44" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="45" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -3973,16 +4203,16 @@
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="F45" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>290</v>
+        <v>273</v>
       </c>
       <c r="H45" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
       <c r="I45" s="9">
         <v>40834</v>
@@ -3991,22 +4221,22 @@
         <v>2.6458333333333299</v>
       </c>
       <c r="L45" s="12" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="N45" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="O45" t="s">
-        <v>310</v>
+        <v>293</v>
       </c>
       <c r="P45" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -4018,16 +4248,16 @@
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="F46" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>289</v>
+        <v>272</v>
       </c>
       <c r="H46" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
       <c r="I46" s="9">
         <v>40834</v>
@@ -4036,22 +4266,22 @@
         <v>2.6875</v>
       </c>
       <c r="L46" s="12" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="N46" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="O46" t="s">
-        <v>311</v>
+        <v>294</v>
       </c>
       <c r="P46" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="47" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -4063,16 +4293,16 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="F47" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>291</v>
+        <v>274</v>
       </c>
       <c r="H47" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
       <c r="I47" s="9">
         <v>40834</v>
@@ -4081,22 +4311,22 @@
         <v>2.7291666666666701</v>
       </c>
       <c r="L47" s="12" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="N47" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="O47" t="s">
-        <v>312</v>
+        <v>295</v>
       </c>
       <c r="P47" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="48" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -4108,16 +4338,16 @@
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="F48" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>292</v>
+        <v>275</v>
       </c>
       <c r="H48" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
       <c r="I48" s="9">
         <v>40834</v>
@@ -4126,22 +4356,22 @@
         <v>2.7708333333333299</v>
       </c>
       <c r="L48" s="12" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="N48" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="O48" t="s">
-        <v>313</v>
+        <v>296</v>
       </c>
       <c r="P48" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="49" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -4153,16 +4383,16 @@
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="F49" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>293</v>
+        <v>276</v>
       </c>
       <c r="H49" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
       <c r="I49" s="9">
         <v>40834</v>
@@ -4171,22 +4401,22 @@
         <v>2.8125</v>
       </c>
       <c r="L49" s="12" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="N49" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="O49" t="s">
-        <v>314</v>
+        <v>297</v>
       </c>
       <c r="P49" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="50" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -4198,16 +4428,16 @@
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="F50" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>294</v>
+        <v>277</v>
       </c>
       <c r="H50" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
       <c r="I50" s="9">
         <v>40834</v>
@@ -4216,22 +4446,22 @@
         <v>2.8541666666666701</v>
       </c>
       <c r="L50" s="12" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="N50" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="O50" t="s">
-        <v>315</v>
+        <v>298</v>
       </c>
       <c r="P50" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="51" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -4243,16 +4473,16 @@
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="F51" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>295</v>
+        <v>278</v>
       </c>
       <c r="H51" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
       <c r="I51" s="9">
         <v>40834</v>
@@ -4261,22 +4491,22 @@
         <v>2.8958333333333299</v>
       </c>
       <c r="L51" s="12" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="N51" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="O51" t="s">
-        <v>316</v>
+        <v>299</v>
       </c>
       <c r="P51" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52">
-        <f>A42+1</f>
-        <v>27</v>
+        <f t="shared" si="0"/>
+        <v>51</v>
       </c>
       <c r="B52">
         <v>9</v>
@@ -4288,16 +4518,16 @@
         <v>0</v>
       </c>
       <c r="E52" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="F52" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="G52" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="H52" t="s">
         <v>151</v>
-      </c>
-      <c r="H52" t="s">
-        <v>161</v>
       </c>
       <c r="I52" s="9">
         <v>40834</v>
@@ -4306,22 +4536,22 @@
         <v>2.9375</v>
       </c>
       <c r="L52" s="12" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="N52" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="O52" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="P52" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="B53">
         <v>9</v>
@@ -4333,16 +4563,16 @@
         <v>0</v>
       </c>
       <c r="E53" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="F53" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="G53" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="H53" t="s">
         <v>152</v>
-      </c>
-      <c r="H53" t="s">
-        <v>162</v>
       </c>
       <c r="I53" s="9">
         <v>40834</v>
@@ -4351,22 +4581,22 @@
         <v>2.9791666666666701</v>
       </c>
       <c r="L53" s="12" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="N53" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="O53" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="P53" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="B54">
         <v>9</v>
@@ -4378,16 +4608,16 @@
         <v>0</v>
       </c>
       <c r="E54" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F54" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="G54" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="H54" t="s">
         <v>153</v>
-      </c>
-      <c r="H54" t="s">
-        <v>163</v>
       </c>
       <c r="I54" s="9">
         <v>40834</v>
@@ -4396,22 +4626,22 @@
         <v>3.0208333333333299</v>
       </c>
       <c r="L54" s="12" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="N54" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="O54" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="P54" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="B55">
         <v>9</v>
@@ -4423,16 +4653,16 @@
         <v>0</v>
       </c>
       <c r="E55" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="F55" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="G55" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="H55" t="s">
         <v>154</v>
-      </c>
-      <c r="H55" t="s">
-        <v>164</v>
       </c>
       <c r="I55" s="9">
         <v>40834</v>
@@ -4441,22 +4671,22 @@
         <v>3.0625</v>
       </c>
       <c r="L55" s="12" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="N55" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="O55" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="P55" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="B56">
         <v>9</v>
@@ -4471,13 +4701,13 @@
         <v>0</v>
       </c>
       <c r="F56" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="G56" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="H56" t="s">
         <v>155</v>
-      </c>
-      <c r="H56" t="s">
-        <v>165</v>
       </c>
       <c r="I56" s="9">
         <v>40834</v>
@@ -4486,22 +4716,22 @@
         <v>3.1041666666666701</v>
       </c>
       <c r="L56" s="12" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="N56" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="O56" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="P56" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="B57">
         <v>9</v>
@@ -4513,16 +4743,16 @@
         <v>0</v>
       </c>
       <c r="E57" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="F57" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="G57" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="H57" t="s">
         <v>156</v>
-      </c>
-      <c r="H57" t="s">
-        <v>166</v>
       </c>
       <c r="I57" s="9">
         <v>40834</v>
@@ -4531,22 +4761,22 @@
         <v>3.1458333333333299</v>
       </c>
       <c r="L57" s="12" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="N57" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="O57" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="P57" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="B58">
         <v>9</v>
@@ -4558,16 +4788,16 @@
         <v>0</v>
       </c>
       <c r="E58" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="F58" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="G58" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="H58" t="s">
         <v>157</v>
-      </c>
-      <c r="H58" t="s">
-        <v>167</v>
       </c>
       <c r="I58" s="9">
         <v>40834</v>
@@ -4576,22 +4806,22 @@
         <v>3.1875</v>
       </c>
       <c r="L58" s="12" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="N58" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="O58" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="P58" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="B59">
         <v>9</v>
@@ -4603,16 +4833,16 @@
         <v>0</v>
       </c>
       <c r="E59" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="F59" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="G59" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="H59" t="s">
         <v>158</v>
-      </c>
-      <c r="H59" t="s">
-        <v>168</v>
       </c>
       <c r="I59" s="9">
         <v>40834</v>
@@ -4621,22 +4851,22 @@
         <v>3.2291666666666701</v>
       </c>
       <c r="L59" s="12" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="N59" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="O59" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="P59" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="B60">
         <v>9</v>
@@ -4648,16 +4878,16 @@
         <v>0</v>
       </c>
       <c r="E60" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F60" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="G60" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="H60" t="s">
         <v>159</v>
-      </c>
-      <c r="H60" t="s">
-        <v>169</v>
       </c>
       <c r="I60" s="9">
         <v>40834</v>
@@ -4666,22 +4896,22 @@
         <v>3.2708333333333299</v>
       </c>
       <c r="L60" s="12" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="N60" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="O60" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="P60" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="B61">
         <v>9</v>
@@ -4693,16 +4923,16 @@
         <v>0</v>
       </c>
       <c r="E61" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="F61" t="s">
+        <v>140</v>
+      </c>
+      <c r="G61" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="G61" s="6" t="s">
+      <c r="H61" t="s">
         <v>160</v>
-      </c>
-      <c r="H61" t="s">
-        <v>170</v>
       </c>
       <c r="I61" s="9">
         <v>40834</v>
@@ -4711,16 +4941,16 @@
         <v>3.3125</v>
       </c>
       <c r="L61" s="12" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="N61" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="O61" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="P61" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -4738,7 +4968,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4750,37 +4980,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C1" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D1" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E1" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="F1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="G1" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="H1" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="I1" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="J1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="K1" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -5124,37 +5354,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="D1" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E1" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="F1" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="G1" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="H1" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="I1" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="J1" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="K1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -5317,25 +5547,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="C1" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="D1" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="E1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="F1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="G1" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -5343,16 +5573,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D2">
         <v>150</v>
       </c>
       <c r="F2" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -5361,16 +5591,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <v>150</v>
       </c>
       <c r="F3" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -5379,16 +5609,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C4" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="D4">
         <v>150</v>
       </c>
       <c r="F4" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -5397,16 +5627,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C5" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="D5">
         <v>150</v>
       </c>
       <c r="F5" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -5415,16 +5645,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C6" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D6">
         <v>150</v>
       </c>
       <c r="F6" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -5433,16 +5663,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C7" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="D7">
         <v>129</v>
       </c>
       <c r="F7" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -5451,16 +5681,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C8" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="D8">
         <v>129</v>
       </c>
       <c r="F8" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -5469,16 +5699,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C9" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="D9">
         <v>129</v>
       </c>
       <c r="F9" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -5487,16 +5717,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C10" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="D10">
         <v>129</v>
       </c>
       <c r="F10" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -5505,16 +5735,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C11" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="D11">
         <v>129</v>
       </c>
       <c r="F11" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -5523,16 +5753,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C12" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="D12">
         <v>99</v>
       </c>
       <c r="F12" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -5541,16 +5771,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C13" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D13">
         <v>99</v>
       </c>
       <c r="F13" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -5559,16 +5789,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C14" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="D14">
         <v>99</v>
       </c>
       <c r="F14" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -5577,16 +5807,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C15" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="D15">
         <v>99</v>
       </c>
       <c r="F15" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -5595,16 +5825,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C16" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="D16">
         <v>99</v>
       </c>
       <c r="F16" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -5613,16 +5843,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C17" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="D17">
         <v>99</v>
       </c>
       <c r="F17" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -5631,16 +5861,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C18" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="D18">
         <v>99</v>
       </c>
       <c r="F18" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -5649,16 +5879,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C19" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="D19">
         <v>99</v>
       </c>
       <c r="F19" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -5667,16 +5897,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C20" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="D20">
         <v>99</v>
       </c>
       <c r="F20" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -5685,16 +5915,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" t="s">
         <v>128</v>
-      </c>
-      <c r="C21" t="s">
-        <v>138</v>
       </c>
       <c r="D21">
         <v>99</v>
       </c>
       <c r="F21" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -5703,16 +5933,16 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="C22" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="D22">
         <v>25</v>
       </c>
       <c r="F22" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -5721,16 +5951,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="C23" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D23">
         <v>25</v>
       </c>
       <c r="F23" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -5739,16 +5969,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="C24" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="D24">
         <v>25</v>
       </c>
       <c r="F24" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -5757,16 +5987,16 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="C25" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="D25">
         <v>25</v>
       </c>
       <c r="F25" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -5775,16 +6005,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="C26" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="D26">
         <v>25</v>
       </c>
       <c r="F26" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -5793,16 +6023,16 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="C27" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D27">
         <v>25</v>
       </c>
       <c r="F27" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -5811,16 +6041,16 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="C28" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="D28">
         <v>25</v>
       </c>
       <c r="F28" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -5829,16 +6059,16 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="C29" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="D29">
         <v>25</v>
       </c>
       <c r="F29" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -5847,16 +6077,16 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="C30" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="D30">
         <v>25</v>
       </c>
       <c r="F30" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -5865,16 +6095,16 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>129</v>
+      </c>
+      <c r="C31" t="s">
         <v>139</v>
-      </c>
-      <c r="C31" t="s">
-        <v>149</v>
       </c>
       <c r="D31">
         <v>25</v>
       </c>
       <c r="F31" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
series tab now shows first changed the order of the movies - moved the drab banners to the bottom
</commit_message>
<xml_diff>
--- a/data/EventData.xlsx
+++ b/data/EventData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="WBS" sheetId="2" r:id="rId1"/>
@@ -2172,8 +2172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2260,15 +2260,15 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="180.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="156.75" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -2280,49 +2280,50 @@
         <v>0</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>234</v>
+        <v>268</v>
       </c>
       <c r="H2" t="s">
-        <v>1</v>
+        <v>249</v>
       </c>
       <c r="I2" s="9">
         <v>40834</v>
       </c>
       <c r="J2" s="5">
-        <v>0.85416666666666663</v>
-      </c>
+        <v>1.0625</v>
+      </c>
+      <c r="K2" s="4"/>
       <c r="L2" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="N2" t="s">
-        <v>240</v>
+        <v>269</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>270</v>
       </c>
       <c r="O2" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="P2" t="s">
-        <v>239</v>
+        <v>271</v>
       </c>
       <c r="Q2" t="s">
-        <v>236</v>
+        <v>272</v>
       </c>
       <c r="S2" t="s">
-        <v>235</v>
+        <v>273</v>
       </c>
       <c r="T2">
         <v>2011</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="108.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="84.75" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>A2+1</f>
+        <f t="shared" ref="A3:A51" si="0">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
@@ -2334,7 +2335,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>241</v>
+        <v>274</v>
       </c>
       <c r="H3" t="s">
         <v>247</v>
@@ -2343,40 +2344,40 @@
         <v>40834</v>
       </c>
       <c r="J3" s="5">
-        <v>0.89583333333333337</v>
+        <v>1.1041666666666701</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>246</v>
+        <v>275</v>
+      </c>
+      <c r="N3" t="s">
+        <v>276</v>
       </c>
       <c r="O3" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="P3" t="s">
-        <v>242</v>
+        <v>277</v>
       </c>
       <c r="Q3" t="s">
-        <v>245</v>
+        <v>279</v>
       </c>
       <c r="S3" t="s">
-        <v>244</v>
+        <v>278</v>
       </c>
       <c r="T3">
         <v>2011</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="132.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="96.75" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>A3+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -2388,50 +2389,49 @@
         <v>0</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>248</v>
+        <v>280</v>
       </c>
       <c r="H4" t="s">
-        <v>249</v>
+        <v>2</v>
       </c>
       <c r="I4" s="9">
         <v>40834</v>
       </c>
       <c r="J4" s="5">
-        <v>0.9375</v>
-      </c>
-      <c r="K4" s="4"/>
+        <v>1.1458333333333299</v>
+      </c>
       <c r="L4" s="12" t="s">
-        <v>250</v>
+        <v>281</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>251</v>
+        <v>282</v>
       </c>
       <c r="O4" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="P4" t="s">
-        <v>252</v>
+        <v>283</v>
       </c>
       <c r="Q4" t="s">
-        <v>254</v>
+        <v>285</v>
       </c>
       <c r="S4" t="s">
-        <v>253</v>
+        <v>284</v>
       </c>
       <c r="T4">
         <v>2011</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="108.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="156.75" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>A4+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
@@ -2443,49 +2443,50 @@
         <v>0</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>255</v>
+        <v>286</v>
       </c>
       <c r="H5" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="I5" s="9">
         <v>40834</v>
       </c>
       <c r="J5" s="5">
-        <v>0.97916666666666696</v>
-      </c>
+        <v>1.1875</v>
+      </c>
+      <c r="K5" s="4"/>
       <c r="L5" s="12" t="s">
-        <v>257</v>
-      </c>
-      <c r="N5" t="s">
-        <v>258</v>
+        <v>287</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>288</v>
       </c>
       <c r="O5" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="P5" t="s">
-        <v>259</v>
+        <v>289</v>
       </c>
       <c r="Q5" t="s">
-        <v>261</v>
+        <v>291</v>
       </c>
       <c r="S5" t="s">
-        <v>260</v>
+        <v>290</v>
       </c>
       <c r="T5">
         <v>2011</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="72.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="144.75" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f>A5+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
@@ -2497,49 +2498,46 @@
         <v>0</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>262</v>
+        <v>292</v>
       </c>
       <c r="H6" t="s">
-        <v>247</v>
+        <v>1</v>
       </c>
       <c r="I6" s="9">
         <v>40834</v>
       </c>
       <c r="J6" s="5">
-        <v>1.0208333333333299</v>
+        <v>1.2291666666666701</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="N6" s="2" t="s">
-        <v>264</v>
+        <v>293</v>
+      </c>
+      <c r="N6" t="s">
+        <v>294</v>
       </c>
       <c r="O6" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="P6" t="s">
-        <v>265</v>
+        <v>295</v>
       </c>
       <c r="Q6" t="s">
-        <v>267</v>
+        <v>297</v>
       </c>
       <c r="S6" t="s">
-        <v>266</v>
-      </c>
-      <c r="T6">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" ht="156.75" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="180.75" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" ref="A7:A61" si="0">A6+1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D7" t="b">
         <v>1</v>
@@ -2551,50 +2549,49 @@
         <v>0</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>268</v>
+        <v>234</v>
       </c>
       <c r="H7" t="s">
-        <v>249</v>
+        <v>1</v>
       </c>
       <c r="I7" s="9">
         <v>40834</v>
       </c>
       <c r="J7" s="5">
-        <v>1.0625</v>
-      </c>
-      <c r="K7" s="4"/>
+        <v>0.85416666666666663</v>
+      </c>
       <c r="L7" s="12" t="s">
-        <v>269</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>270</v>
+        <v>237</v>
+      </c>
+      <c r="N7" t="s">
+        <v>240</v>
       </c>
       <c r="O7" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="P7" t="s">
-        <v>271</v>
+        <v>239</v>
       </c>
       <c r="Q7" t="s">
-        <v>272</v>
+        <v>236</v>
       </c>
       <c r="S7" t="s">
-        <v>273</v>
+        <v>235</v>
       </c>
       <c r="T7">
         <v>2011</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="84.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="108.75" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" t="b">
         <v>1</v>
@@ -2606,7 +2603,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>274</v>
+        <v>241</v>
       </c>
       <c r="H8" t="s">
         <v>247</v>
@@ -2615,40 +2612,40 @@
         <v>40834</v>
       </c>
       <c r="J8" s="5">
-        <v>1.1041666666666701</v>
+        <v>0.89583333333333337</v>
       </c>
       <c r="L8" s="12" t="s">
-        <v>275</v>
-      </c>
-      <c r="N8" t="s">
-        <v>276</v>
+        <v>243</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>246</v>
       </c>
       <c r="O8" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="P8" t="s">
-        <v>277</v>
+        <v>242</v>
       </c>
       <c r="Q8" t="s">
-        <v>279</v>
+        <v>245</v>
       </c>
       <c r="S8" t="s">
-        <v>278</v>
+        <v>244</v>
       </c>
       <c r="T8">
         <v>2011</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="96.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="132.75" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D9" t="b">
         <v>1</v>
@@ -2660,49 +2657,50 @@
         <v>0</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>280</v>
+        <v>248</v>
       </c>
       <c r="H9" t="s">
-        <v>2</v>
+        <v>249</v>
       </c>
       <c r="I9" s="9">
         <v>40834</v>
       </c>
       <c r="J9" s="5">
-        <v>1.1458333333333299</v>
-      </c>
+        <v>0.9375</v>
+      </c>
+      <c r="K9" s="4"/>
       <c r="L9" s="12" t="s">
-        <v>281</v>
+        <v>250</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>282</v>
+        <v>251</v>
       </c>
       <c r="O9" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="P9" t="s">
-        <v>283</v>
+        <v>252</v>
       </c>
       <c r="Q9" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
       <c r="S9" t="s">
-        <v>284</v>
+        <v>253</v>
       </c>
       <c r="T9">
         <v>2011</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="108.75" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D10" t="b">
         <v>1</v>
@@ -2714,50 +2712,49 @@
         <v>0</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>286</v>
+        <v>255</v>
       </c>
       <c r="H10" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="I10" s="9">
         <v>40834</v>
       </c>
       <c r="J10" s="5">
-        <v>1.1875</v>
-      </c>
-      <c r="K10" s="4"/>
+        <v>0.97916666666666696</v>
+      </c>
       <c r="L10" s="12" t="s">
-        <v>287</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>288</v>
+        <v>257</v>
+      </c>
+      <c r="N10" t="s">
+        <v>258</v>
       </c>
       <c r="O10" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="P10" t="s">
-        <v>289</v>
+        <v>259</v>
       </c>
       <c r="Q10" t="s">
-        <v>291</v>
+        <v>261</v>
       </c>
       <c r="S10" t="s">
-        <v>290</v>
+        <v>260</v>
       </c>
       <c r="T10">
         <v>2011</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="144.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>
@@ -2769,34 +2766,37 @@
         <v>0</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>292</v>
+        <v>262</v>
       </c>
       <c r="H11" t="s">
-        <v>1</v>
+        <v>247</v>
       </c>
       <c r="I11" s="9">
         <v>40834</v>
       </c>
       <c r="J11" s="5">
-        <v>1.2291666666666701</v>
+        <v>1.0208333333333299</v>
       </c>
       <c r="L11" s="12" t="s">
-        <v>293</v>
-      </c>
-      <c r="N11" t="s">
-        <v>294</v>
+        <v>263</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>264</v>
       </c>
       <c r="O11" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="P11" t="s">
-        <v>295</v>
+        <v>265</v>
       </c>
       <c r="Q11" t="s">
-        <v>297</v>
+        <v>267</v>
       </c>
       <c r="S11" t="s">
-        <v>296</v>
+        <v>266</v>
+      </c>
+      <c r="T11">
+        <v>2011</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="36.75" x14ac:dyDescent="0.25">
@@ -3555,7 +3555,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C28">
         <v>7</v>
@@ -3600,7 +3600,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C29">
         <v>8</v>
@@ -3645,7 +3645,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C30">
         <v>9</v>
@@ -3690,7 +3690,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C31">
         <v>5</v>
@@ -3735,7 +3735,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C32">
         <v>6</v>
@@ -3780,7 +3780,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C33">
         <v>7</v>
@@ -3870,7 +3870,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C35">
         <v>7</v>
@@ -3915,7 +3915,7 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C36">
         <v>8</v>
@@ -3960,7 +3960,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C37">
         <v>9</v>
@@ -4050,7 +4050,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C39">
         <v>5</v>
@@ -4095,7 +4095,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C40">
         <v>6</v>
@@ -4140,7 +4140,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C41">
         <v>3</v>
@@ -4230,7 +4230,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C43">
         <v>4</v>
@@ -4320,7 +4320,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C45">
         <v>9</v>
@@ -4410,7 +4410,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C47">
         <v>3</v>
@@ -4455,7 +4455,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C48">
         <v>4</v>
@@ -4500,7 +4500,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C49">
         <v>5</v>
@@ -4545,7 +4545,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -4590,7 +4590,7 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C51">
         <v>2</v>
@@ -4643,7 +4643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
@@ -5968,7 +5968,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A36" si="0">A3+1</f>
+        <f t="shared" ref="A4:A32" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">

</xml_diff>

<commit_message>
Added rating to event details fragment. Channel name also shows correctly now.
</commit_message>
<xml_diff>
--- a/data/EventData.xlsx
+++ b/data/EventData.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="442">
   <si>
     <t>Movies</t>
   </si>
@@ -375,30 +375,6 @@
     <t>Vaugan/Satya</t>
   </si>
   <si>
-    <t>ddaily094.jpg</t>
-  </si>
-  <si>
-    <t>ddaily095.jpg</t>
-  </si>
-  <si>
-    <t>ddaily096.jpg</t>
-  </si>
-  <si>
-    <t>ddaily097.jpg</t>
-  </si>
-  <si>
-    <t>ddaily098.jpg</t>
-  </si>
-  <si>
-    <t>ddaily099.jpg</t>
-  </si>
-  <si>
-    <t>ddaily100.jpg</t>
-  </si>
-  <si>
-    <t>ddaily101.jpg</t>
-  </si>
-  <si>
     <t>category</t>
   </si>
   <si>
@@ -1252,6 +1228,126 @@
   </si>
   <si>
     <t>http://omusic.dstv.com/12763931/Roger_Sanchez/Album/Release_Yourself</t>
+  </si>
+  <si>
+    <t>series_poster01.jpg</t>
+  </si>
+  <si>
+    <t>series_poster02.jpg</t>
+  </si>
+  <si>
+    <t>series_poster03.jpg</t>
+  </si>
+  <si>
+    <t>series_poster04.jpg</t>
+  </si>
+  <si>
+    <t>series_poster05.jpg</t>
+  </si>
+  <si>
+    <t>series_poster06.jpg</t>
+  </si>
+  <si>
+    <t>series_poster07.jpg</t>
+  </si>
+  <si>
+    <t>series_poster08.jpg</t>
+  </si>
+  <si>
+    <t>series_poster09.jpg</t>
+  </si>
+  <si>
+    <t>series_poster10.jpg</t>
+  </si>
+  <si>
+    <t>sport_poster01.jpg</t>
+  </si>
+  <si>
+    <t>sport_poster10.jpg</t>
+  </si>
+  <si>
+    <t>sport_poster09.jpg</t>
+  </si>
+  <si>
+    <t>sport_poster08.jpg</t>
+  </si>
+  <si>
+    <t>sport_poster07.jpg</t>
+  </si>
+  <si>
+    <t>sport_poster06.jpg</t>
+  </si>
+  <si>
+    <t>sport_poster05.jpg</t>
+  </si>
+  <si>
+    <t>sport_poster04.jpg</t>
+  </si>
+  <si>
+    <t>sport_poster02.jpg</t>
+  </si>
+  <si>
+    <t>sport_poster03.jpg</t>
+  </si>
+  <si>
+    <t>documentary_poster01.jpg</t>
+  </si>
+  <si>
+    <t>documentary_poster02.jpg</t>
+  </si>
+  <si>
+    <t>documentary_poster03.jpg</t>
+  </si>
+  <si>
+    <t>documentary_poster04.jpg</t>
+  </si>
+  <si>
+    <t>documentary_poster05.jpg</t>
+  </si>
+  <si>
+    <t>documentary_poster06.jpg</t>
+  </si>
+  <si>
+    <t>documentary_poster07.jpg</t>
+  </si>
+  <si>
+    <t>documentary_poster08.jpg</t>
+  </si>
+  <si>
+    <t>documentary_poster09.jpg</t>
+  </si>
+  <si>
+    <t>documentary_poster10.jpg</t>
+  </si>
+  <si>
+    <t>lifestyle_poster01.jpg</t>
+  </si>
+  <si>
+    <t>lifestyle_poster02.jpg</t>
+  </si>
+  <si>
+    <t>lifestyle_poster03.jpg</t>
+  </si>
+  <si>
+    <t>lifestyle_poster04.jpg</t>
+  </si>
+  <si>
+    <t>lifestyle_poster05.jpg</t>
+  </si>
+  <si>
+    <t>lifestyle_poster06.jpg</t>
+  </si>
+  <si>
+    <t>lifestyle_poster07.jpg</t>
+  </si>
+  <si>
+    <t>lifestyle_poster08.jpg</t>
+  </si>
+  <si>
+    <t>lifestyle_poster09.jpg</t>
+  </si>
+  <si>
+    <t>lifestyle_poster10.jpg</t>
   </si>
 </sst>
 </file>
@@ -1854,7 +1950,7 @@
         <v>64</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1863,7 +1959,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>32</v>
@@ -1934,7 +2030,7 @@
       </c>
       <c r="E9" s="19"/>
       <c r="F9" s="22" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2043,7 +2139,7 @@
         <v>10</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="F15" s="22"/>
     </row>
@@ -2172,8 +2268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="N35" workbookViewId="0">
+      <selection activeCell="R52" sqref="R52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2192,7 +2288,7 @@
     <col min="12" max="12" width="15.85546875" style="12" customWidth="1"/>
     <col min="13" max="13" width="7.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.85546875" customWidth="1"/>
     <col min="17" max="17" width="47.28515625" customWidth="1"/>
     <col min="18" max="18" width="13.28515625" customWidth="1"/>
     <col min="20" max="20" width="15.5703125" customWidth="1"/>
@@ -2212,7 +2308,7 @@
         <v>77</v>
       </c>
       <c r="E1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>37</v>
@@ -2251,7 +2347,7 @@
         <v>44</v>
       </c>
       <c r="R1" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="S1" t="s">
         <v>45</v>
@@ -2280,10 +2376,10 @@
         <v>0</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="H2" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="I2" s="9">
         <v>40834</v>
@@ -2293,22 +2389,25 @@
       </c>
       <c r="K2" s="4"/>
       <c r="L2" s="12" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="O2" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="P2" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="Q2" t="s">
-        <v>272</v>
+        <v>264</v>
+      </c>
+      <c r="R2">
+        <v>7</v>
       </c>
       <c r="S2" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="T2">
         <v>2011</v>
@@ -2335,10 +2434,10 @@
         <v>0</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="H3" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="I3" s="9">
         <v>40834</v>
@@ -2347,22 +2446,25 @@
         <v>1.1041666666666701</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="N3" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="O3" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="P3" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="Q3" t="s">
-        <v>279</v>
+        <v>271</v>
+      </c>
+      <c r="R3">
+        <v>8</v>
       </c>
       <c r="S3" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="T3">
         <v>2011</v>
@@ -2389,7 +2491,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="H4" t="s">
         <v>2</v>
@@ -2401,22 +2503,25 @@
         <v>1.1458333333333299</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="O4" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="P4" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="Q4" t="s">
-        <v>285</v>
+        <v>277</v>
+      </c>
+      <c r="R4">
+        <v>9</v>
       </c>
       <c r="S4" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="T4">
         <v>2011</v>
@@ -2443,10 +2548,10 @@
         <v>0</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="H5" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="I5" s="9">
         <v>40834</v>
@@ -2456,22 +2561,25 @@
       </c>
       <c r="K5" s="4"/>
       <c r="L5" s="12" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="O5" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="P5" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="Q5" t="s">
-        <v>291</v>
+        <v>283</v>
+      </c>
+      <c r="R5">
+        <v>6</v>
       </c>
       <c r="S5" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="T5">
         <v>2011</v>
@@ -2498,7 +2606,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="H6" t="s">
         <v>1</v>
@@ -2510,22 +2618,25 @@
         <v>1.2291666666666701</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="N6" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="O6" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="P6" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="Q6" t="s">
-        <v>297</v>
+        <v>289</v>
+      </c>
+      <c r="R6">
+        <v>7</v>
       </c>
       <c r="S6" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="180.75" x14ac:dyDescent="0.25">
@@ -2549,7 +2660,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="H7" t="s">
         <v>1</v>
@@ -2561,22 +2672,25 @@
         <v>0.85416666666666663</v>
       </c>
       <c r="L7" s="12" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="N7" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="O7" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="P7" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="Q7" t="s">
-        <v>236</v>
+        <v>228</v>
+      </c>
+      <c r="R7">
+        <v>8</v>
       </c>
       <c r="S7" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="T7">
         <v>2011</v>
@@ -2603,10 +2717,10 @@
         <v>0</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="H8" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="I8" s="9">
         <v>40834</v>
@@ -2615,22 +2729,25 @@
         <v>0.89583333333333337</v>
       </c>
       <c r="L8" s="12" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="O8" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="P8" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="Q8" t="s">
-        <v>245</v>
+        <v>237</v>
+      </c>
+      <c r="R8">
+        <v>8</v>
       </c>
       <c r="S8" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="T8">
         <v>2011</v>
@@ -2657,10 +2774,10 @@
         <v>0</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="H9" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="I9" s="9">
         <v>40834</v>
@@ -2670,22 +2787,25 @@
       </c>
       <c r="K9" s="4"/>
       <c r="L9" s="12" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="O9" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="P9" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="Q9" t="s">
-        <v>254</v>
+        <v>246</v>
+      </c>
+      <c r="R9">
+        <v>8</v>
       </c>
       <c r="S9" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="T9">
         <v>2011</v>
@@ -2712,10 +2832,10 @@
         <v>0</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="H10" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="I10" s="9">
         <v>40834</v>
@@ -2724,22 +2844,25 @@
         <v>0.97916666666666696</v>
       </c>
       <c r="L10" s="12" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="N10" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="O10" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="P10" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="Q10" t="s">
-        <v>261</v>
+        <v>253</v>
+      </c>
+      <c r="R10">
+        <v>9</v>
       </c>
       <c r="S10" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="T10">
         <v>2011</v>
@@ -2766,10 +2889,10 @@
         <v>0</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="H11" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="I11" s="9">
         <v>40834</v>
@@ -2778,22 +2901,25 @@
         <v>1.0208333333333299</v>
       </c>
       <c r="L11" s="12" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="O11" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="P11" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="Q11" t="s">
-        <v>267</v>
+        <v>259</v>
+      </c>
+      <c r="R11">
+        <v>9</v>
       </c>
       <c r="S11" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="T11">
         <v>2011</v>
@@ -2820,7 +2946,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="H12" t="s">
         <v>5</v>
@@ -2838,13 +2964,16 @@
         <v>6</v>
       </c>
       <c r="N12" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="O12" t="s">
         <v>131</v>
       </c>
-      <c r="O12" t="s">
-        <v>139</v>
-      </c>
       <c r="P12" t="s">
-        <v>118</v>
+        <v>402</v>
+      </c>
+      <c r="R12">
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="60.75" x14ac:dyDescent="0.25">
@@ -2868,7 +2997,7 @@
         <v>3</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="H13" t="s">
         <v>5</v>
@@ -2886,13 +3015,16 @@
         <v>9</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="O13" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="P13" t="s">
-        <v>119</v>
+        <v>403</v>
+      </c>
+      <c r="R13">
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="60.75" x14ac:dyDescent="0.25">
@@ -2916,7 +3048,7 @@
         <v>3</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="H14" t="s">
         <v>3</v>
@@ -2928,19 +3060,22 @@
         <v>1.3541666666666701</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="L14" s="12" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="N14" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="O14" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="P14" t="s">
-        <v>120</v>
+        <v>404</v>
+      </c>
+      <c r="R14">
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="60.75" x14ac:dyDescent="0.25">
@@ -2964,7 +3099,7 @@
         <v>3</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="H15" t="s">
         <v>11</v>
@@ -2982,13 +3117,16 @@
         <v>4</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="O15" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="P15" t="s">
-        <v>121</v>
+        <v>405</v>
+      </c>
+      <c r="R15">
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="36.75" x14ac:dyDescent="0.25">
@@ -3012,7 +3150,7 @@
         <v>3</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="H16" t="s">
         <v>5</v>
@@ -3030,16 +3168,19 @@
         <v>6</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="O16" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="P16" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="60.75" x14ac:dyDescent="0.25">
+        <v>406</v>
+      </c>
+      <c r="R16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -3060,7 +3201,7 @@
         <v>3</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="H17" t="s">
         <v>5</v>
@@ -3078,16 +3219,19 @@
         <v>9</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="O17" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="P17" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="60.75" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+      <c r="R17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -3108,7 +3252,7 @@
         <v>3</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="H18" t="s">
         <v>3</v>
@@ -3120,22 +3264,25 @@
         <v>1.5208333333333299</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="L18" s="12" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="N18" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="O18" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="P18" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="60.75" x14ac:dyDescent="0.25">
+        <v>408</v>
+      </c>
+      <c r="R18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -3156,7 +3303,7 @@
         <v>3</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="H19" t="s">
         <v>11</v>
@@ -3174,16 +3321,19 @@
         <v>4</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="O19" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="P19" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="60.75" x14ac:dyDescent="0.25">
+        <v>409</v>
+      </c>
+      <c r="R19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -3204,7 +3354,7 @@
         <v>3</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="H20" t="s">
         <v>3</v>
@@ -3216,22 +3366,25 @@
         <v>1.6041666666666701</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="L20" s="12" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="N20" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="O20" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="P20" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="60.75" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+      <c r="R20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -3252,7 +3405,7 @@
         <v>3</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="H21" t="s">
         <v>11</v>
@@ -3270,16 +3423,19 @@
         <v>4</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="O21" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="P21" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="72.75" x14ac:dyDescent="0.25">
+        <v>411</v>
+      </c>
+      <c r="R21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -3297,7 +3453,7 @@
         <v>12</v>
       </c>
       <c r="F22" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>13</v>
@@ -3315,16 +3471,19 @@
         <v>15</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="O22" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="P22" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="60.75" x14ac:dyDescent="0.25">
+        <v>412</v>
+      </c>
+      <c r="R22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -3342,7 +3501,7 @@
         <v>12</v>
       </c>
       <c r="F23" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>16</v>
@@ -3360,16 +3519,19 @@
         <v>18</v>
       </c>
       <c r="N23" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="O23" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="P23" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" ht="72.75" x14ac:dyDescent="0.25">
+        <v>420</v>
+      </c>
+      <c r="R23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -3387,7 +3549,7 @@
         <v>12</v>
       </c>
       <c r="F24" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>20</v>
@@ -3405,16 +3567,19 @@
         <v>19</v>
       </c>
       <c r="N24" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="O24" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="P24" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
+        <v>421</v>
+      </c>
+      <c r="R24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -3432,7 +3597,7 @@
         <v>12</v>
       </c>
       <c r="F25" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>22</v>
@@ -3450,16 +3615,19 @@
         <v>23</v>
       </c>
       <c r="N25" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="O25" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="P25" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="72.75" x14ac:dyDescent="0.25">
+        <v>419</v>
+      </c>
+      <c r="R25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -3495,16 +3663,19 @@
         <v>15</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="O26" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="P26" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="60.75" x14ac:dyDescent="0.25">
+        <v>418</v>
+      </c>
+      <c r="R26">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="60.75" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -3522,7 +3693,7 @@
         <v>12</v>
       </c>
       <c r="F27" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>16</v>
@@ -3540,16 +3711,19 @@
         <v>18</v>
       </c>
       <c r="N27" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="O27" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="P27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" ht="72.75" x14ac:dyDescent="0.25">
+        <v>417</v>
+      </c>
+      <c r="R27">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -3567,10 +3741,10 @@
         <v>12</v>
       </c>
       <c r="F28" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="H28" t="s">
         <v>21</v>
@@ -3585,16 +3759,19 @@
         <v>19</v>
       </c>
       <c r="N28" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="O28" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="P28" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
+        <v>416</v>
+      </c>
+      <c r="R28">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -3612,7 +3789,7 @@
         <v>12</v>
       </c>
       <c r="F29" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="G29" s="6" t="s">
         <v>22</v>
@@ -3630,16 +3807,19 @@
         <v>23</v>
       </c>
       <c r="N29" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="O29" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="P29" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" ht="72.75" x14ac:dyDescent="0.25">
+        <v>415</v>
+      </c>
+      <c r="R29">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="72.75" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -3657,10 +3837,10 @@
         <v>12</v>
       </c>
       <c r="F30" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="H30" t="s">
         <v>21</v>
@@ -3675,16 +3855,19 @@
         <v>19</v>
       </c>
       <c r="N30" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="O30" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="P30" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
+        <v>414</v>
+      </c>
+      <c r="R30">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -3702,10 +3885,10 @@
         <v>12</v>
       </c>
       <c r="F31" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="H31" t="s">
         <v>14</v>
@@ -3720,16 +3903,19 @@
         <v>23</v>
       </c>
       <c r="N31" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="O31" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="P31" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+      <c r="R31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -3750,10 +3936,10 @@
         <v>109</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="H32" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="I32" s="9">
         <v>40834</v>
@@ -3765,16 +3951,19 @@
         <v>23</v>
       </c>
       <c r="N32" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="O32" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="P32" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
+        <v>422</v>
+      </c>
+      <c r="R32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -3795,10 +3984,10 @@
         <v>109</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H33" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="I33" s="9">
         <v>40834</v>
@@ -3810,16 +3999,19 @@
         <v>23</v>
       </c>
       <c r="N33" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="O33" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="P33" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
+        <v>423</v>
+      </c>
+      <c r="R33">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -3840,10 +4032,10 @@
         <v>109</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="H34" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="I34" s="9">
         <v>40834</v>
@@ -3855,16 +4047,19 @@
         <v>23</v>
       </c>
       <c r="N34" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="O34" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="P34" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
+        <v>424</v>
+      </c>
+      <c r="R34">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -3885,10 +4080,10 @@
         <v>109</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="H35" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="I35" s="9">
         <v>40834</v>
@@ -3900,16 +4095,19 @@
         <v>23</v>
       </c>
       <c r="N35" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="O35" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="P35" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
+        <v>425</v>
+      </c>
+      <c r="R35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -3930,10 +4128,10 @@
         <v>109</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="H36" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="I36" s="9">
         <v>40834</v>
@@ -3945,16 +4143,19 @@
         <v>23</v>
       </c>
       <c r="N36" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="O36" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="P36" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
+        <v>426</v>
+      </c>
+      <c r="R36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -3975,10 +4176,10 @@
         <v>109</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="H37" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="I37" s="9">
         <v>40834</v>
@@ -3990,16 +4191,19 @@
         <v>23</v>
       </c>
       <c r="N37" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="O37" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="P37" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
+        <v>427</v>
+      </c>
+      <c r="R37">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -4020,10 +4224,10 @@
         <v>109</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="H38" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="I38" s="9">
         <v>40834</v>
@@ -4035,16 +4239,19 @@
         <v>23</v>
       </c>
       <c r="N38" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="O38" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="P38" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+      <c r="R38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -4065,10 +4272,10 @@
         <v>109</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="H39" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="I39" s="9">
         <v>40834</v>
@@ -4080,16 +4287,19 @@
         <v>23</v>
       </c>
       <c r="N39" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="O39" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="P39" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
+        <v>429</v>
+      </c>
+      <c r="R39">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -4110,10 +4320,10 @@
         <v>109</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="H40" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="I40" s="9">
         <v>40834</v>
@@ -4125,16 +4335,19 @@
         <v>23</v>
       </c>
       <c r="N40" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="O40" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="P40" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
+        <v>430</v>
+      </c>
+      <c r="R40">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -4155,10 +4368,10 @@
         <v>109</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="H41" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="I41" s="9">
         <v>40834</v>
@@ -4170,16 +4383,19 @@
         <v>23</v>
       </c>
       <c r="N41" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="O41" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="P41" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
+        <v>431</v>
+      </c>
+      <c r="R41">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -4194,16 +4410,16 @@
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="F42" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="H42" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="I42" s="9">
         <v>40834</v>
@@ -4215,16 +4431,19 @@
         <v>23</v>
       </c>
       <c r="N42" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="O42" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="P42" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
+        <v>432</v>
+      </c>
+      <c r="R42">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -4239,16 +4458,16 @@
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="F43" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="H43" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="I43" s="9">
         <v>40834</v>
@@ -4260,16 +4479,19 @@
         <v>23</v>
       </c>
       <c r="N43" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="O43" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="P43" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
+        <v>433</v>
+      </c>
+      <c r="R43">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -4284,16 +4506,16 @@
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="F44" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="H44" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="I44" s="9">
         <v>40834</v>
@@ -4305,16 +4527,19 @@
         <v>23</v>
       </c>
       <c r="N44" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="O44" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="P44" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
+        <v>434</v>
+      </c>
+      <c r="R44">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -4329,16 +4554,16 @@
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="F45" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="H45" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="I45" s="9">
         <v>40834</v>
@@ -4350,16 +4575,19 @@
         <v>23</v>
       </c>
       <c r="N45" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="O45" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="P45" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
+        <v>435</v>
+      </c>
+      <c r="R45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -4374,16 +4602,16 @@
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="F46" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="H46" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="I46" s="9">
         <v>40834</v>
@@ -4395,16 +4623,19 @@
         <v>23</v>
       </c>
       <c r="N46" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="O46" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="P46" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
+        <v>436</v>
+      </c>
+      <c r="R46">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -4419,16 +4650,16 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
+        <v>188</v>
+      </c>
+      <c r="F47" t="s">
+        <v>188</v>
+      </c>
+      <c r="G47" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="F47" t="s">
-        <v>196</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>204</v>
-      </c>
       <c r="H47" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="I47" s="9">
         <v>40834</v>
@@ -4440,16 +4671,19 @@
         <v>23</v>
       </c>
       <c r="N47" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="O47" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="P47" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
+        <v>437</v>
+      </c>
+      <c r="R47">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -4464,16 +4698,16 @@
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="F48" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="H48" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="I48" s="9">
         <v>40834</v>
@@ -4485,16 +4719,19 @@
         <v>23</v>
       </c>
       <c r="N48" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="O48" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="P48" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
+        <v>438</v>
+      </c>
+      <c r="R48">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -4509,16 +4746,16 @@
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="F49" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="H49" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="I49" s="9">
         <v>40834</v>
@@ -4530,16 +4767,19 @@
         <v>23</v>
       </c>
       <c r="N49" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="O49" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="P49" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+      <c r="R49">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -4554,16 +4794,16 @@
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="F50" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="H50" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="I50" s="9">
         <v>40834</v>
@@ -4575,16 +4815,19 @@
         <v>23</v>
       </c>
       <c r="N50" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="O50" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="P50" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
+        <v>440</v>
+      </c>
+      <c r="R50">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -4599,16 +4842,16 @@
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="F51" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="H51" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="I51" s="9">
         <v>40834</v>
@@ -4620,13 +4863,16 @@
         <v>23</v>
       </c>
       <c r="N51" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="O51" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="P51" t="s">
-        <v>125</v>
+        <v>441</v>
+      </c>
+      <c r="R51">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -5927,19 +6173,19 @@
         <v>107</v>
       </c>
       <c r="C2" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="D2" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="E2" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="F2" t="s">
         <v>105</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -5951,19 +6197,19 @@
         <v>107</v>
       </c>
       <c r="C3" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="D3" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="E3" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="F3" t="s">
         <v>105</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -5975,19 +6221,19 @@
         <v>107</v>
       </c>
       <c r="C4" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="D4" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="E4" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="F4" t="s">
         <v>105</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -5999,19 +6245,19 @@
         <v>107</v>
       </c>
       <c r="C5" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="D5" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="E5" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="F5" t="s">
         <v>105</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -6023,19 +6269,19 @@
         <v>107</v>
       </c>
       <c r="C6" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="D6" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="E6" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="F6" t="s">
         <v>105</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -6047,19 +6293,19 @@
         <v>107</v>
       </c>
       <c r="C7" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="D7" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="E7" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="F7" t="s">
         <v>105</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -6071,19 +6317,19 @@
         <v>107</v>
       </c>
       <c r="C8" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="D8" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="E8" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="F8" t="s">
         <v>105</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -6095,19 +6341,19 @@
         <v>107</v>
       </c>
       <c r="C9" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="D9" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="E9" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="F9" t="s">
         <v>105</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -6119,19 +6365,19 @@
         <v>107</v>
       </c>
       <c r="C10" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="D10" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="E10" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="F10" t="s">
         <v>105</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -6143,19 +6389,19 @@
         <v>107</v>
       </c>
       <c r="C11" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="E11" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="F11" t="s">
         <v>105</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -6167,19 +6413,19 @@
         <v>108</v>
       </c>
       <c r="C12" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="D12" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="E12" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="F12" t="s">
         <v>105</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -6191,19 +6437,19 @@
         <v>108</v>
       </c>
       <c r="C13" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="D13" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="E13" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="F13" t="s">
         <v>105</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -6215,19 +6461,19 @@
         <v>108</v>
       </c>
       <c r="C14" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="D14" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="E14" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="F14" t="s">
         <v>105</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -6239,19 +6485,19 @@
         <v>108</v>
       </c>
       <c r="C15" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="D15" t="s">
+        <v>296</v>
+      </c>
+      <c r="E15" t="s">
         <v>304</v>
-      </c>
-      <c r="E15" t="s">
-        <v>312</v>
       </c>
       <c r="F15" t="s">
         <v>105</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -6263,19 +6509,19 @@
         <v>108</v>
       </c>
       <c r="C16" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="D16" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="E16" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="F16" t="s">
         <v>105</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -6287,19 +6533,19 @@
         <v>108</v>
       </c>
       <c r="C17" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="D17" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="E17" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="F17" t="s">
         <v>105</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -6311,19 +6557,19 @@
         <v>108</v>
       </c>
       <c r="C18" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="D18" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="E18" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="F18" t="s">
         <v>105</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -6335,19 +6581,19 @@
         <v>108</v>
       </c>
       <c r="C19" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="D19" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="E19" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="F19" t="s">
         <v>105</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -6359,19 +6605,19 @@
         <v>108</v>
       </c>
       <c r="C20" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="D20" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="E20" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="F20" t="s">
         <v>105</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -6383,19 +6629,19 @@
         <v>108</v>
       </c>
       <c r="C21" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="D21" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="E21" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="F21" t="s">
         <v>105</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -6407,19 +6653,19 @@
         <v>108</v>
       </c>
       <c r="C22" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="D22" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="E22" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="F22" t="s">
         <v>105</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -6431,19 +6677,19 @@
         <v>108</v>
       </c>
       <c r="C23" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="D23" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="E23" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="F23" t="s">
         <v>105</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -6455,19 +6701,19 @@
         <v>108</v>
       </c>
       <c r="C24" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="D24" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="E24" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="F24" t="s">
         <v>105</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -6479,19 +6725,19 @@
         <v>108</v>
       </c>
       <c r="C25" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="D25" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="E25" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="F25" t="s">
         <v>105</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -6503,19 +6749,19 @@
         <v>108</v>
       </c>
       <c r="C26" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="D26" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="E26" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="F26" t="s">
         <v>105</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -6527,19 +6773,19 @@
         <v>110</v>
       </c>
       <c r="C27" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="D27">
         <v>99</v>
       </c>
       <c r="E27" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="F27" t="s">
         <v>106</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -6551,19 +6797,19 @@
         <v>110</v>
       </c>
       <c r="C28" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="D28">
         <v>99</v>
       </c>
       <c r="E28" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="F28" t="s">
         <v>106</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -6575,19 +6821,19 @@
         <v>110</v>
       </c>
       <c r="C29" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="D29">
         <v>99</v>
       </c>
       <c r="E29" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="F29" t="s">
         <v>106</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -6599,19 +6845,19 @@
         <v>110</v>
       </c>
       <c r="C30" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="D30">
         <v>99</v>
       </c>
       <c r="E30" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="F30" t="s">
         <v>106</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -6623,19 +6869,19 @@
         <v>110</v>
       </c>
       <c r="C31" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="D31">
         <v>99</v>
       </c>
       <c r="E31" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="F31" t="s">
         <v>106</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -6647,19 +6893,19 @@
         <v>110</v>
       </c>
       <c r="C32" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="D32">
         <v>99</v>
       </c>
       <c r="E32" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="F32" t="s">
         <v>106</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated event data: proper short descriptions for series events
</commit_message>
<xml_diff>
--- a/data/EventData.xlsx
+++ b/data/EventData.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="449">
   <si>
     <t>Movies</t>
   </si>
@@ -32,13 +32,7 @@
     <t>Series</t>
   </si>
   <si>
-    <t>It's senior year! The gang from 90210 return for a third season of more drama.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> M-Net</t>
-  </si>
-  <si>
-    <t>Winter is coming. Let the Game of Thrones begin.</t>
   </si>
   <si>
     <t xml:space="preserve">Episode 1, S1 </t>
@@ -48,9 +42,6 @@
 </t>
   </si>
   <si>
-    <t>It's time to bid farewell to the Emmy Award-winning family in the season finale.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Episode 1, S3 </t>
   </si>
   <si>
@@ -382,9 +373,6 @@
   </si>
   <si>
     <t>S06E01</t>
-  </si>
-  <si>
-    <t>Has Dexter finally seen the light? Get ready for the most rapturous season yet.</t>
   </si>
   <si>
     <t>RsvGslI_KcM</t>
@@ -1348,6 +1336,42 @@
   </si>
   <si>
     <t>lifestyle_poster10.jpg</t>
+  </si>
+  <si>
+    <t>In the year 2030, Ted Mosby (voiced by Bob Saget) sits his daughter and son down to tell them the story of how he met their mother.
+The story begins in 2005 with Ted (Josh Radnor) as a single, 27-year-old architect living with his two best friends from college; Marshall Eriksen (Jason Segel), a law student, and Lily Aldrin (Alyson Hannigan), a kindergarten teacher, and an aspiring artist. Lily and Marshall have been dating for almost nine years when Marshall finally proposes. Their engagement causes Ted to think about marriage and finding his soul mate, much to the disgust of his self-appointed best friend Barney Stinson (Neil Patrick Harris), whom he met in the restroom at a bar. Barney is a serial womanizer who concocts elaborate con games, usually involving costumes and fake identities, designed to bed women he discards immediately afterward.</t>
+  </si>
+  <si>
+    <t>Two brilliant young physicists, Leonard and Sheldon, are the kind of "beautiful minds" that understand how the universe works (this episode reveals that Sheldon and Leonard have a combined IQ of 360 with Leonard having 173 and Sheldon having 187). But their Ph.Ds don't help them interact with people, especially women. All of this is about to change when a free-spirited newly single beauty named Penny moves in next door. When Leonard and Sheldon meet Penny, Leonard is immediately interested in her (saying their babies will be smart and beautiful), but Sheldon feels his friend is chasing a dream he'll never catch (adding "imaginary").</t>
+  </si>
+  <si>
+    <t>Entourage revolves around Vincent Chase (Adrian Grenier). His best friend and manager is Eric Murphy (Kevin Connolly). "E," as his friends call him, is based on Mark Wahlberg's friend and executive producer Eric Weinstein. He's also been reported to be inspired by Stephen Levinson, Mark Wahlberg's manager.
+Vincent's older half-brother Johnny "Drama" Chase (Kevin Dillon), is Vince's personal chef, trainer and bodyguard. Johnny is a C-list actor who was in the fictional show Viking Quest during his younger days. His role in the new fictional hit show Five Towns has begun to resurrect his fame and career, although he still receives less acknowledgment than he would like for it. This character is based on Johnny "Drama" Alves (cousin of Mark Wahlberg), whom Donnie Wahlberg had hired to keep his younger brother out of trouble.</t>
+  </si>
+  <si>
+    <t>Peter loses his job after drinking too much at a stag party and falls asleep at work. He then signs up for welfare to keep his wife Lois from finding out, but gets much more money than he expected. Lois finds out and Peter decides to dump the money from a blimp at the Super Bowl. He is then arrested, and must await his family's rescue.</t>
+  </si>
+  <si>
+    <t>S06E01 - Death has a shadow</t>
+  </si>
+  <si>
+    <t>Dexter is an American television drama series that centers on Dexter Morgan (Michael C. Hall), a bloodstain pattern analyst for the Miami Metro Police Department who moonlights as a serial killer. The show debuted on October 1, 2006, on Showtime and the sixth season premiered on October 2, 2011. Set in Miami, the show's first season was largely based on the novel Darkly Dreaming Dexter by Jeff Lindsay, the first of his Dexter series novels. Subsequent seasons have evolved independently of Lindsay's works. It was adapted for television by screenwriter James Manos, Jr., who wrote the first episode.</t>
+  </si>
+  <si>
+    <t>Liz Lemon, head writer of the sketch comedy show "TGS with Tracy Jordan", must deal with an arrogant new boss and a crazy new star, all while trying to run a successful TV show without losing her mind.</t>
+  </si>
+  <si>
+    <t>Fringe is an American science fiction television series created by J. J. Abrams, Alex Kurtzman and Roberto Orci. The series follows a Federal Bureau of Investigation "Fringe Division" team based in Boston, Massachusetts under the supervision of Homeland Security. The team uses unorthodox "fringe" science and FBI investigative techniques to investigate a series of unexplained, often ghastly occurrences, which are related to mysteries surrounding a parallel universe.</t>
+  </si>
+  <si>
+    <t>True Blood is an American television series created and produced by Alan Ball. It is based on The Southern Vampire Mysteries series of novels by Charlaine Harris, detailing the co-existence of vampires and humans in Bon Temps, a fictional, small town in the state of Louisiana. The series centers on Sookie Stackhouse (played by actress Anna Paquin), a telepathic waitress who falls in love with vampire Bill Compton (Stephen Moyer).</t>
+  </si>
+  <si>
+    <t>The one-hour series follows an optimistic high school teacher as he tries to transform the school's Glee Club and inspire a group of ragtag performers to make it to the biggest competition of them all: Nationals.
+McKinley High School's Glee Club used to be at the top of the show choir world, but years later, a series of scandals have turned it into a haven for misfits and social outcasts. Will Schuester (Matthew Morrison, Broadway's "Hairspray") has offered to take on the Herculean task of restoring the Glee Club to its former glory.</t>
+  </si>
+  <si>
+    <t>In its war on the Greek peninsula, the Romans convince the Thracians to join them in defeating the Getae, who have been raiding Thracian villages for generations. The Thracians are fierce warriors and prove to be valiant in battle. They are deceived by the Roman commander, Claudius Glaber, who orders them to fight against the Greeks, something they had not counted on. One of them in particular refuses to fight and rebels against the Romans only to lose the fight and is enslaved along with his wife Sura. The Thracian is transported to Capua where Senator Albinius is sponsoring gladiatorial games. In the arena, the enslaved Thracian manages to defeat four opponents and in allowing the Thracian to live, Senator Albinius decides to name him after a Thracian king from the past: Spartacus.</t>
   </si>
 </sst>
 </file>
@@ -1854,22 +1878,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="F1" s="21" t="s">
         <v>57</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1877,19 +1901,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D2" s="19">
         <v>50</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1898,19 +1922,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D3" s="19">
         <v>50</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1919,16 +1943,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D4" s="23">
         <v>100</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F4" s="24"/>
     </row>
@@ -1938,19 +1962,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D5" s="23">
         <v>100</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1959,19 +1983,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D6" s="19">
         <v>50</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1980,19 +2004,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D7" s="23">
         <v>100</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2001,16 +2025,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D8" s="19">
         <v>0</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F8" s="22"/>
     </row>
@@ -2020,17 +2044,17 @@
         <v>8</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D9" s="19">
         <v>50</v>
       </c>
       <c r="E9" s="19"/>
       <c r="F9" s="22" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2039,10 +2063,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D10" s="19">
         <v>50</v>
@@ -2056,17 +2080,17 @@
         <v>10</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D11" s="19">
         <v>50</v>
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="22" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2075,17 +2099,17 @@
         <v>11</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D12" s="19">
         <v>80</v>
       </c>
       <c r="E12" s="19"/>
       <c r="F12" s="22" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2094,17 +2118,17 @@
         <v>12</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D13" s="19">
         <v>80</v>
       </c>
       <c r="E13" s="19"/>
       <c r="F13" s="22" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2113,10 +2137,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D14" s="19">
         <v>80</v>
@@ -2130,16 +2154,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D15" s="19">
         <v>10</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F15" s="22"/>
     </row>
@@ -2149,17 +2173,17 @@
         <v>15</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="19">
         <v>0</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2168,19 +2192,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D17" s="23">
         <v>100</v>
       </c>
       <c r="E17" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="24" t="s">
         <v>64</v>
-      </c>
-      <c r="F17" s="24" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2189,19 +2213,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D18" s="19">
         <v>80</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F18" s="22" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -2210,13 +2234,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2225,19 +2249,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D20" s="28">
         <v>100</v>
       </c>
       <c r="E20" s="28" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F20" s="29" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2268,8 +2292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N35" workbookViewId="0">
-      <selection activeCell="R52" sqref="R52"/>
+    <sheetView tabSelected="1" topLeftCell="C20" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2296,64 +2320,64 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="K1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="N1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="L1" s="11" t="s">
+      <c r="O1" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="P1" t="s">
         <v>40</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" t="s">
         <v>41</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
+        <v>226</v>
+      </c>
+      <c r="S1" t="s">
         <v>42</v>
       </c>
-      <c r="P1" t="s">
+      <c r="T1" t="s">
         <v>43</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>44</v>
-      </c>
-      <c r="R1" t="s">
-        <v>230</v>
-      </c>
-      <c r="S1" t="s">
-        <v>45</v>
-      </c>
-      <c r="T1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="156.75" x14ac:dyDescent="0.25">
@@ -2376,10 +2400,10 @@
         <v>0</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="H2" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I2" s="9">
         <v>40834</v>
@@ -2389,25 +2413,25 @@
       </c>
       <c r="K2" s="4"/>
       <c r="L2" s="12" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="O2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="P2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="Q2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="R2">
         <v>7</v>
       </c>
       <c r="S2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="T2">
         <v>2011</v>
@@ -2434,10 +2458,10 @@
         <v>0</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="H3" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="I3" s="9">
         <v>40834</v>
@@ -2446,25 +2470,25 @@
         <v>1.1041666666666701</v>
       </c>
       <c r="L3" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="N3" t="s">
+        <v>264</v>
+      </c>
+      <c r="O3" t="s">
+        <v>170</v>
+      </c>
+      <c r="P3" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q3" t="s">
         <v>267</v>
-      </c>
-      <c r="N3" t="s">
-        <v>268</v>
-      </c>
-      <c r="O3" t="s">
-        <v>174</v>
-      </c>
-      <c r="P3" t="s">
-        <v>269</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>271</v>
       </c>
       <c r="R3">
         <v>8</v>
       </c>
       <c r="S3" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="T3">
         <v>2011</v>
@@ -2491,7 +2515,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="H4" t="s">
         <v>2</v>
@@ -2503,25 +2527,25 @@
         <v>1.1458333333333299</v>
       </c>
       <c r="L4" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="O4" t="s">
+        <v>171</v>
+      </c>
+      <c r="P4" t="s">
+        <v>271</v>
+      </c>
+      <c r="Q4" t="s">
         <v>273</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="O4" t="s">
-        <v>175</v>
-      </c>
-      <c r="P4" t="s">
-        <v>275</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>277</v>
       </c>
       <c r="R4">
         <v>9</v>
       </c>
       <c r="S4" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="T4">
         <v>2011</v>
@@ -2548,10 +2572,10 @@
         <v>0</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="H5" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I5" s="9">
         <v>40834</v>
@@ -2561,25 +2585,25 @@
       </c>
       <c r="K5" s="4"/>
       <c r="L5" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="O5" t="s">
+        <v>172</v>
+      </c>
+      <c r="P5" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q5" t="s">
         <v>279</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="O5" t="s">
-        <v>176</v>
-      </c>
-      <c r="P5" t="s">
-        <v>281</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>283</v>
       </c>
       <c r="R5">
         <v>6</v>
       </c>
       <c r="S5" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="T5">
         <v>2011</v>
@@ -2606,7 +2630,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="H6" t="s">
         <v>1</v>
@@ -2618,25 +2642,25 @@
         <v>1.2291666666666701</v>
       </c>
       <c r="L6" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="N6" t="s">
+        <v>282</v>
+      </c>
+      <c r="O6" t="s">
+        <v>173</v>
+      </c>
+      <c r="P6" t="s">
+        <v>283</v>
+      </c>
+      <c r="Q6" t="s">
         <v>285</v>
-      </c>
-      <c r="N6" t="s">
-        <v>286</v>
-      </c>
-      <c r="O6" t="s">
-        <v>177</v>
-      </c>
-      <c r="P6" t="s">
-        <v>287</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>289</v>
       </c>
       <c r="R6">
         <v>7</v>
       </c>
       <c r="S6" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="180.75" x14ac:dyDescent="0.25">
@@ -2660,7 +2684,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="H7" t="s">
         <v>1</v>
@@ -2672,25 +2696,25 @@
         <v>0.85416666666666663</v>
       </c>
       <c r="L7" s="12" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="N7" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="O7" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="P7" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="Q7" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="R7">
         <v>8</v>
       </c>
       <c r="S7" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="T7">
         <v>2011</v>
@@ -2717,10 +2741,10 @@
         <v>0</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="H8" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="I8" s="9">
         <v>40834</v>
@@ -2729,25 +2753,25 @@
         <v>0.89583333333333337</v>
       </c>
       <c r="L8" s="12" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="O8" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="P8" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="Q8" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="R8">
         <v>8</v>
       </c>
       <c r="S8" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="T8">
         <v>2011</v>
@@ -2774,10 +2798,10 @@
         <v>0</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="H9" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I9" s="9">
         <v>40834</v>
@@ -2787,25 +2811,25 @@
       </c>
       <c r="K9" s="4"/>
       <c r="L9" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="O9" t="s">
+        <v>166</v>
+      </c>
+      <c r="P9" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q9" t="s">
         <v>242</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="O9" t="s">
-        <v>170</v>
-      </c>
-      <c r="P9" t="s">
-        <v>244</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>246</v>
       </c>
       <c r="R9">
         <v>8</v>
       </c>
       <c r="S9" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="T9">
         <v>2011</v>
@@ -2832,10 +2856,10 @@
         <v>0</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="H10" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="I10" s="9">
         <v>40834</v>
@@ -2844,25 +2868,25 @@
         <v>0.97916666666666696</v>
       </c>
       <c r="L10" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="N10" t="s">
+        <v>246</v>
+      </c>
+      <c r="O10" t="s">
+        <v>167</v>
+      </c>
+      <c r="P10" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q10" t="s">
         <v>249</v>
-      </c>
-      <c r="N10" t="s">
-        <v>250</v>
-      </c>
-      <c r="O10" t="s">
-        <v>171</v>
-      </c>
-      <c r="P10" t="s">
-        <v>251</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>253</v>
       </c>
       <c r="R10">
         <v>9</v>
       </c>
       <c r="S10" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="T10">
         <v>2011</v>
@@ -2889,10 +2913,10 @@
         <v>0</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="H11" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="I11" s="9">
         <v>40834</v>
@@ -2901,31 +2925,31 @@
         <v>1.0208333333333299</v>
       </c>
       <c r="L11" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="O11" t="s">
+        <v>168</v>
+      </c>
+      <c r="P11" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q11" t="s">
         <v>255</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="O11" t="s">
-        <v>172</v>
-      </c>
-      <c r="P11" t="s">
-        <v>257</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>259</v>
       </c>
       <c r="R11">
         <v>9</v>
       </c>
       <c r="S11" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="T11">
         <v>2011</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2946,10 +2970,10 @@
         <v>3</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="H12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I12" s="9">
         <v>40834</v>
@@ -2958,25 +2982,25 @@
         <v>1.2708333333333299</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L12" s="12" t="s">
-        <v>6</v>
+        <v>440</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="O12" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="P12" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="R12">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2997,10 +3021,10 @@
         <v>3</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="H13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I13" s="9">
         <v>40834</v>
@@ -3009,25 +3033,25 @@
         <v>1.3125</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L13" s="12" t="s">
-        <v>9</v>
+        <v>438</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="O13" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="P13" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="R13">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="252.75" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -3048,7 +3072,7 @@
         <v>3</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H14" t="s">
         <v>3</v>
@@ -3060,25 +3084,25 @@
         <v>1.3541666666666701</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>120</v>
+        <v>442</v>
       </c>
       <c r="L14" s="12" t="s">
-        <v>121</v>
+        <v>441</v>
       </c>
       <c r="N14" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="O14" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="P14" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="R14">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -3099,10 +3123,10 @@
         <v>3</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H15" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I15" s="9">
         <v>40834</v>
@@ -3111,25 +3135,25 @@
         <v>1.3958333333333299</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L15" s="12" t="s">
-        <v>4</v>
+        <v>443</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="O15" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="P15" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="R15">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="156.75" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -3150,10 +3174,10 @@
         <v>3</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="H16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I16" s="9">
         <v>40834</v>
@@ -3162,25 +3186,25 @@
         <v>1.4375</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L16" s="12" t="s">
-        <v>6</v>
+        <v>444</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="O16" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="P16" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="R16">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -3201,10 +3225,10 @@
         <v>3</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="H17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I17" s="9">
         <v>40834</v>
@@ -3213,25 +3237,25 @@
         <v>1.4791666666666701</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L17" s="12" t="s">
-        <v>9</v>
+        <v>439</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="O17" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="P17" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="R17">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" ht="384.75" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -3252,7 +3276,7 @@
         <v>3</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="H18" t="s">
         <v>3</v>
@@ -3264,25 +3288,25 @@
         <v>1.5208333333333299</v>
       </c>
       <c r="K18" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="L18" s="12" t="s">
-        <v>121</v>
+        <v>445</v>
       </c>
       <c r="N18" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="O18" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="P18" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="R18">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" ht="336.75" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -3303,10 +3327,10 @@
         <v>3</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="H19" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I19" s="9">
         <v>40834</v>
@@ -3315,25 +3339,25 @@
         <v>1.5625</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L19" s="12" t="s">
-        <v>4</v>
+        <v>446</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="O19" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="P19" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="R19">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -3354,7 +3378,7 @@
         <v>3</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H20" t="s">
         <v>3</v>
@@ -3366,25 +3390,25 @@
         <v>1.6041666666666701</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="L20" s="12" t="s">
-        <v>121</v>
+        <v>447</v>
       </c>
       <c r="N20" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="O20" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="P20" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="R20">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -3405,10 +3429,10 @@
         <v>3</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="H21" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I21" s="9">
         <v>40834</v>
@@ -3417,19 +3441,19 @@
         <v>1.6458333333333299</v>
       </c>
       <c r="K21" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L21" s="12" t="s">
-        <v>4</v>
+        <v>448</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="O21" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="P21" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="R21">
         <v>9</v>
@@ -3450,16 +3474,16 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F22" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H22" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I22" s="9">
         <v>40834</v>
@@ -3468,16 +3492,16 @@
         <v>1.6875</v>
       </c>
       <c r="L22" s="12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="O22" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="P22" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="R22">
         <v>7</v>
@@ -3498,16 +3522,16 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F23" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H23" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I23" s="9">
         <v>40834</v>
@@ -3516,16 +3540,16 @@
         <v>1.7291666666666701</v>
       </c>
       <c r="L23" s="12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="N23" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="O23" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="P23" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="R23">
         <v>8</v>
@@ -3546,16 +3570,16 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F24" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H24" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I24" s="9">
         <v>40834</v>
@@ -3564,16 +3588,16 @@
         <v>1.7708333333333299</v>
       </c>
       <c r="L24" s="12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="N24" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="O24" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="P24" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="R24">
         <v>9</v>
@@ -3594,16 +3618,16 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F25" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H25" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I25" s="9">
         <v>40834</v>
@@ -3612,16 +3636,16 @@
         <v>1.8125</v>
       </c>
       <c r="L25" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N25" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="O25" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="P25" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="R25">
         <v>8</v>
@@ -3642,16 +3666,16 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H26" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I26" s="9">
         <v>40834</v>
@@ -3660,16 +3684,16 @@
         <v>1.8541666666666701</v>
       </c>
       <c r="L26" s="12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="O26" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="P26" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="R26">
         <v>9</v>
@@ -3690,16 +3714,16 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F27" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H27" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I27" s="9">
         <v>40834</v>
@@ -3708,16 +3732,16 @@
         <v>1.8958333333333299</v>
       </c>
       <c r="L27" s="12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="N27" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="O27" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="P27" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="R27">
         <v>8</v>
@@ -3738,16 +3762,16 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F28" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="H28" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I28" s="9">
         <v>40834</v>
@@ -3756,16 +3780,16 @@
         <v>1.9375</v>
       </c>
       <c r="L28" s="12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="N28" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="O28" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="P28" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="R28">
         <v>9</v>
@@ -3786,16 +3810,16 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F29" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H29" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I29" s="9">
         <v>40834</v>
@@ -3804,16 +3828,16 @@
         <v>1.9791666666666701</v>
       </c>
       <c r="L29" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N29" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="O29" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="P29" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="R29">
         <v>9</v>
@@ -3834,16 +3858,16 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F30" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I30" s="9">
         <v>40834</v>
@@ -3852,16 +3876,16 @@
         <v>2.0208333333333299</v>
       </c>
       <c r="L30" s="12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="N30" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="O30" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="P30" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="R30">
         <v>9</v>
@@ -3882,16 +3906,16 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F31" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="H31" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I31" s="9">
         <v>40834</v>
@@ -3900,16 +3924,16 @@
         <v>2.0625</v>
       </c>
       <c r="L31" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N31" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="O31" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="P31" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="R31">
         <v>7</v>
@@ -3930,16 +3954,16 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F32" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="H32" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="I32" s="9">
         <v>40834</v>
@@ -3948,16 +3972,16 @@
         <v>2.1041666666666701</v>
       </c>
       <c r="L32" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N32" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="O32" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="P32" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="R32">
         <v>6</v>
@@ -3978,16 +4002,16 @@
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F33" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="H33" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="I33" s="9">
         <v>40834</v>
@@ -3996,16 +4020,16 @@
         <v>2.1458333333333299</v>
       </c>
       <c r="L33" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N33" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="O33" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="P33" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="R33">
         <v>7</v>
@@ -4026,16 +4050,16 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F34" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="H34" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="I34" s="9">
         <v>40834</v>
@@ -4044,16 +4068,16 @@
         <v>2.1875</v>
       </c>
       <c r="L34" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N34" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="O34" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="P34" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="R34">
         <v>6</v>
@@ -4074,16 +4098,16 @@
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F35" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="H35" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="I35" s="9">
         <v>40834</v>
@@ -4092,16 +4116,16 @@
         <v>2.2291666666666701</v>
       </c>
       <c r="L35" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N35" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="O35" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="P35" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="R35">
         <v>7</v>
@@ -4122,16 +4146,16 @@
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F36" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="H36" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="I36" s="9">
         <v>40834</v>
@@ -4140,16 +4164,16 @@
         <v>2.2708333333333299</v>
       </c>
       <c r="L36" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N36" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="O36" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="P36" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="R36">
         <v>8</v>
@@ -4170,16 +4194,16 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="H37" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="I37" s="9">
         <v>40834</v>
@@ -4188,16 +4212,16 @@
         <v>2.3125</v>
       </c>
       <c r="L37" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N37" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="O37" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="P37" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="R37">
         <v>6</v>
@@ -4218,16 +4242,16 @@
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F38" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="H38" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="I38" s="9">
         <v>40834</v>
@@ -4236,16 +4260,16 @@
         <v>2.3541666666666701</v>
       </c>
       <c r="L38" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N38" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="O38" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="P38" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="R38">
         <v>5</v>
@@ -4266,16 +4290,16 @@
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F39" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="H39" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="I39" s="9">
         <v>40834</v>
@@ -4284,16 +4308,16 @@
         <v>2.3958333333333299</v>
       </c>
       <c r="L39" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N39" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="O39" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="P39" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="R39">
         <v>8</v>
@@ -4314,16 +4338,16 @@
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F40" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H40" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="I40" s="9">
         <v>40834</v>
@@ -4332,16 +4356,16 @@
         <v>2.4375</v>
       </c>
       <c r="L40" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N40" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="O40" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="P40" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="R40">
         <v>7</v>
@@ -4362,16 +4386,16 @@
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F41" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="H41" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="I41" s="9">
         <v>40834</v>
@@ -4380,16 +4404,16 @@
         <v>2.4791666666666701</v>
       </c>
       <c r="L41" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N41" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="O41" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="P41" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="R41">
         <v>9</v>
@@ -4410,16 +4434,16 @@
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F42" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="H42" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="I42" s="9">
         <v>40834</v>
@@ -4428,16 +4452,16 @@
         <v>2.5208333333333299</v>
       </c>
       <c r="L42" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N42" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="O42" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="P42" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="R42">
         <v>6</v>
@@ -4458,16 +4482,16 @@
         <v>1</v>
       </c>
       <c r="E43" t="s">
+        <v>184</v>
+      </c>
+      <c r="F43" t="s">
+        <v>184</v>
+      </c>
+      <c r="G43" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="F43" t="s">
-        <v>188</v>
-      </c>
-      <c r="G43" s="6" t="s">
-        <v>192</v>
-      </c>
       <c r="H43" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="I43" s="9">
         <v>40834</v>
@@ -4476,16 +4500,16 @@
         <v>2.5625</v>
       </c>
       <c r="L43" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N43" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="O43" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="P43" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="R43">
         <v>7</v>
@@ -4506,16 +4530,16 @@
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F44" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="H44" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="I44" s="9">
         <v>40834</v>
@@ -4524,16 +4548,16 @@
         <v>2.6041666666666701</v>
       </c>
       <c r="L44" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N44" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="O44" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="P44" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="R44">
         <v>9</v>
@@ -4554,16 +4578,16 @@
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F45" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="H45" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="I45" s="9">
         <v>40834</v>
@@ -4572,16 +4596,16 @@
         <v>2.6458333333333299</v>
       </c>
       <c r="L45" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N45" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="O45" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="P45" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="R45">
         <v>7</v>
@@ -4602,16 +4626,16 @@
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F46" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="H46" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="I46" s="9">
         <v>40834</v>
@@ -4620,16 +4644,16 @@
         <v>2.6875</v>
       </c>
       <c r="L46" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N46" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="O46" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="P46" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="R46">
         <v>9</v>
@@ -4650,16 +4674,16 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F47" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="H47" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="I47" s="9">
         <v>40834</v>
@@ -4668,16 +4692,16 @@
         <v>2.7291666666666701</v>
       </c>
       <c r="L47" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N47" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="O47" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="P47" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="R47">
         <v>6</v>
@@ -4698,16 +4722,16 @@
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F48" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="H48" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="I48" s="9">
         <v>40834</v>
@@ -4716,16 +4740,16 @@
         <v>2.7708333333333299</v>
       </c>
       <c r="L48" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N48" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="O48" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="P48" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="R48">
         <v>7</v>
@@ -4746,16 +4770,16 @@
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F49" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="H49" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="I49" s="9">
         <v>40834</v>
@@ -4764,16 +4788,16 @@
         <v>2.8125</v>
       </c>
       <c r="L49" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N49" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="O49" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="P49" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="R49">
         <v>8</v>
@@ -4794,16 +4818,16 @@
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F50" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="H50" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="I50" s="9">
         <v>40834</v>
@@ -4812,16 +4836,16 @@
         <v>2.8541666666666701</v>
       </c>
       <c r="L50" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N50" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="O50" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="P50" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="R50">
         <v>6</v>
@@ -4842,16 +4866,16 @@
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F51" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="H51" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="I51" s="9">
         <v>40834</v>
@@ -4860,16 +4884,16 @@
         <v>2.8958333333333299</v>
       </c>
       <c r="L51" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N51" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="O51" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="P51" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="R51">
         <v>8</v>
@@ -4902,37 +4926,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>79</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>80</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>81</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>82</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>83</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>84</v>
-      </c>
-      <c r="I1" t="s">
-        <v>85</v>
-      </c>
-      <c r="J1" t="s">
-        <v>86</v>
-      </c>
-      <c r="K1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -5762,37 +5786,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" t="s">
         <v>88</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>89</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>90</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>91</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>92</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>93</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>94</v>
-      </c>
-      <c r="I1" t="s">
-        <v>95</v>
-      </c>
-      <c r="J1" t="s">
-        <v>96</v>
-      </c>
-      <c r="K1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -6144,25 +6168,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G1" t="s">
         <v>98</v>
-      </c>
-      <c r="C1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -6170,22 +6194,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C2" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="D2" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E2" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="F2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -6194,22 +6218,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C3" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="D3" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="E3" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="F3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -6218,22 +6242,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C4" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D4" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="E4" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="F4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -6242,22 +6266,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C5" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="D5" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="E5" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="F5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -6266,22 +6290,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C6" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="D6" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="E6" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="F6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -6290,22 +6314,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C7" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="D7" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="E7" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="F7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -6314,22 +6338,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C8" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D8" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E8" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="F8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -6338,22 +6362,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C9" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="D9" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E9" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F9" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -6362,22 +6386,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C10" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="D10" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="E10" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="F10" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -6386,22 +6410,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C11" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="E11" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="F11" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -6410,22 +6434,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C12" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D12" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="E12" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="F12" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -6434,22 +6458,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C13" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D13" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="E13" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="F13" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -6458,22 +6482,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C14" t="s">
+        <v>295</v>
+      </c>
+      <c r="D14" t="s">
+        <v>292</v>
+      </c>
+      <c r="E14" t="s">
         <v>299</v>
       </c>
-      <c r="D14" t="s">
-        <v>296</v>
-      </c>
-      <c r="E14" t="s">
-        <v>303</v>
-      </c>
       <c r="F14" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -6482,22 +6506,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C15" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D15" t="s">
+        <v>292</v>
+      </c>
+      <c r="E15" t="s">
+        <v>300</v>
+      </c>
+      <c r="F15" t="s">
+        <v>102</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>296</v>
-      </c>
-      <c r="E15" t="s">
-        <v>304</v>
-      </c>
-      <c r="F15" t="s">
-        <v>105</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -6506,22 +6530,22 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C16" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D16" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="E16" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="F16" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -6530,22 +6554,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C17" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D17" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="E17" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="F17" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -6554,22 +6578,22 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C18" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="D18" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="E18" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="F18" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -6578,22 +6602,22 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C19" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="D19" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="E19" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="F19" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -6602,22 +6626,22 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C20" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="D20" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="E20" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="F20" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -6626,22 +6650,22 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C21" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D21" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="E21" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="F21" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -6650,22 +6674,22 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C22" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="D22" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E22" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="F22" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -6674,22 +6698,22 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C23" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="D23" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="E23" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F23" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -6698,22 +6722,22 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C24" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D24" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E24" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="F24" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -6722,22 +6746,22 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C25" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="D25" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="E25" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="F25" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -6746,22 +6770,22 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C26" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="D26" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="E26" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="F26" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -6770,22 +6794,22 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C27" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="D27">
         <v>99</v>
       </c>
       <c r="E27" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="F27" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -6794,22 +6818,22 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C28" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D28">
         <v>99</v>
       </c>
       <c r="E28" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="F28" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -6818,22 +6842,22 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C29" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="D29">
         <v>99</v>
       </c>
       <c r="E29" t="s">
+        <v>383</v>
+      </c>
+      <c r="F29" t="s">
+        <v>103</v>
+      </c>
+      <c r="G29" s="2" t="s">
         <v>387</v>
-      </c>
-      <c r="F29" t="s">
-        <v>106</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -6842,22 +6866,22 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C30" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="D30">
         <v>99</v>
       </c>
       <c r="E30" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="F30" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -6866,22 +6890,22 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C31" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="D31">
         <v>99</v>
       </c>
       <c r="E31" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="F31" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -6890,22 +6914,22 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C32" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="D32">
         <v>99</v>
       </c>
       <c r="E32" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="F32" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed errors with SQLite db
1. Only open/close the db from the main activity. Reuse the myDBHelper in
all fragments.
2. Updated the sports images and database
</commit_message>
<xml_diff>
--- a/data/EventData.xlsx
+++ b/data/EventData.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="458">
   <si>
     <t>Movies</t>
   </si>
@@ -414,9 +414,6 @@
     <t>2hMCycsef8A</t>
   </si>
   <si>
-    <t>Man U vs Chelsea</t>
-  </si>
-  <si>
     <t>Football</t>
   </si>
   <si>
@@ -481,36 +478,6 @@
   </si>
   <si>
     <t>series10.jpg</t>
-  </si>
-  <si>
-    <t>sport01.jpg</t>
-  </si>
-  <si>
-    <t>sport02.jpg</t>
-  </si>
-  <si>
-    <t>sport03.jpg</t>
-  </si>
-  <si>
-    <t>sport04.jpg</t>
-  </si>
-  <si>
-    <t>sport05.jpg</t>
-  </si>
-  <si>
-    <t>sport06.jpg</t>
-  </si>
-  <si>
-    <t>sport07.jpg</t>
-  </si>
-  <si>
-    <t>sport08.jpg</t>
-  </si>
-  <si>
-    <t>sport09.jpg</t>
-  </si>
-  <si>
-    <t>sport10.jpg</t>
   </si>
   <si>
     <t>movies01.jpg</t>
@@ -1372,6 +1339,66 @@
   </si>
   <si>
     <t>In its war on the Greek peninsula, the Romans convince the Thracians to join them in defeating the Getae, who have been raiding Thracian villages for generations. The Thracians are fierce warriors and prove to be valiant in battle. They are deceived by the Roman commander, Claudius Glaber, who orders them to fight against the Greeks, something they had not counted on. One of them in particular refuses to fight and rebels against the Romans only to lose the fight and is enslaved along with his wife Sura. The Thracian is transported to Capua where Senator Albinius is sponsoring gladiatorial games. In the arena, the enslaved Thracian manages to defeat four opponents and in allowing the Thracian to live, Senator Albinius decides to name him after a Thracian king from the past: Spartacus.</t>
+  </si>
+  <si>
+    <t>Djokovic vs Nadal</t>
+  </si>
+  <si>
+    <t>US Open Final</t>
+  </si>
+  <si>
+    <t>Everton vs Totenham</t>
+  </si>
+  <si>
+    <t>Man United vs Chelsea</t>
+  </si>
+  <si>
+    <t>South Africa vs Australia</t>
+  </si>
+  <si>
+    <t>Tennis</t>
+  </si>
+  <si>
+    <t>Manchester United vs Chelsea in a premiership showdown</t>
+  </si>
+  <si>
+    <t>Everton and Totenham in a premiership showdown</t>
+  </si>
+  <si>
+    <t>Australia tour to South Africa.</t>
+  </si>
+  <si>
+    <t>Rugby world cup qualifying round</t>
+  </si>
+  <si>
+    <t>sport01.png</t>
+  </si>
+  <si>
+    <t>sport02.png</t>
+  </si>
+  <si>
+    <t>sport04.png</t>
+  </si>
+  <si>
+    <t>sport05.png</t>
+  </si>
+  <si>
+    <t>sport06.png</t>
+  </si>
+  <si>
+    <t>sport07.png</t>
+  </si>
+  <si>
+    <t>sport08.png</t>
+  </si>
+  <si>
+    <t>sport09.png</t>
+  </si>
+  <si>
+    <t>sport10.png</t>
+  </si>
+  <si>
+    <t>sport03.png</t>
   </si>
 </sst>
 </file>
@@ -1974,7 +2001,7 @@
         <v>61</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1983,7 +2010,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>29</v>
@@ -2054,7 +2081,7 @@
       </c>
       <c r="E9" s="19"/>
       <c r="F9" s="22" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2163,7 +2190,7 @@
         <v>10</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="F15" s="22"/>
     </row>
@@ -2292,8 +2319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C20" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2371,7 +2398,7 @@
         <v>41</v>
       </c>
       <c r="R1" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="S1" t="s">
         <v>42</v>
@@ -2400,10 +2427,10 @@
         <v>0</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="H2" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="I2" s="9">
         <v>40834</v>
@@ -2413,25 +2440,25 @@
       </c>
       <c r="K2" s="4"/>
       <c r="L2" s="12" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="O2" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="P2" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="Q2" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="R2">
         <v>7</v>
       </c>
       <c r="S2" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="T2">
         <v>2011</v>
@@ -2458,10 +2485,10 @@
         <v>0</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="H3" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="I3" s="9">
         <v>40834</v>
@@ -2470,25 +2497,25 @@
         <v>1.1041666666666701</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="N3" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="O3" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="P3" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="Q3" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="R3">
         <v>8</v>
       </c>
       <c r="S3" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="T3">
         <v>2011</v>
@@ -2515,7 +2542,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="H4" t="s">
         <v>2</v>
@@ -2527,25 +2554,25 @@
         <v>1.1458333333333299</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="O4" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="P4" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="Q4" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="R4">
         <v>9</v>
       </c>
       <c r="S4" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="T4">
         <v>2011</v>
@@ -2572,10 +2599,10 @@
         <v>0</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="H5" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="I5" s="9">
         <v>40834</v>
@@ -2585,25 +2612,25 @@
       </c>
       <c r="K5" s="4"/>
       <c r="L5" s="12" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="O5" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="P5" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="Q5" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="R5">
         <v>6</v>
       </c>
       <c r="S5" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="T5">
         <v>2011</v>
@@ -2630,7 +2657,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="H6" t="s">
         <v>1</v>
@@ -2642,25 +2669,25 @@
         <v>1.2291666666666701</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="N6" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="O6" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="P6" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="Q6" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="R6">
         <v>7</v>
       </c>
       <c r="S6" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="180.75" x14ac:dyDescent="0.25">
@@ -2684,7 +2711,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="H7" t="s">
         <v>1</v>
@@ -2696,25 +2723,25 @@
         <v>0.85416666666666663</v>
       </c>
       <c r="L7" s="12" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="N7" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="O7" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="P7" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="Q7" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="R7">
         <v>8</v>
       </c>
       <c r="S7" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="T7">
         <v>2011</v>
@@ -2741,10 +2768,10 @@
         <v>0</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="H8" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="I8" s="9">
         <v>40834</v>
@@ -2753,25 +2780,25 @@
         <v>0.89583333333333337</v>
       </c>
       <c r="L8" s="12" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="O8" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="P8" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="Q8" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="R8">
         <v>8</v>
       </c>
       <c r="S8" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="T8">
         <v>2011</v>
@@ -2798,10 +2825,10 @@
         <v>0</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="H9" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="I9" s="9">
         <v>40834</v>
@@ -2811,25 +2838,25 @@
       </c>
       <c r="K9" s="4"/>
       <c r="L9" s="12" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="O9" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="P9" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="Q9" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="R9">
         <v>8</v>
       </c>
       <c r="S9" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="T9">
         <v>2011</v>
@@ -2856,10 +2883,10 @@
         <v>0</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="H10" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="I10" s="9">
         <v>40834</v>
@@ -2868,25 +2895,25 @@
         <v>0.97916666666666696</v>
       </c>
       <c r="L10" s="12" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="N10" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="O10" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="P10" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="Q10" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="R10">
         <v>9</v>
       </c>
       <c r="S10" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="T10">
         <v>2011</v>
@@ -2913,10 +2940,10 @@
         <v>0</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="H11" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="I11" s="9">
         <v>40834</v>
@@ -2925,25 +2952,25 @@
         <v>1.0208333333333299</v>
       </c>
       <c r="L11" s="12" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="O11" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="P11" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="Q11" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="R11">
         <v>9</v>
       </c>
       <c r="S11" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="T11">
         <v>2011</v>
@@ -2985,7 +3012,7 @@
         <v>5</v>
       </c>
       <c r="L12" s="12" t="s">
-        <v>440</v>
+        <v>429</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>119</v>
@@ -2994,7 +3021,7 @@
         <v>127</v>
       </c>
       <c r="P12" t="s">
-        <v>398</v>
+        <v>387</v>
       </c>
       <c r="R12">
         <v>6</v>
@@ -3021,7 +3048,7 @@
         <v>3</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H13" t="s">
         <v>4</v>
@@ -3036,16 +3063,16 @@
         <v>6</v>
       </c>
       <c r="L13" s="12" t="s">
-        <v>438</v>
+        <v>427</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>120</v>
       </c>
       <c r="O13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="P13" t="s">
-        <v>399</v>
+        <v>388</v>
       </c>
       <c r="R13">
         <v>7</v>
@@ -3072,7 +3099,7 @@
         <v>3</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H14" t="s">
         <v>3</v>
@@ -3084,19 +3111,19 @@
         <v>1.3541666666666701</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>442</v>
+        <v>431</v>
       </c>
       <c r="L14" s="12" t="s">
-        <v>441</v>
+        <v>430</v>
       </c>
       <c r="N14" t="s">
         <v>118</v>
       </c>
       <c r="O14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="P14" t="s">
-        <v>400</v>
+        <v>389</v>
       </c>
       <c r="R14">
         <v>6</v>
@@ -3138,16 +3165,16 @@
         <v>7</v>
       </c>
       <c r="L15" s="12" t="s">
-        <v>443</v>
+        <v>432</v>
       </c>
       <c r="N15" s="2" t="s">
         <v>121</v>
       </c>
       <c r="O15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P15" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
       <c r="R15">
         <v>7</v>
@@ -3174,7 +3201,7 @@
         <v>3</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H16" t="s">
         <v>4</v>
@@ -3189,16 +3216,16 @@
         <v>5</v>
       </c>
       <c r="L16" s="12" t="s">
-        <v>444</v>
+        <v>433</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>119</v>
       </c>
       <c r="O16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P16" t="s">
-        <v>402</v>
+        <v>391</v>
       </c>
       <c r="R16">
         <v>6</v>
@@ -3225,7 +3252,7 @@
         <v>3</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H17" t="s">
         <v>4</v>
@@ -3240,16 +3267,16 @@
         <v>6</v>
       </c>
       <c r="L17" s="12" t="s">
-        <v>439</v>
+        <v>428</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>120</v>
       </c>
       <c r="O17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="P17" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
       <c r="R17">
         <v>7</v>
@@ -3276,7 +3303,7 @@
         <v>3</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H18" t="s">
         <v>3</v>
@@ -3291,16 +3318,16 @@
         <v>117</v>
       </c>
       <c r="L18" s="12" t="s">
-        <v>445</v>
+        <v>434</v>
       </c>
       <c r="N18" t="s">
         <v>118</v>
       </c>
       <c r="O18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P18" t="s">
-        <v>404</v>
+        <v>393</v>
       </c>
       <c r="R18">
         <v>8</v>
@@ -3327,7 +3354,7 @@
         <v>3</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H19" t="s">
         <v>8</v>
@@ -3342,16 +3369,16 @@
         <v>7</v>
       </c>
       <c r="L19" s="12" t="s">
-        <v>446</v>
+        <v>435</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>121</v>
       </c>
       <c r="O19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P19" t="s">
-        <v>405</v>
+        <v>394</v>
       </c>
       <c r="R19">
         <v>7</v>
@@ -3378,7 +3405,7 @@
         <v>3</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H20" t="s">
         <v>3</v>
@@ -3393,16 +3420,16 @@
         <v>117</v>
       </c>
       <c r="L20" s="12" t="s">
-        <v>447</v>
+        <v>436</v>
       </c>
       <c r="N20" t="s">
         <v>118</v>
       </c>
       <c r="O20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P20" t="s">
-        <v>406</v>
+        <v>395</v>
       </c>
       <c r="R20">
         <v>8</v>
@@ -3429,7 +3456,7 @@
         <v>3</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H21" t="s">
         <v>8</v>
@@ -3444,16 +3471,16 @@
         <v>5</v>
       </c>
       <c r="L21" s="12" t="s">
-        <v>448</v>
+        <v>437</v>
       </c>
       <c r="N21" s="2" t="s">
         <v>121</v>
       </c>
       <c r="O21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P21" t="s">
-        <v>407</v>
+        <v>396</v>
       </c>
       <c r="R21">
         <v>9</v>
@@ -3477,7 +3504,7 @@
         <v>9</v>
       </c>
       <c r="F22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>10</v>
@@ -3498,10 +3525,10 @@
         <v>122</v>
       </c>
       <c r="O22" t="s">
-        <v>154</v>
+        <v>448</v>
       </c>
       <c r="P22" t="s">
-        <v>408</v>
+        <v>397</v>
       </c>
       <c r="R22">
         <v>7</v>
@@ -3525,7 +3552,7 @@
         <v>9</v>
       </c>
       <c r="F23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>13</v>
@@ -3546,10 +3573,10 @@
         <v>123</v>
       </c>
       <c r="O23" t="s">
-        <v>155</v>
+        <v>449</v>
       </c>
       <c r="P23" t="s">
-        <v>416</v>
+        <v>405</v>
       </c>
       <c r="R23">
         <v>8</v>
@@ -3573,7 +3600,7 @@
         <v>9</v>
       </c>
       <c r="F24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>17</v>
@@ -3594,10 +3621,10 @@
         <v>124</v>
       </c>
       <c r="O24" t="s">
-        <v>156</v>
+        <v>457</v>
       </c>
       <c r="P24" t="s">
-        <v>417</v>
+        <v>406</v>
       </c>
       <c r="R24">
         <v>9</v>
@@ -3621,7 +3648,7 @@
         <v>9</v>
       </c>
       <c r="F25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>19</v>
@@ -3642,16 +3669,16 @@
         <v>125</v>
       </c>
       <c r="O25" t="s">
-        <v>157</v>
+        <v>450</v>
       </c>
       <c r="P25" t="s">
-        <v>415</v>
+        <v>404</v>
       </c>
       <c r="R25">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="72.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -3669,10 +3696,10 @@
         <v>9</v>
       </c>
       <c r="F26" t="s">
-        <v>9</v>
+        <v>443</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>10</v>
+        <v>438</v>
       </c>
       <c r="H26" t="s">
         <v>11</v>
@@ -3684,22 +3711,22 @@
         <v>1.8541666666666701</v>
       </c>
       <c r="L26" s="12" t="s">
-        <v>12</v>
+        <v>439</v>
       </c>
       <c r="N26" s="2" t="s">
         <v>130</v>
       </c>
       <c r="O26" t="s">
-        <v>158</v>
+        <v>451</v>
       </c>
       <c r="P26" t="s">
-        <v>414</v>
+        <v>403</v>
       </c>
       <c r="R26">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -3717,10 +3744,10 @@
         <v>9</v>
       </c>
       <c r="F27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>13</v>
+        <v>440</v>
       </c>
       <c r="H27" t="s">
         <v>14</v>
@@ -3732,22 +3759,22 @@
         <v>1.8958333333333299</v>
       </c>
       <c r="L27" s="12" t="s">
-        <v>15</v>
+        <v>445</v>
       </c>
       <c r="N27" t="s">
         <v>130</v>
       </c>
       <c r="O27" t="s">
-        <v>159</v>
+        <v>452</v>
       </c>
       <c r="P27" t="s">
-        <v>413</v>
+        <v>402</v>
       </c>
       <c r="R27">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="72.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -3765,10 +3792,10 @@
         <v>9</v>
       </c>
       <c r="F28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>131</v>
+        <v>441</v>
       </c>
       <c r="H28" t="s">
         <v>18</v>
@@ -3780,22 +3807,22 @@
         <v>1.9375</v>
       </c>
       <c r="L28" s="12" t="s">
-        <v>16</v>
+        <v>444</v>
       </c>
       <c r="N28" t="s">
         <v>130</v>
       </c>
       <c r="O28" t="s">
-        <v>160</v>
+        <v>453</v>
       </c>
       <c r="P28" t="s">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="R28">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -3816,7 +3843,7 @@
         <v>133</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>19</v>
+        <v>442</v>
       </c>
       <c r="H29" t="s">
         <v>11</v>
@@ -3828,16 +3855,16 @@
         <v>1.9791666666666701</v>
       </c>
       <c r="L29" s="12" t="s">
-        <v>20</v>
+        <v>446</v>
       </c>
       <c r="N29" t="s">
         <v>130</v>
       </c>
       <c r="O29" t="s">
-        <v>161</v>
+        <v>454</v>
       </c>
       <c r="P29" t="s">
-        <v>411</v>
+        <v>400</v>
       </c>
       <c r="R29">
         <v>9</v>
@@ -3861,10 +3888,10 @@
         <v>9</v>
       </c>
       <c r="F30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H30" t="s">
         <v>18</v>
@@ -3882,16 +3909,16 @@
         <v>130</v>
       </c>
       <c r="O30" t="s">
-        <v>162</v>
+        <v>455</v>
       </c>
       <c r="P30" t="s">
-        <v>410</v>
+        <v>399</v>
       </c>
       <c r="R30">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -3909,10 +3936,10 @@
         <v>9</v>
       </c>
       <c r="F31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H31" t="s">
         <v>11</v>
@@ -3924,16 +3951,16 @@
         <v>2.0625</v>
       </c>
       <c r="L31" s="12" t="s">
-        <v>20</v>
+        <v>447</v>
       </c>
       <c r="N31" t="s">
         <v>130</v>
       </c>
       <c r="O31" t="s">
-        <v>163</v>
+        <v>456</v>
       </c>
       <c r="P31" t="s">
-        <v>409</v>
+        <v>398</v>
       </c>
       <c r="R31">
         <v>7</v>
@@ -3960,10 +3987,10 @@
         <v>106</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="H32" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="I32" s="9">
         <v>40834</v>
@@ -3978,10 +4005,10 @@
         <v>129</v>
       </c>
       <c r="O32" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="P32" t="s">
-        <v>418</v>
+        <v>407</v>
       </c>
       <c r="R32">
         <v>6</v>
@@ -4008,10 +4035,10 @@
         <v>106</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="H33" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="I33" s="9">
         <v>40834</v>
@@ -4026,10 +4053,10 @@
         <v>129</v>
       </c>
       <c r="O33" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="P33" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
       <c r="R33">
         <v>7</v>
@@ -4056,10 +4083,10 @@
         <v>106</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="H34" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="I34" s="9">
         <v>40834</v>
@@ -4074,10 +4101,10 @@
         <v>129</v>
       </c>
       <c r="O34" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="P34" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
       <c r="R34">
         <v>6</v>
@@ -4104,10 +4131,10 @@
         <v>106</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="H35" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="I35" s="9">
         <v>40834</v>
@@ -4122,10 +4149,10 @@
         <v>129</v>
       </c>
       <c r="O35" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="P35" t="s">
-        <v>421</v>
+        <v>410</v>
       </c>
       <c r="R35">
         <v>7</v>
@@ -4152,7 +4179,7 @@
         <v>106</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="H36" t="s">
         <v>128</v>
@@ -4170,10 +4197,10 @@
         <v>129</v>
       </c>
       <c r="O36" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="P36" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
       <c r="R36">
         <v>8</v>
@@ -4200,7 +4227,7 @@
         <v>106</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="H37" t="s">
         <v>128</v>
@@ -4218,10 +4245,10 @@
         <v>129</v>
       </c>
       <c r="O37" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="P37" t="s">
-        <v>423</v>
+        <v>412</v>
       </c>
       <c r="R37">
         <v>6</v>
@@ -4248,7 +4275,7 @@
         <v>106</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="H38" t="s">
         <v>128</v>
@@ -4266,10 +4293,10 @@
         <v>129</v>
       </c>
       <c r="O38" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="P38" t="s">
-        <v>424</v>
+        <v>413</v>
       </c>
       <c r="R38">
         <v>5</v>
@@ -4296,7 +4323,7 @@
         <v>106</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="H39" t="s">
         <v>128</v>
@@ -4314,10 +4341,10 @@
         <v>129</v>
       </c>
       <c r="O39" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="P39" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="R39">
         <v>8</v>
@@ -4344,7 +4371,7 @@
         <v>106</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="H40" t="s">
         <v>128</v>
@@ -4362,10 +4389,10 @@
         <v>129</v>
       </c>
       <c r="O40" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="P40" t="s">
-        <v>426</v>
+        <v>415</v>
       </c>
       <c r="R40">
         <v>7</v>
@@ -4392,7 +4419,7 @@
         <v>106</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="H41" t="s">
         <v>128</v>
@@ -4410,10 +4437,10 @@
         <v>129</v>
       </c>
       <c r="O41" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="P41" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
       <c r="R41">
         <v>9</v>
@@ -4434,16 +4461,16 @@
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="F42" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="H42" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="I42" s="9">
         <v>40834</v>
@@ -4458,10 +4485,10 @@
         <v>125</v>
       </c>
       <c r="O42" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="P42" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="R42">
         <v>6</v>
@@ -4482,16 +4509,16 @@
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="F43" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="H43" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="I43" s="9">
         <v>40834</v>
@@ -4506,10 +4533,10 @@
         <v>125</v>
       </c>
       <c r="O43" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="P43" t="s">
-        <v>429</v>
+        <v>418</v>
       </c>
       <c r="R43">
         <v>7</v>
@@ -4530,16 +4557,16 @@
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="F44" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="H44" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="I44" s="9">
         <v>40834</v>
@@ -4554,10 +4581,10 @@
         <v>125</v>
       </c>
       <c r="O44" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="P44" t="s">
-        <v>430</v>
+        <v>419</v>
       </c>
       <c r="R44">
         <v>9</v>
@@ -4578,16 +4605,16 @@
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="F45" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="H45" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="I45" s="9">
         <v>40834</v>
@@ -4602,10 +4629,10 @@
         <v>125</v>
       </c>
       <c r="O45" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="P45" t="s">
-        <v>431</v>
+        <v>420</v>
       </c>
       <c r="R45">
         <v>7</v>
@@ -4626,16 +4653,16 @@
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="F46" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="H46" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="I46" s="9">
         <v>40834</v>
@@ -4650,10 +4677,10 @@
         <v>125</v>
       </c>
       <c r="O46" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="P46" t="s">
-        <v>432</v>
+        <v>421</v>
       </c>
       <c r="R46">
         <v>9</v>
@@ -4674,16 +4701,16 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="F47" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="H47" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="I47" s="9">
         <v>40834</v>
@@ -4698,10 +4725,10 @@
         <v>125</v>
       </c>
       <c r="O47" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="P47" t="s">
-        <v>433</v>
+        <v>422</v>
       </c>
       <c r="R47">
         <v>6</v>
@@ -4722,16 +4749,16 @@
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="F48" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="H48" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="I48" s="9">
         <v>40834</v>
@@ -4746,10 +4773,10 @@
         <v>125</v>
       </c>
       <c r="O48" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="P48" t="s">
-        <v>434</v>
+        <v>423</v>
       </c>
       <c r="R48">
         <v>7</v>
@@ -4770,16 +4797,16 @@
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="F49" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="H49" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="I49" s="9">
         <v>40834</v>
@@ -4794,10 +4821,10 @@
         <v>125</v>
       </c>
       <c r="O49" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="P49" t="s">
-        <v>435</v>
+        <v>424</v>
       </c>
       <c r="R49">
         <v>8</v>
@@ -4818,16 +4845,16 @@
         <v>1</v>
       </c>
       <c r="E50" t="s">
+        <v>173</v>
+      </c>
+      <c r="F50" t="s">
+        <v>173</v>
+      </c>
+      <c r="G50" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="F50" t="s">
-        <v>184</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>195</v>
-      </c>
       <c r="H50" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="I50" s="9">
         <v>40834</v>
@@ -4842,10 +4869,10 @@
         <v>125</v>
       </c>
       <c r="O50" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="P50" t="s">
-        <v>436</v>
+        <v>425</v>
       </c>
       <c r="R50">
         <v>6</v>
@@ -4866,16 +4893,16 @@
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="F51" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="H51" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="I51" s="9">
         <v>40834</v>
@@ -4890,10 +4917,10 @@
         <v>125</v>
       </c>
       <c r="O51" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="P51" t="s">
-        <v>437</v>
+        <v>426</v>
       </c>
       <c r="R51">
         <v>8</v>
@@ -6197,19 +6224,19 @@
         <v>104</v>
       </c>
       <c r="C2" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="D2" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="E2" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="F2" t="s">
         <v>102</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -6221,19 +6248,19 @@
         <v>104</v>
       </c>
       <c r="C3" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
       <c r="D3" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
       <c r="E3" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="F3" t="s">
         <v>102</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -6245,19 +6272,19 @@
         <v>104</v>
       </c>
       <c r="C4" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
       <c r="D4" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
       <c r="E4" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="F4" t="s">
         <v>102</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -6269,19 +6296,19 @@
         <v>104</v>
       </c>
       <c r="C5" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
       <c r="D5" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
       <c r="E5" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="F5" t="s">
         <v>102</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -6293,19 +6320,19 @@
         <v>104</v>
       </c>
       <c r="C6" t="s">
-        <v>358</v>
+        <v>347</v>
       </c>
       <c r="D6" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
       <c r="E6" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="F6" t="s">
         <v>102</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -6317,19 +6344,19 @@
         <v>104</v>
       </c>
       <c r="C7" t="s">
-        <v>366</v>
+        <v>355</v>
       </c>
       <c r="D7" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
       <c r="E7" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
       <c r="F7" t="s">
         <v>102</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>367</v>
+        <v>356</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -6341,19 +6368,19 @@
         <v>104</v>
       </c>
       <c r="C8" t="s">
-        <v>369</v>
+        <v>358</v>
       </c>
       <c r="D8" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
       <c r="E8" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
       <c r="F8" t="s">
         <v>102</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -6365,19 +6392,19 @@
         <v>104</v>
       </c>
       <c r="C9" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
       <c r="D9" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="E9" t="s">
-        <v>363</v>
+        <v>352</v>
       </c>
       <c r="F9" t="s">
         <v>102</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -6389,19 +6416,19 @@
         <v>104</v>
       </c>
       <c r="C10" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
       <c r="D10" t="s">
-        <v>375</v>
+        <v>364</v>
       </c>
       <c r="E10" t="s">
-        <v>364</v>
+        <v>353</v>
       </c>
       <c r="F10" t="s">
         <v>102</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -6413,19 +6440,19 @@
         <v>104</v>
       </c>
       <c r="C11" t="s">
-        <v>377</v>
+        <v>366</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>379</v>
+        <v>368</v>
       </c>
       <c r="E11" t="s">
-        <v>365</v>
+        <v>354</v>
       </c>
       <c r="F11" t="s">
         <v>102</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -6437,19 +6464,19 @@
         <v>105</v>
       </c>
       <c r="C12" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="D12" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="E12" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="F12" t="s">
         <v>102</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -6461,19 +6488,19 @@
         <v>105</v>
       </c>
       <c r="C13" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="D13" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="E13" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="F13" t="s">
         <v>102</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -6485,19 +6512,19 @@
         <v>105</v>
       </c>
       <c r="C14" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="D14" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="E14" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="F14" t="s">
         <v>102</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -6509,19 +6536,19 @@
         <v>105</v>
       </c>
       <c r="C15" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="D15" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="E15" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="F15" t="s">
         <v>102</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -6533,19 +6560,19 @@
         <v>105</v>
       </c>
       <c r="C16" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="D16" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="E16" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="F16" t="s">
         <v>102</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -6557,19 +6584,19 @@
         <v>105</v>
       </c>
       <c r="C17" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="D17" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="E17" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="F17" t="s">
         <v>102</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -6581,19 +6608,19 @@
         <v>105</v>
       </c>
       <c r="C18" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="D18" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="E18" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="F18" t="s">
         <v>102</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -6605,19 +6632,19 @@
         <v>105</v>
       </c>
       <c r="C19" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="D19" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="E19" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="F19" t="s">
         <v>102</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -6629,19 +6656,19 @@
         <v>105</v>
       </c>
       <c r="C20" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="D20" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="E20" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="F20" t="s">
         <v>102</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -6653,19 +6680,19 @@
         <v>105</v>
       </c>
       <c r="C21" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="D21" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="E21" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="F21" t="s">
         <v>102</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -6677,19 +6704,19 @@
         <v>105</v>
       </c>
       <c r="C22" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="D22" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="E22" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="F22" t="s">
         <v>102</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -6701,19 +6728,19 @@
         <v>105</v>
       </c>
       <c r="C23" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="D23" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="E23" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="F23" t="s">
         <v>102</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -6725,19 +6752,19 @@
         <v>105</v>
       </c>
       <c r="C24" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
       <c r="D24" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="E24" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="F24" t="s">
         <v>102</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -6749,19 +6776,19 @@
         <v>105</v>
       </c>
       <c r="C25" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
       <c r="D25" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="E25" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="F25" t="s">
         <v>102</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -6773,19 +6800,19 @@
         <v>105</v>
       </c>
       <c r="C26" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="D26" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
       <c r="E26" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="F26" t="s">
         <v>102</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -6797,19 +6824,19 @@
         <v>107</v>
       </c>
       <c r="C27" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
       <c r="D27">
         <v>99</v>
       </c>
       <c r="E27" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
       <c r="F27" t="s">
         <v>103</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>380</v>
+        <v>369</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -6821,19 +6848,19 @@
         <v>107</v>
       </c>
       <c r="C28" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="D28">
         <v>99</v>
       </c>
       <c r="E28" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="F28" t="s">
         <v>103</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -6845,19 +6872,19 @@
         <v>107</v>
       </c>
       <c r="C29" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="D29">
         <v>99</v>
       </c>
       <c r="E29" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="F29" t="s">
         <v>103</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -6869,19 +6896,19 @@
         <v>107</v>
       </c>
       <c r="C30" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
       <c r="D30">
         <v>99</v>
       </c>
       <c r="E30" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
       <c r="F30" t="s">
         <v>103</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -6893,19 +6920,19 @@
         <v>107</v>
       </c>
       <c r="C31" t="s">
-        <v>394</v>
+        <v>383</v>
       </c>
       <c r="D31">
         <v>99</v>
       </c>
       <c r="E31" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
       <c r="F31" t="s">
         <v>103</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>395</v>
+        <v>384</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -6917,19 +6944,19 @@
         <v>107</v>
       </c>
       <c r="C32" t="s">
-        <v>396</v>
+        <v>385</v>
       </c>
       <c r="D32">
         <v>99</v>
       </c>
       <c r="E32" t="s">
-        <v>386</v>
+        <v>375</v>
       </c>
       <c r="F32" t="s">
         <v>103</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>397</v>
+        <v>386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated lifestyle content and supersport trailers
</commit_message>
<xml_diff>
--- a/data/EventData.xlsx
+++ b/data/EventData.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="486">
   <si>
     <t>Movies</t>
   </si>
@@ -411,9 +411,6 @@
     <t>qQtbklwKm48</t>
   </si>
   <si>
-    <t>2hMCycsef8A</t>
-  </si>
-  <si>
     <t>Football</t>
   </si>
   <si>
@@ -549,24 +546,6 @@
     <t>E!</t>
   </si>
   <si>
-    <t>Jamie Oliver</t>
-  </si>
-  <si>
-    <t>True Hollywood Story</t>
-  </si>
-  <si>
-    <t>Master Chef</t>
-  </si>
-  <si>
-    <t>Chopped</t>
-  </si>
-  <si>
-    <t>Emmy Awards 2011</t>
-  </si>
-  <si>
-    <t>Ten Dollar Dinners</t>
-  </si>
-  <si>
     <t>Paula's Best Dishes</t>
   </si>
   <si>
@@ -574,9 +553,6 @@
   </si>
   <si>
     <t>Iron Chef America</t>
-  </si>
-  <si>
-    <t>Good Eats: Alton's Best</t>
   </si>
   <si>
     <t>Ancient Discoveries</t>
@@ -615,36 +591,6 @@
 Desert Car Kings </t>
   </si>
   <si>
-    <t>Lifestyle01.jpg</t>
-  </si>
-  <si>
-    <t>Lifestyle02.jpg</t>
-  </si>
-  <si>
-    <t>Lifestyle03.jpg</t>
-  </si>
-  <si>
-    <t>Lifestyle04.jpg</t>
-  </si>
-  <si>
-    <t>Lifestyle05.jpg</t>
-  </si>
-  <si>
-    <t>Lifestyle06.jpg</t>
-  </si>
-  <si>
-    <t>Lifestyle07.jpg</t>
-  </si>
-  <si>
-    <t>Lifestyle08.jpg</t>
-  </si>
-  <si>
-    <t>Lifestyle09.jpg</t>
-  </si>
-  <si>
-    <t>Lifestyle10.jpg</t>
-  </si>
-  <si>
     <t>Can launch the YouTube app to play videos using intent.</t>
   </si>
   <si>
@@ -1399,6 +1345,147 @@
   </si>
   <si>
     <t>sport03.png</t>
+  </si>
+  <si>
+    <t>Ramsay's best restaurant</t>
+  </si>
+  <si>
+    <t>Gordon Ramsay returns with a brand new series seeking out the very best British restaurants up and down the country. Thousands of restaurants have been nominated by diners as their favourite local eatery, now Ramsay sets out to put these restaurants to the test before finally crowning the best of the best.
+Across eight heats Gordon puts two restaurants from different cuisines - from Italian and French to Chinese - head to head to really test their mettle. Will their food be able to stand a series of rigorous tests? Can the chefs cope cooking under Gordon's watch and in a kitchen that's not their own? And how will they fare under the glare of the cameras?</t>
+  </si>
+  <si>
+    <t>Jamie Oliver is here to start a revolution. The impassioned chef, TV personality and best-selling author is determined to take on the high statistics of obesity, heart disease and diabetes in this country, where our nation's children are the first generation not expected to live as long as their parents.
+Oliver is inviting viewers to take a stand and change the way America eats, in our home kitchens, schools and workplaces, with this thought-provoking new series.</t>
+  </si>
+  <si>
+    <t>Jamie Oliver's Food Revolution</t>
+  </si>
+  <si>
+    <t>BBC Lifestyle</t>
+  </si>
+  <si>
+    <t>Celebrity Masterchef Goes Large S2</t>
+  </si>
+  <si>
+    <t>Top chef and restaurateur John Torode and food writer and ingredients expert Gregg Wallace are back, judging the cooking skills of 24 well-known faces chosen for their passion for food.
+If the competing Celebrities can't stand the heat, John and Greg will order them out of the kitchen!</t>
+  </si>
+  <si>
+    <t>Top Gear series 17</t>
+  </si>
+  <si>
+    <t>BBC Entertainment</t>
+  </si>
+  <si>
+    <t>The series kicks off with the legendary Jaguar E-type’s 50th birthday, and Jeremy celebrates it in style with live music, fighter planes, and some Royal Marines. There’s also a trip to Italy, where Richard, James and Jeremy negotiate baffling Italian towns and take part in a scavenger hunt to find the world’s best hatchback.</t>
+  </si>
+  <si>
+    <t>lifestyle01.jpg</t>
+  </si>
+  <si>
+    <t>lifestyle02.jpg</t>
+  </si>
+  <si>
+    <t>lifestyle03.jpg</t>
+  </si>
+  <si>
+    <t>lifestyle04.jpg</t>
+  </si>
+  <si>
+    <t>lifestyle05.jpg</t>
+  </si>
+  <si>
+    <t>lifestyle06.jpg</t>
+  </si>
+  <si>
+    <t>lifestyle07.jpg</t>
+  </si>
+  <si>
+    <t>lifestyle08.jpg</t>
+  </si>
+  <si>
+    <t>lifestyle09.jpg</t>
+  </si>
+  <si>
+    <t>lifestyle10.jpg</t>
+  </si>
+  <si>
+    <t>Roomers is a exciting new interior design series, which is hosted by Neville Knott. In this eight part series Neville is joined by interior designers Joseph McCann, Karl Fradgley and Anne-Marie Hamill, who will bring their specialist skills to different houses around Ireland as they attempt to transform unsightly rooms.</t>
+  </si>
+  <si>
+    <t>Roomers</t>
+  </si>
+  <si>
+    <t>Home Channel</t>
+  </si>
+  <si>
+    <t>Decked Out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DECKED OUT is an entertaining, funny, irreverent show for the viewer who is fascinated with, or even mildly interested in, watching (and learning about) the creative process of designing and building impressively intricate outdoor decks and beautiful backyard spaces.  Each episode follows, from concept to completion, the story of a backyard makeover with a focus on the construction of the unique deck project. </t>
+  </si>
+  <si>
+    <t>What happens when America's favorite southern cook opens up her kitchen to family, friends, viewers and the best home cooks in the country? It's anyone's guess! Paula Deen is cookin' up something new as she rescues viewer recipes, shares stories and traditions with friends and strangers alike, and learns the secrets of some of America's best cooks. You just never know what you might get when the queen of southern cuisine dishes up good times and great food with the gang.</t>
+  </si>
+  <si>
+    <t>On her new show, Giada at Home, Giada De Laurentiis shares her love for entertaining California-style. Be Giada's guest as she puts together unique meals for gatherings with friends and family. Whether it's a festive bash or an intimate meal, in her own kitchen or at the beach, it's a day of memorable food and fun with Giada at Home</t>
+  </si>
+  <si>
+    <t>Based upon the Japanese cult sensation, Iron Chef America carries on the legend of Kitchen Stadium and the famed "secret ingredient." Each week, world-class chefs battle the legendary Iron Chefs of America: Bobby Flay, Mario Batali, Masaharu Morimoto, Cat Cora, Jose Garces, Michael Symon and Marc Forgione. Alton Brown serves as Commentator and Mark Dacascos is Chairman.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good Eats: Alton's Best </t>
+  </si>
+  <si>
+    <t>Pop culture, comedy, and plain good eating: Host Alton Brown explores the origins of ingredients, decodes culinary customs and presents food and equipment trends. Punctuated by unusual interludes, simple preparations and unconventional discussions, he'll bring you food in its finest and funniest form.</t>
+  </si>
+  <si>
+    <t>ZzzVdhyKjww</t>
+  </si>
+  <si>
+    <t>JvokX0_TGH8</t>
+  </si>
+  <si>
+    <t>8YKa-7knY1M</t>
+  </si>
+  <si>
+    <t>HNiW_n2bfIA</t>
+  </si>
+  <si>
+    <t>wVpi_4j0hrM</t>
+  </si>
+  <si>
+    <t>g2hZt0ULCe0</t>
+  </si>
+  <si>
+    <t>WaWoo82zNUA</t>
+  </si>
+  <si>
+    <t>t2ovJLs0-Ys</t>
+  </si>
+  <si>
+    <t>oLgmk323H6k</t>
+  </si>
+  <si>
+    <t>qoqo_UNb08E</t>
+  </si>
+  <si>
+    <t>sZCJDq-kFwQ</t>
+  </si>
+  <si>
+    <t>tR6SCBi2UEM</t>
+  </si>
+  <si>
+    <t>b4V0qrgqM70</t>
+  </si>
+  <si>
+    <t>dSU1y1MmHLI</t>
+  </si>
+  <si>
+    <t>MSA0WbFR1ds</t>
+  </si>
+  <si>
+    <t>JyE4lUcTxXU</t>
   </si>
 </sst>
 </file>
@@ -2001,7 +2088,7 @@
         <v>61</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2010,7 +2097,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>29</v>
@@ -2081,7 +2168,7 @@
       </c>
       <c r="E9" s="19"/>
       <c r="F9" s="22" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2190,7 +2277,7 @@
         <v>10</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="F15" s="22"/>
     </row>
@@ -2319,8 +2406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2398,7 +2485,7 @@
         <v>41</v>
       </c>
       <c r="R1" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="S1" t="s">
         <v>42</v>
@@ -2427,10 +2514,10 @@
         <v>0</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
       <c r="H2" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="I2" s="9">
         <v>40834</v>
@@ -2440,25 +2527,25 @@
       </c>
       <c r="K2" s="4"/>
       <c r="L2" s="12" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="O2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P2" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
       <c r="Q2" t="s">
-        <v>249</v>
+        <v>231</v>
       </c>
       <c r="R2">
         <v>7</v>
       </c>
       <c r="S2" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="T2">
         <v>2011</v>
@@ -2485,10 +2572,10 @@
         <v>0</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="H3" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="I3" s="9">
         <v>40834</v>
@@ -2497,25 +2584,25 @@
         <v>1.1041666666666701</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="N3" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="O3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="P3" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
       <c r="Q3" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
       <c r="R3">
         <v>8</v>
       </c>
       <c r="S3" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
       <c r="T3">
         <v>2011</v>
@@ -2542,7 +2629,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="H4" t="s">
         <v>2</v>
@@ -2554,25 +2641,25 @@
         <v>1.1458333333333299</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
       <c r="O4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="P4" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
       <c r="Q4" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
       <c r="R4">
         <v>9</v>
       </c>
       <c r="S4" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
       <c r="T4">
         <v>2011</v>
@@ -2599,10 +2686,10 @@
         <v>0</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
       <c r="H5" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="I5" s="9">
         <v>40834</v>
@@ -2612,25 +2699,25 @@
       </c>
       <c r="K5" s="4"/>
       <c r="L5" s="12" t="s">
-        <v>264</v>
+        <v>246</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>265</v>
+        <v>247</v>
       </c>
       <c r="O5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="P5" t="s">
-        <v>266</v>
+        <v>248</v>
       </c>
       <c r="Q5" t="s">
-        <v>268</v>
+        <v>250</v>
       </c>
       <c r="R5">
         <v>6</v>
       </c>
       <c r="S5" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="T5">
         <v>2011</v>
@@ -2657,7 +2744,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>269</v>
+        <v>251</v>
       </c>
       <c r="H6" t="s">
         <v>1</v>
@@ -2669,25 +2756,25 @@
         <v>1.2291666666666701</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="N6" t="s">
-        <v>271</v>
+        <v>253</v>
       </c>
       <c r="O6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P6" t="s">
-        <v>272</v>
+        <v>254</v>
       </c>
       <c r="Q6" t="s">
-        <v>274</v>
+        <v>256</v>
       </c>
       <c r="R6">
         <v>7</v>
       </c>
       <c r="S6" t="s">
-        <v>273</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="180.75" x14ac:dyDescent="0.25">
@@ -2711,7 +2798,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="H7" t="s">
         <v>1</v>
@@ -2723,25 +2810,25 @@
         <v>0.85416666666666663</v>
       </c>
       <c r="L7" s="12" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="N7" t="s">
-        <v>217</v>
+        <v>199</v>
       </c>
       <c r="O7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P7" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="Q7" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="R7">
         <v>8</v>
       </c>
       <c r="S7" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="T7">
         <v>2011</v>
@@ -2768,10 +2855,10 @@
         <v>0</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="H8" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="I8" s="9">
         <v>40834</v>
@@ -2780,25 +2867,25 @@
         <v>0.89583333333333337</v>
       </c>
       <c r="L8" s="12" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="O8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="P8" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="Q8" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="R8">
         <v>8</v>
       </c>
       <c r="S8" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="T8">
         <v>2011</v>
@@ -2825,10 +2912,10 @@
         <v>0</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="H9" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="I9" s="9">
         <v>40834</v>
@@ -2838,25 +2925,25 @@
       </c>
       <c r="K9" s="4"/>
       <c r="L9" s="12" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="O9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="P9" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="Q9" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
       <c r="R9">
         <v>8</v>
       </c>
       <c r="S9" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="T9">
         <v>2011</v>
@@ -2883,10 +2970,10 @@
         <v>0</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="H10" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="I10" s="9">
         <v>40834</v>
@@ -2895,25 +2982,25 @@
         <v>0.97916666666666696</v>
       </c>
       <c r="L10" s="12" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="N10" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="O10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="P10" t="s">
-        <v>236</v>
+        <v>218</v>
       </c>
       <c r="Q10" t="s">
-        <v>238</v>
+        <v>220</v>
       </c>
       <c r="R10">
         <v>9</v>
       </c>
       <c r="S10" t="s">
-        <v>237</v>
+        <v>219</v>
       </c>
       <c r="T10">
         <v>2011</v>
@@ -2940,10 +3027,10 @@
         <v>0</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
       <c r="H11" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="I11" s="9">
         <v>40834</v>
@@ -2952,25 +3039,25 @@
         <v>1.0208333333333299</v>
       </c>
       <c r="L11" s="12" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
       <c r="O11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="P11" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
       <c r="Q11" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="R11">
         <v>9</v>
       </c>
       <c r="S11" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="T11">
         <v>2011</v>
@@ -3012,7 +3099,7 @@
         <v>5</v>
       </c>
       <c r="L12" s="12" t="s">
-        <v>429</v>
+        <v>411</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>119</v>
@@ -3021,7 +3108,7 @@
         <v>127</v>
       </c>
       <c r="P12" t="s">
-        <v>387</v>
+        <v>369</v>
       </c>
       <c r="R12">
         <v>6</v>
@@ -3048,7 +3135,7 @@
         <v>3</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H13" t="s">
         <v>4</v>
@@ -3063,16 +3150,16 @@
         <v>6</v>
       </c>
       <c r="L13" s="12" t="s">
-        <v>427</v>
+        <v>409</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>120</v>
       </c>
       <c r="O13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P13" t="s">
-        <v>388</v>
+        <v>370</v>
       </c>
       <c r="R13">
         <v>7</v>
@@ -3099,7 +3186,7 @@
         <v>3</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H14" t="s">
         <v>3</v>
@@ -3111,19 +3198,19 @@
         <v>1.3541666666666701</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>431</v>
+        <v>413</v>
       </c>
       <c r="L14" s="12" t="s">
-        <v>430</v>
+        <v>412</v>
       </c>
       <c r="N14" t="s">
         <v>118</v>
       </c>
       <c r="O14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="P14" t="s">
-        <v>389</v>
+        <v>371</v>
       </c>
       <c r="R14">
         <v>6</v>
@@ -3165,16 +3252,16 @@
         <v>7</v>
       </c>
       <c r="L15" s="12" t="s">
-        <v>432</v>
+        <v>414</v>
       </c>
       <c r="N15" s="2" t="s">
         <v>121</v>
       </c>
       <c r="O15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="P15" t="s">
-        <v>390</v>
+        <v>372</v>
       </c>
       <c r="R15">
         <v>7</v>
@@ -3201,7 +3288,7 @@
         <v>3</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H16" t="s">
         <v>4</v>
@@ -3216,16 +3303,16 @@
         <v>5</v>
       </c>
       <c r="L16" s="12" t="s">
-        <v>433</v>
+        <v>415</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>119</v>
       </c>
       <c r="O16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P16" t="s">
-        <v>391</v>
+        <v>373</v>
       </c>
       <c r="R16">
         <v>6</v>
@@ -3252,7 +3339,7 @@
         <v>3</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H17" t="s">
         <v>4</v>
@@ -3267,16 +3354,16 @@
         <v>6</v>
       </c>
       <c r="L17" s="12" t="s">
-        <v>428</v>
+        <v>410</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>120</v>
       </c>
       <c r="O17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P17" t="s">
-        <v>392</v>
+        <v>374</v>
       </c>
       <c r="R17">
         <v>7</v>
@@ -3303,7 +3390,7 @@
         <v>3</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H18" t="s">
         <v>3</v>
@@ -3318,16 +3405,16 @@
         <v>117</v>
       </c>
       <c r="L18" s="12" t="s">
-        <v>434</v>
+        <v>416</v>
       </c>
       <c r="N18" t="s">
         <v>118</v>
       </c>
       <c r="O18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="P18" t="s">
-        <v>393</v>
+        <v>375</v>
       </c>
       <c r="R18">
         <v>8</v>
@@ -3354,7 +3441,7 @@
         <v>3</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H19" t="s">
         <v>8</v>
@@ -3369,16 +3456,16 @@
         <v>7</v>
       </c>
       <c r="L19" s="12" t="s">
-        <v>435</v>
+        <v>417</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>121</v>
       </c>
       <c r="O19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P19" t="s">
-        <v>394</v>
+        <v>376</v>
       </c>
       <c r="R19">
         <v>7</v>
@@ -3405,7 +3492,7 @@
         <v>3</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H20" t="s">
         <v>3</v>
@@ -3420,16 +3507,16 @@
         <v>117</v>
       </c>
       <c r="L20" s="12" t="s">
-        <v>436</v>
+        <v>418</v>
       </c>
       <c r="N20" t="s">
         <v>118</v>
       </c>
       <c r="O20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P20" t="s">
-        <v>395</v>
+        <v>377</v>
       </c>
       <c r="R20">
         <v>8</v>
@@ -3456,7 +3543,7 @@
         <v>3</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H21" t="s">
         <v>8</v>
@@ -3471,16 +3558,16 @@
         <v>5</v>
       </c>
       <c r="L21" s="12" t="s">
-        <v>437</v>
+        <v>419</v>
       </c>
       <c r="N21" s="2" t="s">
         <v>121</v>
       </c>
       <c r="O21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P21" t="s">
-        <v>396</v>
+        <v>378</v>
       </c>
       <c r="R21">
         <v>9</v>
@@ -3504,7 +3591,7 @@
         <v>9</v>
       </c>
       <c r="F22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>10</v>
@@ -3525,10 +3612,10 @@
         <v>122</v>
       </c>
       <c r="O22" t="s">
-        <v>448</v>
+        <v>430</v>
       </c>
       <c r="P22" t="s">
-        <v>397</v>
+        <v>379</v>
       </c>
       <c r="R22">
         <v>7</v>
@@ -3552,7 +3639,7 @@
         <v>9</v>
       </c>
       <c r="F23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>13</v>
@@ -3573,10 +3660,10 @@
         <v>123</v>
       </c>
       <c r="O23" t="s">
-        <v>449</v>
+        <v>431</v>
       </c>
       <c r="P23" t="s">
-        <v>405</v>
+        <v>387</v>
       </c>
       <c r="R23">
         <v>8</v>
@@ -3600,7 +3687,7 @@
         <v>9</v>
       </c>
       <c r="F24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>17</v>
@@ -3621,10 +3708,10 @@
         <v>124</v>
       </c>
       <c r="O24" t="s">
-        <v>457</v>
+        <v>439</v>
       </c>
       <c r="P24" t="s">
-        <v>406</v>
+        <v>388</v>
       </c>
       <c r="R24">
         <v>9</v>
@@ -3648,7 +3735,7 @@
         <v>9</v>
       </c>
       <c r="F25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>19</v>
@@ -3669,10 +3756,10 @@
         <v>125</v>
       </c>
       <c r="O25" t="s">
-        <v>450</v>
+        <v>432</v>
       </c>
       <c r="P25" t="s">
-        <v>404</v>
+        <v>386</v>
       </c>
       <c r="R25">
         <v>8</v>
@@ -3696,10 +3783,10 @@
         <v>9</v>
       </c>
       <c r="F26" t="s">
-        <v>443</v>
+        <v>425</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>438</v>
+        <v>420</v>
       </c>
       <c r="H26" t="s">
         <v>11</v>
@@ -3711,16 +3798,16 @@
         <v>1.8541666666666701</v>
       </c>
       <c r="L26" s="12" t="s">
-        <v>439</v>
+        <v>421</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>130</v>
+        <v>480</v>
       </c>
       <c r="O26" t="s">
-        <v>451</v>
+        <v>433</v>
       </c>
       <c r="P26" t="s">
-        <v>403</v>
+        <v>385</v>
       </c>
       <c r="R26">
         <v>9</v>
@@ -3744,10 +3831,10 @@
         <v>9</v>
       </c>
       <c r="F27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>440</v>
+        <v>422</v>
       </c>
       <c r="H27" t="s">
         <v>14</v>
@@ -3759,16 +3846,16 @@
         <v>1.8958333333333299</v>
       </c>
       <c r="L27" s="12" t="s">
-        <v>445</v>
+        <v>427</v>
       </c>
       <c r="N27" t="s">
-        <v>130</v>
+        <v>481</v>
       </c>
       <c r="O27" t="s">
-        <v>452</v>
+        <v>434</v>
       </c>
       <c r="P27" t="s">
-        <v>402</v>
+        <v>384</v>
       </c>
       <c r="R27">
         <v>8</v>
@@ -3792,10 +3879,10 @@
         <v>9</v>
       </c>
       <c r="F28" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>441</v>
+        <v>423</v>
       </c>
       <c r="H28" t="s">
         <v>18</v>
@@ -3807,16 +3894,16 @@
         <v>1.9375</v>
       </c>
       <c r="L28" s="12" t="s">
-        <v>444</v>
+        <v>426</v>
       </c>
       <c r="N28" t="s">
-        <v>130</v>
+        <v>482</v>
       </c>
       <c r="O28" t="s">
-        <v>453</v>
+        <v>435</v>
       </c>
       <c r="P28" t="s">
-        <v>401</v>
+        <v>383</v>
       </c>
       <c r="R28">
         <v>9</v>
@@ -3840,10 +3927,10 @@
         <v>9</v>
       </c>
       <c r="F29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>442</v>
+        <v>424</v>
       </c>
       <c r="H29" t="s">
         <v>11</v>
@@ -3855,16 +3942,16 @@
         <v>1.9791666666666701</v>
       </c>
       <c r="L29" s="12" t="s">
-        <v>446</v>
+        <v>428</v>
       </c>
       <c r="N29" t="s">
-        <v>130</v>
+        <v>483</v>
       </c>
       <c r="O29" t="s">
-        <v>454</v>
+        <v>436</v>
       </c>
       <c r="P29" t="s">
-        <v>400</v>
+        <v>382</v>
       </c>
       <c r="R29">
         <v>9</v>
@@ -3888,10 +3975,10 @@
         <v>9</v>
       </c>
       <c r="F30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H30" t="s">
         <v>18</v>
@@ -3906,13 +3993,13 @@
         <v>16</v>
       </c>
       <c r="N30" t="s">
-        <v>130</v>
+        <v>484</v>
       </c>
       <c r="O30" t="s">
-        <v>455</v>
+        <v>437</v>
       </c>
       <c r="P30" t="s">
-        <v>399</v>
+        <v>381</v>
       </c>
       <c r="R30">
         <v>9</v>
@@ -3936,10 +4023,10 @@
         <v>9</v>
       </c>
       <c r="F31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H31" t="s">
         <v>11</v>
@@ -3951,16 +4038,16 @@
         <v>2.0625</v>
       </c>
       <c r="L31" s="12" t="s">
-        <v>447</v>
+        <v>429</v>
       </c>
       <c r="N31" t="s">
-        <v>130</v>
+        <v>485</v>
       </c>
       <c r="O31" t="s">
-        <v>456</v>
+        <v>438</v>
       </c>
       <c r="P31" t="s">
-        <v>398</v>
+        <v>380</v>
       </c>
       <c r="R31">
         <v>7</v>
@@ -3987,10 +4074,10 @@
         <v>106</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="H32" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="I32" s="9">
         <v>40834</v>
@@ -4005,10 +4092,10 @@
         <v>129</v>
       </c>
       <c r="O32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P32" t="s">
-        <v>407</v>
+        <v>389</v>
       </c>
       <c r="R32">
         <v>6</v>
@@ -4035,10 +4122,10 @@
         <v>106</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="H33" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="I33" s="9">
         <v>40834</v>
@@ -4053,10 +4140,10 @@
         <v>129</v>
       </c>
       <c r="O33" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="P33" t="s">
-        <v>408</v>
+        <v>390</v>
       </c>
       <c r="R33">
         <v>7</v>
@@ -4083,10 +4170,10 @@
         <v>106</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="H34" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="I34" s="9">
         <v>40834</v>
@@ -4101,10 +4188,10 @@
         <v>129</v>
       </c>
       <c r="O34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P34" t="s">
-        <v>409</v>
+        <v>391</v>
       </c>
       <c r="R34">
         <v>6</v>
@@ -4131,10 +4218,10 @@
         <v>106</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="H35" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="I35" s="9">
         <v>40834</v>
@@ -4149,10 +4236,10 @@
         <v>129</v>
       </c>
       <c r="O35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P35" t="s">
-        <v>410</v>
+        <v>392</v>
       </c>
       <c r="R35">
         <v>7</v>
@@ -4179,7 +4266,7 @@
         <v>106</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="H36" t="s">
         <v>128</v>
@@ -4197,10 +4284,10 @@
         <v>129</v>
       </c>
       <c r="O36" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="P36" t="s">
-        <v>411</v>
+        <v>393</v>
       </c>
       <c r="R36">
         <v>8</v>
@@ -4227,7 +4314,7 @@
         <v>106</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="H37" t="s">
         <v>128</v>
@@ -4245,10 +4332,10 @@
         <v>129</v>
       </c>
       <c r="O37" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P37" t="s">
-        <v>412</v>
+        <v>394</v>
       </c>
       <c r="R37">
         <v>6</v>
@@ -4275,7 +4362,7 @@
         <v>106</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="H38" t="s">
         <v>128</v>
@@ -4293,10 +4380,10 @@
         <v>129</v>
       </c>
       <c r="O38" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P38" t="s">
-        <v>413</v>
+        <v>395</v>
       </c>
       <c r="R38">
         <v>5</v>
@@ -4323,7 +4410,7 @@
         <v>106</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="H39" t="s">
         <v>128</v>
@@ -4341,10 +4428,10 @@
         <v>129</v>
       </c>
       <c r="O39" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="P39" t="s">
-        <v>414</v>
+        <v>396</v>
       </c>
       <c r="R39">
         <v>8</v>
@@ -4371,7 +4458,7 @@
         <v>106</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="H40" t="s">
         <v>128</v>
@@ -4389,10 +4476,10 @@
         <v>129</v>
       </c>
       <c r="O40" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="P40" t="s">
-        <v>415</v>
+        <v>397</v>
       </c>
       <c r="R40">
         <v>7</v>
@@ -4419,7 +4506,7 @@
         <v>106</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="H41" t="s">
         <v>128</v>
@@ -4437,16 +4524,16 @@
         <v>129</v>
       </c>
       <c r="O41" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P41" t="s">
-        <v>416</v>
+        <v>398</v>
       </c>
       <c r="R41">
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -4461,16 +4548,16 @@
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F42" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>176</v>
+        <v>440</v>
       </c>
       <c r="H42" t="s">
-        <v>174</v>
+        <v>444</v>
       </c>
       <c r="I42" s="9">
         <v>40834</v>
@@ -4479,22 +4566,22 @@
         <v>2.5208333333333299</v>
       </c>
       <c r="L42" s="12" t="s">
-        <v>20</v>
+        <v>441</v>
       </c>
       <c r="N42" t="s">
-        <v>125</v>
+        <v>479</v>
       </c>
       <c r="O42" t="s">
-        <v>197</v>
+        <v>450</v>
       </c>
       <c r="P42" t="s">
-        <v>417</v>
+        <v>399</v>
       </c>
       <c r="R42">
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" ht="360.75" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -4509,16 +4596,16 @@
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F43" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>177</v>
+        <v>443</v>
       </c>
       <c r="H43" t="s">
-        <v>175</v>
+        <v>444</v>
       </c>
       <c r="I43" s="9">
         <v>40834</v>
@@ -4527,22 +4614,22 @@
         <v>2.5625</v>
       </c>
       <c r="L43" s="12" t="s">
-        <v>20</v>
+        <v>442</v>
       </c>
       <c r="N43" t="s">
-        <v>125</v>
+        <v>478</v>
       </c>
       <c r="O43" t="s">
-        <v>198</v>
+        <v>451</v>
       </c>
       <c r="P43" t="s">
-        <v>418</v>
+        <v>400</v>
       </c>
       <c r="R43">
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" ht="228.75" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -4557,16 +4644,16 @@
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F44" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>178</v>
+        <v>445</v>
       </c>
       <c r="H44" t="s">
-        <v>174</v>
+        <v>444</v>
       </c>
       <c r="I44" s="9">
         <v>40834</v>
@@ -4575,22 +4662,22 @@
         <v>2.6041666666666701</v>
       </c>
       <c r="L44" s="12" t="s">
-        <v>20</v>
+        <v>446</v>
       </c>
       <c r="N44" t="s">
-        <v>125</v>
+        <v>477</v>
       </c>
       <c r="O44" t="s">
-        <v>199</v>
+        <v>452</v>
       </c>
       <c r="P44" t="s">
-        <v>419</v>
+        <v>401</v>
       </c>
       <c r="R44">
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" ht="240.75" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -4605,16 +4692,16 @@
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F45" t="s">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>180</v>
+        <v>447</v>
       </c>
       <c r="H45" t="s">
-        <v>175</v>
+        <v>448</v>
       </c>
       <c r="I45" s="9">
         <v>40834</v>
@@ -4623,22 +4710,22 @@
         <v>2.6458333333333299</v>
       </c>
       <c r="L45" s="12" t="s">
-        <v>20</v>
+        <v>449</v>
       </c>
       <c r="N45" t="s">
-        <v>125</v>
+        <v>476</v>
       </c>
       <c r="O45" t="s">
-        <v>200</v>
+        <v>453</v>
       </c>
       <c r="P45" t="s">
-        <v>420</v>
+        <v>402</v>
       </c>
       <c r="R45">
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" ht="240.75" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -4653,16 +4740,16 @@
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F46" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>179</v>
+        <v>461</v>
       </c>
       <c r="H46" t="s">
-        <v>174</v>
+        <v>462</v>
       </c>
       <c r="I46" s="9">
         <v>40834</v>
@@ -4671,22 +4758,22 @@
         <v>2.6875</v>
       </c>
       <c r="L46" s="12" t="s">
-        <v>20</v>
+        <v>460</v>
       </c>
       <c r="N46" t="s">
-        <v>125</v>
+        <v>475</v>
       </c>
       <c r="O46" t="s">
-        <v>201</v>
+        <v>454</v>
       </c>
       <c r="P46" t="s">
-        <v>421</v>
+        <v>403</v>
       </c>
       <c r="R46">
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" ht="336.75" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -4701,16 +4788,16 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F47" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>181</v>
+        <v>463</v>
       </c>
       <c r="H47" t="s">
-        <v>174</v>
+        <v>462</v>
       </c>
       <c r="I47" s="9">
         <v>40834</v>
@@ -4719,22 +4806,22 @@
         <v>2.7291666666666701</v>
       </c>
       <c r="L47" s="12" t="s">
-        <v>20</v>
+        <v>464</v>
       </c>
       <c r="N47" t="s">
-        <v>125</v>
+        <v>474</v>
       </c>
       <c r="O47" t="s">
-        <v>202</v>
+        <v>455</v>
       </c>
       <c r="P47" t="s">
-        <v>422</v>
+        <v>404</v>
       </c>
       <c r="R47">
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" ht="372.75" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -4749,16 +4836,16 @@
         <v>1</v>
       </c>
       <c r="E48" t="s">
+        <v>172</v>
+      </c>
+      <c r="F48" t="s">
+        <v>172</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="H48" t="s">
         <v>173</v>
-      </c>
-      <c r="F48" t="s">
-        <v>173</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H48" t="s">
-        <v>174</v>
       </c>
       <c r="I48" s="9">
         <v>40834</v>
@@ -4767,22 +4854,22 @@
         <v>2.7708333333333299</v>
       </c>
       <c r="L48" s="12" t="s">
-        <v>20</v>
+        <v>465</v>
       </c>
       <c r="N48" t="s">
-        <v>125</v>
+        <v>473</v>
       </c>
       <c r="O48" t="s">
-        <v>203</v>
+        <v>456</v>
       </c>
       <c r="P48" t="s">
-        <v>423</v>
+        <v>405</v>
       </c>
       <c r="R48">
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" ht="252.75" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -4797,16 +4884,16 @@
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F49" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="H49" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I49" s="9">
         <v>40834</v>
@@ -4815,22 +4902,22 @@
         <v>2.8125</v>
       </c>
       <c r="L49" s="12" t="s">
-        <v>20</v>
+        <v>466</v>
       </c>
       <c r="N49" t="s">
-        <v>125</v>
+        <v>472</v>
       </c>
       <c r="O49" t="s">
-        <v>204</v>
+        <v>457</v>
       </c>
       <c r="P49" t="s">
-        <v>424</v>
+        <v>406</v>
       </c>
       <c r="R49">
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" ht="288.75" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -4845,16 +4932,16 @@
         <v>1</v>
       </c>
       <c r="E50" t="s">
+        <v>172</v>
+      </c>
+      <c r="F50" t="s">
+        <v>172</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="H50" t="s">
         <v>173</v>
-      </c>
-      <c r="F50" t="s">
-        <v>173</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="H50" t="s">
-        <v>174</v>
       </c>
       <c r="I50" s="9">
         <v>40834</v>
@@ -4863,22 +4950,22 @@
         <v>2.8541666666666701</v>
       </c>
       <c r="L50" s="12" t="s">
-        <v>20</v>
+        <v>467</v>
       </c>
       <c r="N50" t="s">
-        <v>125</v>
+        <v>471</v>
       </c>
       <c r="O50" t="s">
-        <v>205</v>
+        <v>458</v>
       </c>
       <c r="P50" t="s">
-        <v>425</v>
+        <v>407</v>
       </c>
       <c r="R50">
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:18" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" ht="240.75" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -4893,16 +4980,16 @@
         <v>1</v>
       </c>
       <c r="E51" t="s">
+        <v>172</v>
+      </c>
+      <c r="F51" t="s">
+        <v>172</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>468</v>
+      </c>
+      <c r="H51" t="s">
         <v>173</v>
-      </c>
-      <c r="F51" t="s">
-        <v>173</v>
-      </c>
-      <c r="G51" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="H51" t="s">
-        <v>174</v>
       </c>
       <c r="I51" s="9">
         <v>40834</v>
@@ -4911,16 +4998,16 @@
         <v>2.8958333333333299</v>
       </c>
       <c r="L51" s="12" t="s">
-        <v>20</v>
+        <v>469</v>
       </c>
       <c r="N51" t="s">
-        <v>125</v>
+        <v>470</v>
       </c>
       <c r="O51" t="s">
-        <v>206</v>
+        <v>459</v>
       </c>
       <c r="P51" t="s">
-        <v>426</v>
+        <v>408</v>
       </c>
       <c r="R51">
         <v>8</v>
@@ -6224,19 +6311,19 @@
         <v>104</v>
       </c>
       <c r="C2" t="s">
-        <v>331</v>
+        <v>313</v>
       </c>
       <c r="D2" t="s">
-        <v>332</v>
+        <v>314</v>
       </c>
       <c r="E2" t="s">
-        <v>333</v>
+        <v>315</v>
       </c>
       <c r="F2" t="s">
         <v>102</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>338</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -6248,19 +6335,19 @@
         <v>104</v>
       </c>
       <c r="C3" t="s">
-        <v>339</v>
+        <v>321</v>
       </c>
       <c r="D3" t="s">
-        <v>341</v>
+        <v>323</v>
       </c>
       <c r="E3" t="s">
-        <v>334</v>
+        <v>316</v>
       </c>
       <c r="F3" t="s">
         <v>102</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>340</v>
+        <v>322</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -6272,19 +6359,19 @@
         <v>104</v>
       </c>
       <c r="C4" t="s">
-        <v>342</v>
+        <v>324</v>
       </c>
       <c r="D4" t="s">
-        <v>343</v>
+        <v>325</v>
       </c>
       <c r="E4" t="s">
-        <v>335</v>
+        <v>317</v>
       </c>
       <c r="F4" t="s">
         <v>102</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>344</v>
+        <v>326</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -6296,19 +6383,19 @@
         <v>104</v>
       </c>
       <c r="C5" t="s">
-        <v>345</v>
+        <v>327</v>
       </c>
       <c r="D5" t="s">
-        <v>343</v>
+        <v>325</v>
       </c>
       <c r="E5" t="s">
-        <v>336</v>
+        <v>318</v>
       </c>
       <c r="F5" t="s">
         <v>102</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>346</v>
+        <v>328</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -6320,19 +6407,19 @@
         <v>104</v>
       </c>
       <c r="C6" t="s">
-        <v>347</v>
+        <v>329</v>
       </c>
       <c r="D6" t="s">
-        <v>348</v>
+        <v>330</v>
       </c>
       <c r="E6" t="s">
-        <v>337</v>
+        <v>319</v>
       </c>
       <c r="F6" t="s">
         <v>102</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>349</v>
+        <v>331</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -6344,19 +6431,19 @@
         <v>104</v>
       </c>
       <c r="C7" t="s">
-        <v>355</v>
+        <v>337</v>
       </c>
       <c r="D7" t="s">
-        <v>357</v>
+        <v>339</v>
       </c>
       <c r="E7" t="s">
-        <v>350</v>
+        <v>332</v>
       </c>
       <c r="F7" t="s">
         <v>102</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>356</v>
+        <v>338</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -6368,19 +6455,19 @@
         <v>104</v>
       </c>
       <c r="C8" t="s">
-        <v>358</v>
+        <v>340</v>
       </c>
       <c r="D8" t="s">
-        <v>359</v>
+        <v>341</v>
       </c>
       <c r="E8" t="s">
-        <v>351</v>
+        <v>333</v>
       </c>
       <c r="F8" t="s">
         <v>102</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -6392,19 +6479,19 @@
         <v>104</v>
       </c>
       <c r="C9" t="s">
-        <v>361</v>
+        <v>343</v>
       </c>
       <c r="D9" t="s">
-        <v>332</v>
+        <v>314</v>
       </c>
       <c r="E9" t="s">
-        <v>352</v>
+        <v>334</v>
       </c>
       <c r="F9" t="s">
         <v>102</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>362</v>
+        <v>344</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -6416,19 +6503,19 @@
         <v>104</v>
       </c>
       <c r="C10" t="s">
-        <v>363</v>
+        <v>345</v>
       </c>
       <c r="D10" t="s">
-        <v>364</v>
+        <v>346</v>
       </c>
       <c r="E10" t="s">
-        <v>353</v>
+        <v>335</v>
       </c>
       <c r="F10" t="s">
         <v>102</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>365</v>
+        <v>347</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -6440,19 +6527,19 @@
         <v>104</v>
       </c>
       <c r="C11" t="s">
-        <v>366</v>
+        <v>348</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>368</v>
+        <v>350</v>
       </c>
       <c r="E11" t="s">
-        <v>354</v>
+        <v>336</v>
       </c>
       <c r="F11" t="s">
         <v>102</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>367</v>
+        <v>349</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -6464,19 +6551,19 @@
         <v>105</v>
       </c>
       <c r="C12" t="s">
-        <v>276</v>
+        <v>258</v>
       </c>
       <c r="D12" t="s">
-        <v>277</v>
+        <v>259</v>
       </c>
       <c r="E12" t="s">
-        <v>286</v>
+        <v>268</v>
       </c>
       <c r="F12" t="s">
         <v>102</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>275</v>
+        <v>257</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -6488,19 +6575,19 @@
         <v>105</v>
       </c>
       <c r="C13" t="s">
-        <v>278</v>
+        <v>260</v>
       </c>
       <c r="D13" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
       <c r="E13" t="s">
-        <v>287</v>
+        <v>269</v>
       </c>
       <c r="F13" t="s">
         <v>102</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>279</v>
+        <v>261</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -6512,19 +6599,19 @@
         <v>105</v>
       </c>
       <c r="C14" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
       <c r="D14" t="s">
-        <v>281</v>
+        <v>263</v>
       </c>
       <c r="E14" t="s">
-        <v>288</v>
+        <v>270</v>
       </c>
       <c r="F14" t="s">
         <v>102</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>282</v>
+        <v>264</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -6536,19 +6623,19 @@
         <v>105</v>
       </c>
       <c r="C15" t="s">
-        <v>283</v>
+        <v>265</v>
       </c>
       <c r="D15" t="s">
-        <v>281</v>
+        <v>263</v>
       </c>
       <c r="E15" t="s">
-        <v>289</v>
+        <v>271</v>
       </c>
       <c r="F15" t="s">
         <v>102</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>285</v>
+        <v>267</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -6560,19 +6647,19 @@
         <v>105</v>
       </c>
       <c r="C16" t="s">
-        <v>290</v>
+        <v>272</v>
       </c>
       <c r="D16" t="s">
-        <v>293</v>
+        <v>275</v>
       </c>
       <c r="E16" t="s">
-        <v>292</v>
+        <v>274</v>
       </c>
       <c r="F16" t="s">
         <v>102</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>291</v>
+        <v>273</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -6584,19 +6671,19 @@
         <v>105</v>
       </c>
       <c r="C17" t="s">
-        <v>299</v>
+        <v>281</v>
       </c>
       <c r="D17" t="s">
-        <v>277</v>
+        <v>259</v>
       </c>
       <c r="E17" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
       <c r="F17" t="s">
         <v>102</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>300</v>
+        <v>282</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -6608,19 +6695,19 @@
         <v>105</v>
       </c>
       <c r="C18" t="s">
-        <v>301</v>
+        <v>283</v>
       </c>
       <c r="D18" t="s">
-        <v>302</v>
+        <v>284</v>
       </c>
       <c r="E18" t="s">
-        <v>295</v>
+        <v>277</v>
       </c>
       <c r="F18" t="s">
         <v>102</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>303</v>
+        <v>285</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -6632,19 +6719,19 @@
         <v>105</v>
       </c>
       <c r="C19" t="s">
-        <v>304</v>
+        <v>286</v>
       </c>
       <c r="D19" t="s">
-        <v>281</v>
+        <v>263</v>
       </c>
       <c r="E19" t="s">
-        <v>296</v>
+        <v>278</v>
       </c>
       <c r="F19" t="s">
         <v>102</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>305</v>
+        <v>287</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -6656,19 +6743,19 @@
         <v>105</v>
       </c>
       <c r="C20" t="s">
-        <v>306</v>
+        <v>288</v>
       </c>
       <c r="D20" t="s">
-        <v>307</v>
+        <v>289</v>
       </c>
       <c r="E20" t="s">
-        <v>297</v>
+        <v>279</v>
       </c>
       <c r="F20" t="s">
         <v>102</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>308</v>
+        <v>290</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -6680,19 +6767,19 @@
         <v>105</v>
       </c>
       <c r="C21" t="s">
-        <v>309</v>
+        <v>291</v>
       </c>
       <c r="D21" t="s">
-        <v>293</v>
+        <v>275</v>
       </c>
       <c r="E21" t="s">
-        <v>298</v>
+        <v>280</v>
       </c>
       <c r="F21" t="s">
         <v>102</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>310</v>
+        <v>292</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -6704,19 +6791,19 @@
         <v>105</v>
       </c>
       <c r="C22" t="s">
-        <v>316</v>
+        <v>298</v>
       </c>
       <c r="D22" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="E22" t="s">
-        <v>311</v>
+        <v>293</v>
       </c>
       <c r="F22" t="s">
         <v>102</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>318</v>
+        <v>300</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -6728,19 +6815,19 @@
         <v>105</v>
       </c>
       <c r="C23" t="s">
-        <v>319</v>
+        <v>301</v>
       </c>
       <c r="D23" t="s">
-        <v>320</v>
+        <v>302</v>
       </c>
       <c r="E23" t="s">
-        <v>312</v>
+        <v>294</v>
       </c>
       <c r="F23" t="s">
         <v>102</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>321</v>
+        <v>303</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -6752,19 +6839,19 @@
         <v>105</v>
       </c>
       <c r="C24" t="s">
-        <v>322</v>
+        <v>304</v>
       </c>
       <c r="D24" t="s">
-        <v>323</v>
+        <v>305</v>
       </c>
       <c r="E24" t="s">
-        <v>313</v>
+        <v>295</v>
       </c>
       <c r="F24" t="s">
         <v>102</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>324</v>
+        <v>306</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -6776,19 +6863,19 @@
         <v>105</v>
       </c>
       <c r="C25" t="s">
-        <v>325</v>
+        <v>307</v>
       </c>
       <c r="D25" t="s">
-        <v>326</v>
+        <v>308</v>
       </c>
       <c r="E25" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="F25" t="s">
         <v>102</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>327</v>
+        <v>309</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -6800,19 +6887,19 @@
         <v>105</v>
       </c>
       <c r="C26" t="s">
-        <v>329</v>
+        <v>311</v>
       </c>
       <c r="D26" t="s">
-        <v>328</v>
+        <v>310</v>
       </c>
       <c r="E26" t="s">
-        <v>315</v>
+        <v>297</v>
       </c>
       <c r="F26" t="s">
         <v>102</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>330</v>
+        <v>312</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -6824,19 +6911,19 @@
         <v>107</v>
       </c>
       <c r="C27" t="s">
-        <v>381</v>
+        <v>363</v>
       </c>
       <c r="D27">
         <v>99</v>
       </c>
       <c r="E27" t="s">
-        <v>370</v>
+        <v>352</v>
       </c>
       <c r="F27" t="s">
         <v>103</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>369</v>
+        <v>351</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -6848,19 +6935,19 @@
         <v>107</v>
       </c>
       <c r="C28" t="s">
-        <v>378</v>
+        <v>360</v>
       </c>
       <c r="D28">
         <v>99</v>
       </c>
       <c r="E28" t="s">
-        <v>371</v>
+        <v>353</v>
       </c>
       <c r="F28" t="s">
         <v>103</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>377</v>
+        <v>359</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -6872,19 +6959,19 @@
         <v>107</v>
       </c>
       <c r="C29" t="s">
-        <v>379</v>
+        <v>361</v>
       </c>
       <c r="D29">
         <v>99</v>
       </c>
       <c r="E29" t="s">
-        <v>372</v>
+        <v>354</v>
       </c>
       <c r="F29" t="s">
         <v>103</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>376</v>
+        <v>358</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -6896,19 +6983,19 @@
         <v>107</v>
       </c>
       <c r="C30" t="s">
-        <v>380</v>
+        <v>362</v>
       </c>
       <c r="D30">
         <v>99</v>
       </c>
       <c r="E30" t="s">
-        <v>373</v>
+        <v>355</v>
       </c>
       <c r="F30" t="s">
         <v>103</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>382</v>
+        <v>364</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -6920,19 +7007,19 @@
         <v>107</v>
       </c>
       <c r="C31" t="s">
-        <v>383</v>
+        <v>365</v>
       </c>
       <c r="D31">
         <v>99</v>
       </c>
       <c r="E31" t="s">
-        <v>374</v>
+        <v>356</v>
       </c>
       <c r="F31" t="s">
         <v>103</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>384</v>
+        <v>366</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -6944,19 +7031,19 @@
         <v>107</v>
       </c>
       <c r="C32" t="s">
-        <v>385</v>
+        <v>367</v>
       </c>
       <c r="D32">
         <v>99</v>
       </c>
       <c r="E32" t="s">
-        <v>375</v>
+        <v>357</v>
       </c>
       <c r="F32" t="s">
         <v>103</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>386</v>
+        <v>368</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
display 20 recommended events/buy items instead of 10 in coverflow.
</commit_message>
<xml_diff>
--- a/data/EventData.xlsx
+++ b/data/EventData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="WBS" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="506">
   <si>
     <t>Movies</t>
   </si>
@@ -1486,6 +1486,66 @@
   </si>
   <si>
     <t>JyE4lUcTxXU</t>
+  </si>
+  <si>
+    <t>buy_rec_11</t>
+  </si>
+  <si>
+    <t>buy_rec_12</t>
+  </si>
+  <si>
+    <t>buy_rec_13</t>
+  </si>
+  <si>
+    <t>buy_rec_14</t>
+  </si>
+  <si>
+    <t>buy_rec_15</t>
+  </si>
+  <si>
+    <t>buy_rec_16</t>
+  </si>
+  <si>
+    <t>buy_rec_17</t>
+  </si>
+  <si>
+    <t>buy_rec_18</t>
+  </si>
+  <si>
+    <t>buy_rec_19</t>
+  </si>
+  <si>
+    <t>buy_rec_20</t>
+  </si>
+  <si>
+    <t>view_rec_11</t>
+  </si>
+  <si>
+    <t>view_rec_12</t>
+  </si>
+  <si>
+    <t>view_rec_13</t>
+  </si>
+  <si>
+    <t>view_rec_14</t>
+  </si>
+  <si>
+    <t>view_rec_15</t>
+  </si>
+  <si>
+    <t>view_rec_16</t>
+  </si>
+  <si>
+    <t>view_rec_17</t>
+  </si>
+  <si>
+    <t>view_rec_18</t>
+  </si>
+  <si>
+    <t>view_rec_19</t>
+  </si>
+  <si>
+    <t>view_rec_20</t>
   </si>
 </sst>
 </file>
@@ -2406,7 +2466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
+    <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
@@ -5025,20 +5085,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:U24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:U24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" customWidth="1"/>
+    <col min="12" max="13" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -5072,8 +5133,38 @@
       <c r="K1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>496</v>
+      </c>
+      <c r="M1" t="s">
+        <v>497</v>
+      </c>
+      <c r="N1" t="s">
+        <v>498</v>
+      </c>
+      <c r="O1" t="s">
+        <v>499</v>
+      </c>
+      <c r="P1" t="s">
+        <v>500</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>501</v>
+      </c>
+      <c r="R1" t="s">
+        <v>502</v>
+      </c>
+      <c r="S1" t="s">
+        <v>503</v>
+      </c>
+      <c r="T1" t="s">
+        <v>504</v>
+      </c>
+      <c r="U1" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5107,8 +5198,38 @@
       <c r="K2">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <v>48</v>
+      </c>
+      <c r="M2">
+        <v>41</v>
+      </c>
+      <c r="N2">
+        <v>25</v>
+      </c>
+      <c r="O2">
+        <v>43</v>
+      </c>
+      <c r="P2">
+        <v>29</v>
+      </c>
+      <c r="Q2">
+        <v>13</v>
+      </c>
+      <c r="R2">
+        <v>45</v>
+      </c>
+      <c r="S2">
+        <v>20</v>
+      </c>
+      <c r="T2">
+        <v>28</v>
+      </c>
+      <c r="U2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5142,8 +5263,38 @@
       <c r="K3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>15</v>
+      </c>
+      <c r="M3">
+        <v>16</v>
+      </c>
+      <c r="N3">
+        <v>17</v>
+      </c>
+      <c r="O3">
+        <v>18</v>
+      </c>
+      <c r="P3">
+        <v>19</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3">
+        <v>3</v>
+      </c>
+      <c r="S3">
+        <v>4</v>
+      </c>
+      <c r="T3">
+        <v>5</v>
+      </c>
+      <c r="U3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5177,8 +5328,38 @@
       <c r="K4">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>40</v>
+      </c>
+      <c r="M4">
+        <v>43</v>
+      </c>
+      <c r="N4">
+        <v>26</v>
+      </c>
+      <c r="O4">
+        <v>46</v>
+      </c>
+      <c r="P4">
+        <v>47</v>
+      </c>
+      <c r="Q4">
+        <v>22</v>
+      </c>
+      <c r="R4">
+        <v>18</v>
+      </c>
+      <c r="S4">
+        <v>23</v>
+      </c>
+      <c r="T4">
+        <v>27</v>
+      </c>
+      <c r="U4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5212,8 +5393,38 @@
       <c r="K5">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>5</v>
+      </c>
+      <c r="M5">
+        <v>6</v>
+      </c>
+      <c r="N5">
+        <v>7</v>
+      </c>
+      <c r="O5">
+        <v>8</v>
+      </c>
+      <c r="P5">
+        <v>11</v>
+      </c>
+      <c r="Q5">
+        <v>13</v>
+      </c>
+      <c r="R5">
+        <v>4</v>
+      </c>
+      <c r="S5">
+        <v>42</v>
+      </c>
+      <c r="T5">
+        <v>3</v>
+      </c>
+      <c r="U5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5247,8 +5458,38 @@
       <c r="K6">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>43</v>
+      </c>
+      <c r="M6">
+        <v>45</v>
+      </c>
+      <c r="N6">
+        <v>26</v>
+      </c>
+      <c r="O6">
+        <v>43</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>23</v>
+      </c>
+      <c r="R6">
+        <v>45</v>
+      </c>
+      <c r="S6">
+        <v>8</v>
+      </c>
+      <c r="T6">
+        <v>28</v>
+      </c>
+      <c r="U6">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5282,8 +5523,38 @@
       <c r="K7">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>15</v>
+      </c>
+      <c r="M7">
+        <v>16</v>
+      </c>
+      <c r="N7">
+        <v>17</v>
+      </c>
+      <c r="O7">
+        <v>18</v>
+      </c>
+      <c r="P7">
+        <v>19</v>
+      </c>
+      <c r="Q7">
+        <v>2</v>
+      </c>
+      <c r="R7">
+        <v>3</v>
+      </c>
+      <c r="S7">
+        <v>4</v>
+      </c>
+      <c r="T7">
+        <v>5</v>
+      </c>
+      <c r="U7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5317,8 +5588,38 @@
       <c r="K8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <v>27</v>
+      </c>
+      <c r="M8">
+        <v>46</v>
+      </c>
+      <c r="N8">
+        <v>26</v>
+      </c>
+      <c r="O8">
+        <v>44</v>
+      </c>
+      <c r="P8">
+        <v>18</v>
+      </c>
+      <c r="Q8">
+        <v>21</v>
+      </c>
+      <c r="R8">
+        <v>17</v>
+      </c>
+      <c r="S8">
+        <v>20</v>
+      </c>
+      <c r="T8">
+        <v>26</v>
+      </c>
+      <c r="U8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5352,8 +5653,38 @@
       <c r="K9">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <v>46</v>
+      </c>
+      <c r="M9">
+        <v>47</v>
+      </c>
+      <c r="N9">
+        <v>26</v>
+      </c>
+      <c r="O9">
+        <v>43</v>
+      </c>
+      <c r="P9">
+        <v>29</v>
+      </c>
+      <c r="Q9">
+        <v>18</v>
+      </c>
+      <c r="R9">
+        <v>45</v>
+      </c>
+      <c r="S9">
+        <v>47</v>
+      </c>
+      <c r="T9">
+        <v>19</v>
+      </c>
+      <c r="U9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5387,8 +5718,38 @@
       <c r="K10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <v>28</v>
+      </c>
+      <c r="M10">
+        <v>21</v>
+      </c>
+      <c r="N10">
+        <v>7</v>
+      </c>
+      <c r="O10">
+        <v>9</v>
+      </c>
+      <c r="P10">
+        <v>12</v>
+      </c>
+      <c r="Q10">
+        <v>13</v>
+      </c>
+      <c r="R10">
+        <v>16</v>
+      </c>
+      <c r="S10">
+        <v>21</v>
+      </c>
+      <c r="T10">
+        <v>18</v>
+      </c>
+      <c r="U10">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5422,8 +5783,38 @@
       <c r="K11">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <v>5</v>
+      </c>
+      <c r="M11">
+        <v>6</v>
+      </c>
+      <c r="N11">
+        <v>7</v>
+      </c>
+      <c r="O11">
+        <v>8</v>
+      </c>
+      <c r="P11">
+        <v>11</v>
+      </c>
+      <c r="Q11">
+        <v>43</v>
+      </c>
+      <c r="R11">
+        <v>4</v>
+      </c>
+      <c r="S11">
+        <v>26</v>
+      </c>
+      <c r="T11">
+        <v>3</v>
+      </c>
+      <c r="U11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5457,8 +5848,38 @@
       <c r="K12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <v>40</v>
+      </c>
+      <c r="M12">
+        <v>41</v>
+      </c>
+      <c r="N12">
+        <v>26</v>
+      </c>
+      <c r="O12">
+        <v>43</v>
+      </c>
+      <c r="P12">
+        <v>29</v>
+      </c>
+      <c r="Q12">
+        <v>13</v>
+      </c>
+      <c r="R12">
+        <v>45</v>
+      </c>
+      <c r="S12">
+        <v>20</v>
+      </c>
+      <c r="T12">
+        <v>28</v>
+      </c>
+      <c r="U12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5492,8 +5913,38 @@
       <c r="K13">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <v>15</v>
+      </c>
+      <c r="M13">
+        <v>16</v>
+      </c>
+      <c r="N13">
+        <v>17</v>
+      </c>
+      <c r="O13">
+        <v>18</v>
+      </c>
+      <c r="P13">
+        <v>19</v>
+      </c>
+      <c r="Q13">
+        <v>2</v>
+      </c>
+      <c r="R13">
+        <v>3</v>
+      </c>
+      <c r="S13">
+        <v>4</v>
+      </c>
+      <c r="T13">
+        <v>5</v>
+      </c>
+      <c r="U13">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5527,8 +5978,38 @@
       <c r="K14">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <v>18</v>
+      </c>
+      <c r="M14">
+        <v>17</v>
+      </c>
+      <c r="N14">
+        <v>26</v>
+      </c>
+      <c r="O14">
+        <v>43</v>
+      </c>
+      <c r="P14">
+        <v>24</v>
+      </c>
+      <c r="Q14">
+        <v>13</v>
+      </c>
+      <c r="R14">
+        <v>48</v>
+      </c>
+      <c r="S14">
+        <v>20</v>
+      </c>
+      <c r="T14">
+        <v>44</v>
+      </c>
+      <c r="U14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5562,8 +6043,38 @@
       <c r="K15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <v>5</v>
+      </c>
+      <c r="M15">
+        <v>6</v>
+      </c>
+      <c r="N15">
+        <v>7</v>
+      </c>
+      <c r="O15">
+        <v>8</v>
+      </c>
+      <c r="P15">
+        <v>12</v>
+      </c>
+      <c r="Q15">
+        <v>22</v>
+      </c>
+      <c r="R15">
+        <v>4</v>
+      </c>
+      <c r="S15">
+        <v>9</v>
+      </c>
+      <c r="T15">
+        <v>3</v>
+      </c>
+      <c r="U15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5597,8 +6108,38 @@
       <c r="K16">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <v>8</v>
+      </c>
+      <c r="M16">
+        <v>41</v>
+      </c>
+      <c r="N16">
+        <v>26</v>
+      </c>
+      <c r="O16">
+        <v>21</v>
+      </c>
+      <c r="P16">
+        <v>29</v>
+      </c>
+      <c r="Q16">
+        <v>13</v>
+      </c>
+      <c r="R16">
+        <v>44</v>
+      </c>
+      <c r="S16">
+        <v>20</v>
+      </c>
+      <c r="T16">
+        <v>28</v>
+      </c>
+      <c r="U16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5632,8 +6173,38 @@
       <c r="K17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <v>40</v>
+      </c>
+      <c r="M17">
+        <v>19</v>
+      </c>
+      <c r="N17">
+        <v>26</v>
+      </c>
+      <c r="O17">
+        <v>43</v>
+      </c>
+      <c r="P17">
+        <v>47</v>
+      </c>
+      <c r="Q17">
+        <v>21</v>
+      </c>
+      <c r="R17">
+        <v>45</v>
+      </c>
+      <c r="S17">
+        <v>11</v>
+      </c>
+      <c r="T17">
+        <v>46</v>
+      </c>
+      <c r="U17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -5667,8 +6238,38 @@
       <c r="K18">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <v>15</v>
+      </c>
+      <c r="M18">
+        <v>16</v>
+      </c>
+      <c r="N18">
+        <v>17</v>
+      </c>
+      <c r="O18">
+        <v>18</v>
+      </c>
+      <c r="P18">
+        <v>19</v>
+      </c>
+      <c r="Q18">
+        <v>2</v>
+      </c>
+      <c r="R18">
+        <v>3</v>
+      </c>
+      <c r="S18">
+        <v>4</v>
+      </c>
+      <c r="T18">
+        <v>5</v>
+      </c>
+      <c r="U18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -5702,8 +6303,38 @@
       <c r="K19">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19">
+        <v>9</v>
+      </c>
+      <c r="M19">
+        <v>26</v>
+      </c>
+      <c r="N19">
+        <v>26</v>
+      </c>
+      <c r="O19">
+        <v>25</v>
+      </c>
+      <c r="P19">
+        <v>29</v>
+      </c>
+      <c r="Q19">
+        <v>49</v>
+      </c>
+      <c r="R19">
+        <v>42</v>
+      </c>
+      <c r="S19">
+        <v>13</v>
+      </c>
+      <c r="T19">
+        <v>28</v>
+      </c>
+      <c r="U19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -5737,8 +6368,38 @@
       <c r="K20">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20">
+        <v>5</v>
+      </c>
+      <c r="M20">
+        <v>6</v>
+      </c>
+      <c r="N20">
+        <v>7</v>
+      </c>
+      <c r="O20">
+        <v>8</v>
+      </c>
+      <c r="P20">
+        <v>10</v>
+      </c>
+      <c r="Q20">
+        <v>45</v>
+      </c>
+      <c r="R20">
+        <v>4</v>
+      </c>
+      <c r="S20">
+        <v>20</v>
+      </c>
+      <c r="T20">
+        <v>3</v>
+      </c>
+      <c r="U20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5772,8 +6433,38 @@
       <c r="K21">
         <v>13</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21">
+        <v>40</v>
+      </c>
+      <c r="M21">
+        <v>41</v>
+      </c>
+      <c r="N21">
+        <v>26</v>
+      </c>
+      <c r="O21">
+        <v>43</v>
+      </c>
+      <c r="P21">
+        <v>46</v>
+      </c>
+      <c r="Q21">
+        <v>13</v>
+      </c>
+      <c r="R21">
+        <v>40</v>
+      </c>
+      <c r="S21">
+        <v>15</v>
+      </c>
+      <c r="T21">
+        <v>48</v>
+      </c>
+      <c r="U21">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5807,8 +6498,38 @@
       <c r="K22">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <v>5</v>
+      </c>
+      <c r="M22">
+        <v>6</v>
+      </c>
+      <c r="N22">
+        <v>7</v>
+      </c>
+      <c r="O22">
+        <v>8</v>
+      </c>
+      <c r="P22">
+        <v>11</v>
+      </c>
+      <c r="Q22">
+        <v>46</v>
+      </c>
+      <c r="R22">
+        <v>4</v>
+      </c>
+      <c r="S22">
+        <v>20</v>
+      </c>
+      <c r="T22">
+        <v>3</v>
+      </c>
+      <c r="U22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5842,8 +6563,38 @@
       <c r="K23">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23">
+        <v>12</v>
+      </c>
+      <c r="M23">
+        <v>28</v>
+      </c>
+      <c r="N23">
+        <v>26</v>
+      </c>
+      <c r="O23">
+        <v>29</v>
+      </c>
+      <c r="P23">
+        <v>29</v>
+      </c>
+      <c r="Q23">
+        <v>44</v>
+      </c>
+      <c r="R23">
+        <v>45</v>
+      </c>
+      <c r="S23">
+        <v>17</v>
+      </c>
+      <c r="T23">
+        <v>28</v>
+      </c>
+      <c r="U23">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5876,6 +6627,36 @@
       </c>
       <c r="K24">
         <v>2</v>
+      </c>
+      <c r="L24">
+        <v>15</v>
+      </c>
+      <c r="M24">
+        <v>16</v>
+      </c>
+      <c r="N24">
+        <v>17</v>
+      </c>
+      <c r="O24">
+        <v>18</v>
+      </c>
+      <c r="P24">
+        <v>19</v>
+      </c>
+      <c r="Q24">
+        <v>2</v>
+      </c>
+      <c r="R24">
+        <v>3</v>
+      </c>
+      <c r="S24">
+        <v>4</v>
+      </c>
+      <c r="T24">
+        <v>5</v>
+      </c>
+      <c r="U24">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -5885,10 +6666,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5896,9 +6677,10 @@
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="10" width="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -5932,8 +6714,38 @@
       <c r="K1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>486</v>
+      </c>
+      <c r="M1" t="s">
+        <v>487</v>
+      </c>
+      <c r="N1" t="s">
+        <v>488</v>
+      </c>
+      <c r="O1" t="s">
+        <v>489</v>
+      </c>
+      <c r="P1" t="s">
+        <v>490</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>491</v>
+      </c>
+      <c r="R1" t="s">
+        <v>492</v>
+      </c>
+      <c r="S1" t="s">
+        <v>493</v>
+      </c>
+      <c r="T1" t="s">
+        <v>494</v>
+      </c>
+      <c r="U1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5967,8 +6779,38 @@
       <c r="K2">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <v>20</v>
+      </c>
+      <c r="M2">
+        <v>4</v>
+      </c>
+      <c r="N2">
+        <v>5</v>
+      </c>
+      <c r="O2">
+        <v>6</v>
+      </c>
+      <c r="P2">
+        <v>7</v>
+      </c>
+      <c r="Q2">
+        <v>21</v>
+      </c>
+      <c r="R2">
+        <v>22</v>
+      </c>
+      <c r="S2">
+        <v>24</v>
+      </c>
+      <c r="T2">
+        <v>25</v>
+      </c>
+      <c r="U2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -6003,8 +6845,38 @@
       <c r="K3">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>7</v>
+      </c>
+      <c r="M3">
+        <v>8</v>
+      </c>
+      <c r="N3">
+        <v>21</v>
+      </c>
+      <c r="O3">
+        <v>22</v>
+      </c>
+      <c r="P3">
+        <v>23</v>
+      </c>
+      <c r="Q3">
+        <v>24</v>
+      </c>
+      <c r="R3">
+        <v>25</v>
+      </c>
+      <c r="S3">
+        <v>27</v>
+      </c>
+      <c r="T3">
+        <v>28</v>
+      </c>
+      <c r="U3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A10" si="0">A3+1</f>
         <v>3</v>
@@ -6039,8 +6911,41 @@
       <c r="K4">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>10</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>15</v>
+      </c>
+      <c r="O4">
+        <v>21</v>
+      </c>
+      <c r="P4">
+        <v>20</v>
+      </c>
+      <c r="Q4">
+        <v>13</v>
+      </c>
+      <c r="R4">
+        <v>12</v>
+      </c>
+      <c r="S4">
+        <v>29</v>
+      </c>
+      <c r="T4">
+        <v>31</v>
+      </c>
+      <c r="U4">
+        <v>20</v>
+      </c>
+      <c r="X4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -6075,8 +6980,38 @@
       <c r="K5">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>20</v>
+      </c>
+      <c r="M5">
+        <v>4</v>
+      </c>
+      <c r="N5">
+        <v>5</v>
+      </c>
+      <c r="O5">
+        <v>6</v>
+      </c>
+      <c r="P5">
+        <v>7</v>
+      </c>
+      <c r="Q5">
+        <v>21</v>
+      </c>
+      <c r="R5">
+        <v>22</v>
+      </c>
+      <c r="S5">
+        <v>24</v>
+      </c>
+      <c r="T5">
+        <v>25</v>
+      </c>
+      <c r="U5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -6111,8 +7046,41 @@
       <c r="K6">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>10</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>15</v>
+      </c>
+      <c r="O6">
+        <v>21</v>
+      </c>
+      <c r="P6">
+        <v>20</v>
+      </c>
+      <c r="Q6">
+        <v>13</v>
+      </c>
+      <c r="R6">
+        <v>12</v>
+      </c>
+      <c r="S6">
+        <v>29</v>
+      </c>
+      <c r="T6">
+        <v>31</v>
+      </c>
+      <c r="U6">
+        <v>20</v>
+      </c>
+      <c r="X6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -6147,8 +7115,38 @@
       <c r="K7">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>4</v>
+      </c>
+      <c r="M7">
+        <v>5</v>
+      </c>
+      <c r="N7">
+        <v>6</v>
+      </c>
+      <c r="O7">
+        <v>7</v>
+      </c>
+      <c r="P7">
+        <v>11</v>
+      </c>
+      <c r="Q7">
+        <v>12</v>
+      </c>
+      <c r="R7">
+        <v>16</v>
+      </c>
+      <c r="S7">
+        <v>2</v>
+      </c>
+      <c r="T7">
+        <v>24</v>
+      </c>
+      <c r="U7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -6183,8 +7181,38 @@
       <c r="K8">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <v>7</v>
+      </c>
+      <c r="M8">
+        <v>8</v>
+      </c>
+      <c r="N8">
+        <v>21</v>
+      </c>
+      <c r="O8">
+        <v>22</v>
+      </c>
+      <c r="P8">
+        <v>23</v>
+      </c>
+      <c r="Q8">
+        <v>24</v>
+      </c>
+      <c r="R8">
+        <v>25</v>
+      </c>
+      <c r="S8">
+        <v>27</v>
+      </c>
+      <c r="T8">
+        <v>28</v>
+      </c>
+      <c r="U8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -6219,8 +7247,38 @@
       <c r="K9">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <v>20</v>
+      </c>
+      <c r="M9">
+        <v>4</v>
+      </c>
+      <c r="N9">
+        <v>5</v>
+      </c>
+      <c r="O9">
+        <v>6</v>
+      </c>
+      <c r="P9">
+        <v>7</v>
+      </c>
+      <c r="Q9">
+        <v>21</v>
+      </c>
+      <c r="R9">
+        <v>22</v>
+      </c>
+      <c r="S9">
+        <v>24</v>
+      </c>
+      <c r="T9">
+        <v>25</v>
+      </c>
+      <c r="U9">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -6254,6 +7312,36 @@
       </c>
       <c r="K10">
         <v>29</v>
+      </c>
+      <c r="L10">
+        <v>24</v>
+      </c>
+      <c r="M10">
+        <v>11</v>
+      </c>
+      <c r="N10">
+        <v>12</v>
+      </c>
+      <c r="O10">
+        <v>15</v>
+      </c>
+      <c r="P10">
+        <v>28</v>
+      </c>
+      <c r="Q10">
+        <v>29</v>
+      </c>
+      <c r="R10">
+        <v>7</v>
+      </c>
+      <c r="S10">
+        <v>8</v>
+      </c>
+      <c r="T10">
+        <v>21</v>
+      </c>
+      <c r="U10">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the dates(02 Nov 2011) in the raw data for demo
</commit_message>
<xml_diff>
--- a/data/EventData.xlsx
+++ b/data/EventData.xlsx
@@ -2466,8 +2466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2580,7 +2580,7 @@
         <v>208</v>
       </c>
       <c r="I2" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J2" s="5">
         <v>1.0625</v>
@@ -2638,7 +2638,7 @@
         <v>206</v>
       </c>
       <c r="I3" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J3" s="5">
         <v>1.1041666666666701</v>
@@ -2695,7 +2695,7 @@
         <v>2</v>
       </c>
       <c r="I4" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J4" s="5">
         <v>1.1458333333333299</v>
@@ -2752,7 +2752,7 @@
         <v>208</v>
       </c>
       <c r="I5" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J5" s="5">
         <v>1.1875</v>
@@ -2810,7 +2810,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J6" s="5">
         <v>1.2291666666666701</v>
@@ -2864,7 +2864,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J7" s="5">
         <v>0.85416666666666663</v>
@@ -2921,7 +2921,7 @@
         <v>206</v>
       </c>
       <c r="I8" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J8" s="5">
         <v>0.89583333333333337</v>
@@ -2978,7 +2978,7 @@
         <v>208</v>
       </c>
       <c r="I9" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J9" s="5">
         <v>0.9375</v>
@@ -3036,7 +3036,7 @@
         <v>215</v>
       </c>
       <c r="I10" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J10" s="5">
         <v>0.97916666666666696</v>
@@ -3093,7 +3093,7 @@
         <v>206</v>
       </c>
       <c r="I11" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J11" s="5">
         <v>1.0208333333333299</v>
@@ -3150,7 +3150,7 @@
         <v>4</v>
       </c>
       <c r="I12" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J12" s="5">
         <v>1.2708333333333299</v>
@@ -3201,7 +3201,7 @@
         <v>4</v>
       </c>
       <c r="I13" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J13" s="5">
         <v>1.3125</v>
@@ -3252,7 +3252,7 @@
         <v>3</v>
       </c>
       <c r="I14" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J14" s="5">
         <v>1.3541666666666701</v>
@@ -3303,7 +3303,7 @@
         <v>8</v>
       </c>
       <c r="I15" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J15" s="5">
         <v>1.3958333333333299</v>
@@ -3354,7 +3354,7 @@
         <v>4</v>
       </c>
       <c r="I16" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J16" s="5">
         <v>1.4375</v>
@@ -3405,7 +3405,7 @@
         <v>4</v>
       </c>
       <c r="I17" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J17" s="5">
         <v>1.4791666666666701</v>
@@ -3456,7 +3456,7 @@
         <v>3</v>
       </c>
       <c r="I18" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J18" s="5">
         <v>1.5208333333333299</v>
@@ -3507,7 +3507,7 @@
         <v>8</v>
       </c>
       <c r="I19" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J19" s="5">
         <v>1.5625</v>
@@ -3558,7 +3558,7 @@
         <v>3</v>
       </c>
       <c r="I20" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J20" s="5">
         <v>1.6041666666666701</v>
@@ -3609,7 +3609,7 @@
         <v>8</v>
       </c>
       <c r="I21" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J21" s="5">
         <v>1.6458333333333299</v>
@@ -3660,7 +3660,7 @@
         <v>11</v>
       </c>
       <c r="I22" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J22" s="5">
         <v>1.6875</v>
@@ -3708,7 +3708,7 @@
         <v>14</v>
       </c>
       <c r="I23" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J23" s="5">
         <v>1.7291666666666701</v>
@@ -3756,7 +3756,7 @@
         <v>18</v>
       </c>
       <c r="I24" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J24" s="5">
         <v>1.7708333333333299</v>
@@ -3804,7 +3804,7 @@
         <v>11</v>
       </c>
       <c r="I25" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J25" s="5">
         <v>1.8125</v>
@@ -3852,7 +3852,7 @@
         <v>11</v>
       </c>
       <c r="I26" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J26" s="5">
         <v>1.8541666666666701</v>
@@ -3900,7 +3900,7 @@
         <v>14</v>
       </c>
       <c r="I27" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J27" s="5">
         <v>1.8958333333333299</v>
@@ -3948,7 +3948,7 @@
         <v>18</v>
       </c>
       <c r="I28" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J28" s="5">
         <v>1.9375</v>
@@ -3996,7 +3996,7 @@
         <v>11</v>
       </c>
       <c r="I29" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J29" s="5">
         <v>1.9791666666666701</v>
@@ -4044,7 +4044,7 @@
         <v>18</v>
       </c>
       <c r="I30" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J30" s="5">
         <v>2.0208333333333299</v>
@@ -4092,7 +4092,7 @@
         <v>11</v>
       </c>
       <c r="I31" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J31" s="5">
         <v>2.0625</v>
@@ -4140,7 +4140,7 @@
         <v>185</v>
       </c>
       <c r="I32" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J32" s="5">
         <v>2.1041666666666701</v>
@@ -4188,7 +4188,7 @@
         <v>185</v>
       </c>
       <c r="I33" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J33" s="5">
         <v>2.1458333333333299</v>
@@ -4236,7 +4236,7 @@
         <v>185</v>
       </c>
       <c r="I34" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J34" s="5">
         <v>2.1875</v>
@@ -4284,7 +4284,7 @@
         <v>185</v>
       </c>
       <c r="I35" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J35" s="5">
         <v>2.2291666666666701</v>
@@ -4332,7 +4332,7 @@
         <v>128</v>
       </c>
       <c r="I36" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J36" s="5">
         <v>2.2708333333333299</v>
@@ -4380,7 +4380,7 @@
         <v>128</v>
       </c>
       <c r="I37" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J37" s="5">
         <v>2.3125</v>
@@ -4428,7 +4428,7 @@
         <v>128</v>
       </c>
       <c r="I38" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J38" s="5">
         <v>2.3541666666666701</v>
@@ -4476,7 +4476,7 @@
         <v>128</v>
       </c>
       <c r="I39" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J39" s="5">
         <v>2.3958333333333299</v>
@@ -4524,7 +4524,7 @@
         <v>128</v>
       </c>
       <c r="I40" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J40" s="5">
         <v>2.4375</v>
@@ -4572,7 +4572,7 @@
         <v>128</v>
       </c>
       <c r="I41" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J41" s="5">
         <v>2.4791666666666701</v>
@@ -4620,7 +4620,7 @@
         <v>434</v>
       </c>
       <c r="I42" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J42" s="5">
         <v>2.5208333333333299</v>
@@ -4668,7 +4668,7 @@
         <v>434</v>
       </c>
       <c r="I43" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J43" s="5">
         <v>2.5625</v>
@@ -4716,7 +4716,7 @@
         <v>434</v>
       </c>
       <c r="I44" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J44" s="5">
         <v>2.6041666666666701</v>
@@ -4764,7 +4764,7 @@
         <v>438</v>
       </c>
       <c r="I45" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J45" s="5">
         <v>2.6458333333333299</v>
@@ -4812,7 +4812,7 @@
         <v>452</v>
       </c>
       <c r="I46" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J46" s="5">
         <v>2.6875</v>
@@ -4860,7 +4860,7 @@
         <v>452</v>
       </c>
       <c r="I47" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J47" s="5">
         <v>2.7291666666666701</v>
@@ -4908,7 +4908,7 @@
         <v>173</v>
       </c>
       <c r="I48" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J48" s="5">
         <v>2.7708333333333299</v>
@@ -4956,7 +4956,7 @@
         <v>174</v>
       </c>
       <c r="I49" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J49" s="5">
         <v>2.8125</v>
@@ -5004,7 +5004,7 @@
         <v>173</v>
       </c>
       <c r="I50" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J50" s="5">
         <v>2.8541666666666701</v>
@@ -5052,7 +5052,7 @@
         <v>173</v>
       </c>
       <c r="I51" s="9">
-        <v>40834</v>
+        <v>40849</v>
       </c>
       <c r="J51" s="5">
         <v>2.8958333333333299</v>

</xml_diff>